<commit_message>
add heatmap in xlsx
</commit_message>
<xml_diff>
--- a/chapter2/input/chapter2_demo_data.xlsx
+++ b/chapter2/input/chapter2_demo_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\副業関連\独立\執筆\practical-mi-guide\chapter2\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85660D61-4B96-4835-B912-63C146A95F34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81551455-ABA1-499F-8765-2586EC360A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" activeTab="4" xr2:uid="{AFFCA931-CB2A-4AED-B7E5-2638B5FCE6AD}"/>
+    <workbookView xWindow="1340" yWindow="3850" windowWidth="36790" windowHeight="17100" activeTab="5" xr2:uid="{AFFCA931-CB2A-4AED-B7E5-2638B5FCE6AD}"/>
   </bookViews>
   <sheets>
     <sheet name="初期データ" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="整形Step2" sheetId="5" r:id="rId3"/>
     <sheet name="整形Step3" sheetId="6" r:id="rId4"/>
     <sheet name="整形後" sheetId="7" r:id="rId5"/>
-    <sheet name="元データ" sheetId="1" r:id="rId6"/>
+    <sheet name="ヒートマップ" sheetId="8" r:id="rId6"/>
+    <sheet name="元データ" sheetId="1" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1536" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1584" uniqueCount="192">
   <si>
     <t>サンプル名</t>
     <rPh sb="4" eb="5">
@@ -1112,6 +1113,78 @@
     <t>未知説明変数</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>溶媒１</t>
+  </si>
+  <si>
+    <t>溶媒2</t>
+  </si>
+  <si>
+    <t>溶媒3</t>
+  </si>
+  <si>
+    <t>添加剤1</t>
+  </si>
+  <si>
+    <t>添加剤2</t>
+  </si>
+  <si>
+    <t>界面活性剤１</t>
+  </si>
+  <si>
+    <t>界面活性剤２</t>
+  </si>
+  <si>
+    <t>界面活性剤３</t>
+  </si>
+  <si>
+    <t>顔料１</t>
+  </si>
+  <si>
+    <t>顔料２</t>
+  </si>
+  <si>
+    <t>定着樹脂１</t>
+  </si>
+  <si>
+    <t>定着樹脂２</t>
+  </si>
+  <si>
+    <t>防腐剤</t>
+  </si>
+  <si>
+    <t>塗布量</t>
+  </si>
+  <si>
+    <t>乾燥方式</t>
+  </si>
+  <si>
+    <t>乾燥温度</t>
+  </si>
+  <si>
+    <t>乾燥時間</t>
+  </si>
+  <si>
+    <t>擦過回数</t>
+  </si>
+  <si>
+    <t>擦過圧力</t>
+  </si>
+  <si>
+    <t>耐擦過性(n10</t>
+  </si>
+  <si>
+    <t>画像濃度</t>
+  </si>
+  <si>
+    <t>粘度</t>
+  </si>
+  <si>
+    <t>表面張力</t>
+  </si>
+  <si>
+    <t>保存後粘度</t>
+  </si>
 </sst>
 </file>
 
@@ -1162,7 +1235,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1321,13 +1394,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1541,6 +1634,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1559,23 +1670,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2986,7 +3094,7 @@
       <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="G50" sqref="G50"/>
+      <selection pane="bottomRight" activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -3222,101 +3330,101 @@
       <c r="C7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="77">
+      <c r="D7" s="71">
         <v>45310</v>
       </c>
-      <c r="E7" s="78"/>
-      <c r="F7" s="78"/>
-      <c r="G7" s="78"/>
-      <c r="H7" s="79"/>
-      <c r="I7" s="77">
+      <c r="E7" s="72"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="72"/>
+      <c r="H7" s="73"/>
+      <c r="I7" s="71">
         <v>45321</v>
       </c>
-      <c r="J7" s="78"/>
-      <c r="K7" s="78"/>
-      <c r="L7" s="78"/>
-      <c r="M7" s="78"/>
-      <c r="N7" s="78"/>
-      <c r="O7" s="78"/>
-      <c r="P7" s="78"/>
-      <c r="Q7" s="79"/>
-      <c r="R7" s="77">
+      <c r="J7" s="72"/>
+      <c r="K7" s="72"/>
+      <c r="L7" s="72"/>
+      <c r="M7" s="72"/>
+      <c r="N7" s="72"/>
+      <c r="O7" s="72"/>
+      <c r="P7" s="72"/>
+      <c r="Q7" s="73"/>
+      <c r="R7" s="71">
         <v>45337</v>
       </c>
-      <c r="S7" s="78"/>
-      <c r="T7" s="78"/>
-      <c r="U7" s="79"/>
-      <c r="V7" s="77">
+      <c r="S7" s="72"/>
+      <c r="T7" s="72"/>
+      <c r="U7" s="73"/>
+      <c r="V7" s="71">
         <v>45350</v>
       </c>
-      <c r="W7" s="78"/>
-      <c r="X7" s="78"/>
-      <c r="Y7" s="79"/>
-      <c r="Z7" s="77">
+      <c r="W7" s="72"/>
+      <c r="X7" s="72"/>
+      <c r="Y7" s="73"/>
+      <c r="Z7" s="71">
         <v>45366</v>
       </c>
-      <c r="AA7" s="78"/>
-      <c r="AB7" s="78"/>
-      <c r="AC7" s="79"/>
-      <c r="AD7" s="77">
+      <c r="AA7" s="72"/>
+      <c r="AB7" s="72"/>
+      <c r="AC7" s="73"/>
+      <c r="AD7" s="71">
         <v>45392</v>
       </c>
-      <c r="AE7" s="78"/>
-      <c r="AF7" s="78"/>
-      <c r="AG7" s="78"/>
-      <c r="AH7" s="78"/>
-      <c r="AI7" s="78"/>
-      <c r="AJ7" s="79"/>
+      <c r="AE7" s="72"/>
+      <c r="AF7" s="72"/>
+      <c r="AG7" s="72"/>
+      <c r="AH7" s="72"/>
+      <c r="AI7" s="72"/>
+      <c r="AJ7" s="73"/>
     </row>
     <row r="8" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="C8" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D8" s="80" t="s">
+      <c r="D8" s="74" t="s">
         <v>63</v>
       </c>
-      <c r="E8" s="81"/>
-      <c r="F8" s="81"/>
-      <c r="G8" s="81"/>
-      <c r="H8" s="82"/>
-      <c r="I8" s="80" t="s">
+      <c r="E8" s="75"/>
+      <c r="F8" s="75"/>
+      <c r="G8" s="75"/>
+      <c r="H8" s="76"/>
+      <c r="I8" s="74" t="s">
         <v>64</v>
       </c>
-      <c r="J8" s="81"/>
-      <c r="K8" s="81"/>
-      <c r="L8" s="81"/>
-      <c r="M8" s="81"/>
-      <c r="N8" s="81"/>
-      <c r="O8" s="81"/>
-      <c r="P8" s="81"/>
-      <c r="Q8" s="82"/>
-      <c r="R8" s="80" t="s">
+      <c r="J8" s="75"/>
+      <c r="K8" s="75"/>
+      <c r="L8" s="75"/>
+      <c r="M8" s="75"/>
+      <c r="N8" s="75"/>
+      <c r="O8" s="75"/>
+      <c r="P8" s="75"/>
+      <c r="Q8" s="76"/>
+      <c r="R8" s="74" t="s">
         <v>63</v>
       </c>
-      <c r="S8" s="81"/>
-      <c r="T8" s="81"/>
-      <c r="U8" s="82"/>
-      <c r="V8" s="80" t="s">
+      <c r="S8" s="75"/>
+      <c r="T8" s="75"/>
+      <c r="U8" s="76"/>
+      <c r="V8" s="74" t="s">
         <v>64</v>
       </c>
-      <c r="W8" s="81"/>
-      <c r="X8" s="81"/>
-      <c r="Y8" s="82"/>
-      <c r="Z8" s="80" t="s">
+      <c r="W8" s="75"/>
+      <c r="X8" s="75"/>
+      <c r="Y8" s="76"/>
+      <c r="Z8" s="74" t="s">
         <v>64</v>
       </c>
-      <c r="AA8" s="81"/>
-      <c r="AB8" s="81"/>
-      <c r="AC8" s="82"/>
-      <c r="AD8" s="80" t="s">
+      <c r="AA8" s="75"/>
+      <c r="AB8" s="75"/>
+      <c r="AC8" s="76"/>
+      <c r="AD8" s="74" t="s">
         <v>63</v>
       </c>
-      <c r="AE8" s="81"/>
-      <c r="AF8" s="81"/>
-      <c r="AG8" s="81"/>
-      <c r="AH8" s="81"/>
-      <c r="AI8" s="81"/>
-      <c r="AJ8" s="82"/>
+      <c r="AE8" s="75"/>
+      <c r="AF8" s="75"/>
+      <c r="AG8" s="75"/>
+      <c r="AH8" s="75"/>
+      <c r="AI8" s="75"/>
+      <c r="AJ8" s="76"/>
     </row>
     <row r="9" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="C9" s="1" t="s">
@@ -5039,34 +5147,34 @@
       <c r="C26" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D26" s="71" t="s">
+      <c r="D26" s="77" t="s">
         <v>130</v>
       </c>
-      <c r="E26" s="72"/>
-      <c r="F26" s="72"/>
-      <c r="G26" s="72"/>
-      <c r="H26" s="72"/>
-      <c r="I26" s="72"/>
-      <c r="J26" s="72"/>
-      <c r="K26" s="72"/>
-      <c r="L26" s="72"/>
-      <c r="M26" s="72"/>
-      <c r="N26" s="72"/>
-      <c r="O26" s="72"/>
-      <c r="P26" s="72"/>
-      <c r="Q26" s="72"/>
-      <c r="R26" s="72"/>
-      <c r="S26" s="72"/>
-      <c r="T26" s="72"/>
-      <c r="U26" s="72"/>
-      <c r="V26" s="72"/>
-      <c r="W26" s="72"/>
-      <c r="X26" s="72"/>
-      <c r="Y26" s="72"/>
-      <c r="Z26" s="72"/>
-      <c r="AA26" s="72"/>
-      <c r="AB26" s="72"/>
-      <c r="AC26" s="73"/>
+      <c r="E26" s="78"/>
+      <c r="F26" s="78"/>
+      <c r="G26" s="78"/>
+      <c r="H26" s="78"/>
+      <c r="I26" s="78"/>
+      <c r="J26" s="78"/>
+      <c r="K26" s="78"/>
+      <c r="L26" s="78"/>
+      <c r="M26" s="78"/>
+      <c r="N26" s="78"/>
+      <c r="O26" s="78"/>
+      <c r="P26" s="78"/>
+      <c r="Q26" s="78"/>
+      <c r="R26" s="78"/>
+      <c r="S26" s="78"/>
+      <c r="T26" s="78"/>
+      <c r="U26" s="78"/>
+      <c r="V26" s="78"/>
+      <c r="W26" s="78"/>
+      <c r="X26" s="78"/>
+      <c r="Y26" s="78"/>
+      <c r="Z26" s="78"/>
+      <c r="AA26" s="78"/>
+      <c r="AB26" s="78"/>
+      <c r="AC26" s="79"/>
       <c r="AD26" s="8">
         <v>9.8199999999999985</v>
       </c>
@@ -5204,65 +5312,65 @@
       <c r="C29" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D29" s="74" t="s">
+      <c r="D29" s="80" t="s">
         <v>140</v>
       </c>
-      <c r="E29" s="75"/>
-      <c r="F29" s="75"/>
-      <c r="G29" s="75"/>
-      <c r="H29" s="75"/>
-      <c r="I29" s="75"/>
-      <c r="J29" s="75"/>
-      <c r="K29" s="75"/>
-      <c r="L29" s="75"/>
-      <c r="M29" s="75"/>
-      <c r="N29" s="75"/>
-      <c r="O29" s="75"/>
-      <c r="P29" s="75"/>
-      <c r="Q29" s="76"/>
-      <c r="R29" s="74" t="s">
+      <c r="E29" s="81"/>
+      <c r="F29" s="81"/>
+      <c r="G29" s="81"/>
+      <c r="H29" s="81"/>
+      <c r="I29" s="81"/>
+      <c r="J29" s="81"/>
+      <c r="K29" s="81"/>
+      <c r="L29" s="81"/>
+      <c r="M29" s="81"/>
+      <c r="N29" s="81"/>
+      <c r="O29" s="81"/>
+      <c r="P29" s="81"/>
+      <c r="Q29" s="82"/>
+      <c r="R29" s="80" t="s">
         <v>162</v>
       </c>
-      <c r="S29" s="75"/>
-      <c r="T29" s="75"/>
-      <c r="U29" s="75"/>
-      <c r="V29" s="75"/>
-      <c r="W29" s="75"/>
-      <c r="X29" s="75"/>
-      <c r="Y29" s="75"/>
-      <c r="Z29" s="75"/>
-      <c r="AA29" s="75"/>
-      <c r="AB29" s="75"/>
-      <c r="AC29" s="75"/>
-      <c r="AD29" s="75"/>
-      <c r="AE29" s="75"/>
-      <c r="AF29" s="75"/>
-      <c r="AG29" s="75"/>
-      <c r="AH29" s="75"/>
-      <c r="AI29" s="75"/>
-      <c r="AJ29" s="76"/>
+      <c r="S29" s="81"/>
+      <c r="T29" s="81"/>
+      <c r="U29" s="81"/>
+      <c r="V29" s="81"/>
+      <c r="W29" s="81"/>
+      <c r="X29" s="81"/>
+      <c r="Y29" s="81"/>
+      <c r="Z29" s="81"/>
+      <c r="AA29" s="81"/>
+      <c r="AB29" s="81"/>
+      <c r="AC29" s="81"/>
+      <c r="AD29" s="81"/>
+      <c r="AE29" s="81"/>
+      <c r="AF29" s="81"/>
+      <c r="AG29" s="81"/>
+      <c r="AH29" s="81"/>
+      <c r="AI29" s="81"/>
+      <c r="AJ29" s="82"/>
     </row>
     <row r="30" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="B30" s="21"/>
       <c r="C30" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D30" s="74" t="s">
+      <c r="D30" s="80" t="s">
         <v>132</v>
       </c>
-      <c r="E30" s="75"/>
-      <c r="F30" s="75"/>
-      <c r="G30" s="75"/>
-      <c r="H30" s="75"/>
-      <c r="I30" s="75"/>
-      <c r="J30" s="75"/>
-      <c r="K30" s="75"/>
-      <c r="L30" s="75"/>
-      <c r="M30" s="75"/>
-      <c r="N30" s="75"/>
-      <c r="O30" s="75"/>
-      <c r="P30" s="75"/>
-      <c r="Q30" s="76"/>
+      <c r="E30" s="81"/>
+      <c r="F30" s="81"/>
+      <c r="G30" s="81"/>
+      <c r="H30" s="81"/>
+      <c r="I30" s="81"/>
+      <c r="J30" s="81"/>
+      <c r="K30" s="81"/>
+      <c r="L30" s="81"/>
+      <c r="M30" s="81"/>
+      <c r="N30" s="81"/>
+      <c r="O30" s="81"/>
+      <c r="P30" s="81"/>
+      <c r="Q30" s="82"/>
       <c r="R30" s="47">
         <v>100</v>
       </c>
@@ -5326,22 +5434,22 @@
       <c r="C31" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D31" s="74" t="s">
+      <c r="D31" s="80" t="s">
         <v>131</v>
       </c>
-      <c r="E31" s="75"/>
-      <c r="F31" s="75"/>
-      <c r="G31" s="75"/>
-      <c r="H31" s="75"/>
-      <c r="I31" s="75"/>
-      <c r="J31" s="75"/>
-      <c r="K31" s="75"/>
-      <c r="L31" s="75"/>
-      <c r="M31" s="75"/>
-      <c r="N31" s="75"/>
-      <c r="O31" s="75"/>
-      <c r="P31" s="75"/>
-      <c r="Q31" s="76"/>
+      <c r="E31" s="81"/>
+      <c r="F31" s="81"/>
+      <c r="G31" s="81"/>
+      <c r="H31" s="81"/>
+      <c r="I31" s="81"/>
+      <c r="J31" s="81"/>
+      <c r="K31" s="81"/>
+      <c r="L31" s="81"/>
+      <c r="M31" s="81"/>
+      <c r="N31" s="81"/>
+      <c r="O31" s="81"/>
+      <c r="P31" s="81"/>
+      <c r="Q31" s="82"/>
       <c r="R31" s="47">
         <v>0.01</v>
       </c>
@@ -5893,23 +6001,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="D26:AC26"/>
+    <mergeCell ref="D31:Q31"/>
+    <mergeCell ref="D30:Q30"/>
+    <mergeCell ref="D29:Q29"/>
+    <mergeCell ref="R29:AJ29"/>
+    <mergeCell ref="V7:Y7"/>
+    <mergeCell ref="V8:Y8"/>
+    <mergeCell ref="Z7:AC7"/>
+    <mergeCell ref="Z8:AC8"/>
+    <mergeCell ref="AD7:AJ7"/>
+    <mergeCell ref="AD8:AJ8"/>
     <mergeCell ref="D7:H7"/>
     <mergeCell ref="I7:Q7"/>
     <mergeCell ref="D8:H8"/>
     <mergeCell ref="I8:Q8"/>
     <mergeCell ref="R8:U8"/>
     <mergeCell ref="R7:U7"/>
-    <mergeCell ref="V7:Y7"/>
-    <mergeCell ref="V8:Y8"/>
-    <mergeCell ref="Z7:AC7"/>
-    <mergeCell ref="Z8:AC8"/>
-    <mergeCell ref="AD7:AJ7"/>
-    <mergeCell ref="AD8:AJ8"/>
-    <mergeCell ref="D26:AC26"/>
-    <mergeCell ref="D31:Q31"/>
-    <mergeCell ref="D30:Q30"/>
-    <mergeCell ref="D29:Q29"/>
-    <mergeCell ref="R29:AJ29"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5921,10 +6029,10 @@
   <dimension ref="B5:AJ37"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="3" ySplit="9" topLeftCell="AC10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="9" topLeftCell="AE20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="AJ26" sqref="AD26:AJ26"/>
+      <selection pane="bottomRight" activeCell="AF16" sqref="AF16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -9111,8 +9219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B744582-CF08-477A-A386-996EB0CCB24C}">
   <dimension ref="B5:AD39"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C5" workbookViewId="0">
-      <selection activeCell="S39" sqref="G7:S39"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -12213,7 +12321,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D727E699-FD26-449C-905C-CDD90899F4AB}">
   <dimension ref="B5:AE39"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D3" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="D1" workbookViewId="0">
       <selection activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
@@ -15367,8 +15475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC155531-539F-473A-BEFE-FAB0C4C3EE43}">
   <dimension ref="B4:AE39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="V7" sqref="V7:V20"/>
+    <sheetView showGridLines="0" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="T42" sqref="T42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -18456,12 +18564,1427 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{946DA809-6F7B-4F40-B49B-27E3855F241E}">
+  <dimension ref="A1:Y25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="21" max="24" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="85"/>
+      <c r="B1" s="85" t="s">
+        <v>168</v>
+      </c>
+      <c r="C1" s="85" t="s">
+        <v>169</v>
+      </c>
+      <c r="D1" s="85" t="s">
+        <v>170</v>
+      </c>
+      <c r="E1" s="85" t="s">
+        <v>171</v>
+      </c>
+      <c r="F1" s="85" t="s">
+        <v>172</v>
+      </c>
+      <c r="G1" s="85" t="s">
+        <v>173</v>
+      </c>
+      <c r="H1" s="85" t="s">
+        <v>174</v>
+      </c>
+      <c r="I1" s="85" t="s">
+        <v>175</v>
+      </c>
+      <c r="J1" s="85" t="s">
+        <v>176</v>
+      </c>
+      <c r="K1" s="85" t="s">
+        <v>177</v>
+      </c>
+      <c r="L1" s="85" t="s">
+        <v>178</v>
+      </c>
+      <c r="M1" s="85" t="s">
+        <v>179</v>
+      </c>
+      <c r="N1" s="85" t="s">
+        <v>180</v>
+      </c>
+      <c r="O1" s="85" t="s">
+        <v>181</v>
+      </c>
+      <c r="P1" s="85" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q1" s="85" t="s">
+        <v>183</v>
+      </c>
+      <c r="R1" s="85" t="s">
+        <v>184</v>
+      </c>
+      <c r="S1" s="85" t="s">
+        <v>185</v>
+      </c>
+      <c r="T1" s="85" t="s">
+        <v>186</v>
+      </c>
+      <c r="U1" s="85" t="s">
+        <v>187</v>
+      </c>
+      <c r="V1" s="85" t="s">
+        <v>188</v>
+      </c>
+      <c r="W1" s="85" t="s">
+        <v>189</v>
+      </c>
+      <c r="X1" s="85" t="s">
+        <v>190</v>
+      </c>
+      <c r="Y1" s="85" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="83" t="s">
+        <v>168</v>
+      </c>
+      <c r="B2" s="86">
+        <v>1</v>
+      </c>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="86"/>
+      <c r="O2" s="86"/>
+      <c r="P2" s="86"/>
+      <c r="Q2" s="86"/>
+      <c r="R2" s="86"/>
+      <c r="S2" s="86"/>
+      <c r="T2" s="86"/>
+      <c r="U2" s="86"/>
+      <c r="V2" s="86"/>
+      <c r="W2" s="86"/>
+      <c r="X2" s="86"/>
+      <c r="Y2" s="86"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="83" t="s">
+        <v>169</v>
+      </c>
+      <c r="B3" s="86">
+        <v>0.54532269214902873</v>
+      </c>
+      <c r="C3" s="86">
+        <v>1</v>
+      </c>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="86"/>
+      <c r="K3" s="86"/>
+      <c r="L3" s="86"/>
+      <c r="M3" s="86"/>
+      <c r="N3" s="86"/>
+      <c r="O3" s="86"/>
+      <c r="P3" s="86"/>
+      <c r="Q3" s="86"/>
+      <c r="R3" s="86"/>
+      <c r="S3" s="86"/>
+      <c r="T3" s="86"/>
+      <c r="U3" s="86"/>
+      <c r="V3" s="86"/>
+      <c r="W3" s="86"/>
+      <c r="X3" s="86"/>
+      <c r="Y3" s="86"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="83" t="s">
+        <v>170</v>
+      </c>
+      <c r="B4" s="86">
+        <v>-0.5693038369307919</v>
+      </c>
+      <c r="C4" s="86">
+        <v>-0.99796012768573961</v>
+      </c>
+      <c r="D4" s="86">
+        <v>1</v>
+      </c>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="86"/>
+      <c r="I4" s="86"/>
+      <c r="J4" s="86"/>
+      <c r="K4" s="86"/>
+      <c r="L4" s="86"/>
+      <c r="M4" s="86"/>
+      <c r="N4" s="86"/>
+      <c r="O4" s="86"/>
+      <c r="P4" s="86"/>
+      <c r="Q4" s="86"/>
+      <c r="R4" s="86"/>
+      <c r="S4" s="86"/>
+      <c r="T4" s="86"/>
+      <c r="U4" s="86"/>
+      <c r="V4" s="86"/>
+      <c r="W4" s="86"/>
+      <c r="X4" s="86"/>
+      <c r="Y4" s="86"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="83" t="s">
+        <v>171</v>
+      </c>
+      <c r="B5" s="86">
+        <v>0.37186951414850039</v>
+      </c>
+      <c r="C5" s="86">
+        <v>0.78685883447847571</v>
+      </c>
+      <c r="D5" s="86">
+        <v>-0.78525374292679184</v>
+      </c>
+      <c r="E5" s="86">
+        <v>1</v>
+      </c>
+      <c r="F5" s="86"/>
+      <c r="G5" s="86"/>
+      <c r="H5" s="86"/>
+      <c r="I5" s="86"/>
+      <c r="J5" s="86"/>
+      <c r="K5" s="86"/>
+      <c r="L5" s="86"/>
+      <c r="M5" s="86"/>
+      <c r="N5" s="86"/>
+      <c r="O5" s="86"/>
+      <c r="P5" s="86"/>
+      <c r="Q5" s="86"/>
+      <c r="R5" s="86"/>
+      <c r="S5" s="86"/>
+      <c r="T5" s="86"/>
+      <c r="U5" s="86"/>
+      <c r="V5" s="86"/>
+      <c r="W5" s="86"/>
+      <c r="X5" s="86"/>
+      <c r="Y5" s="86"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="83" t="s">
+        <v>172</v>
+      </c>
+      <c r="B6" s="86">
+        <v>-0.52142976010762865</v>
+      </c>
+      <c r="C6" s="86">
+        <v>-0.80214333130506021</v>
+      </c>
+      <c r="D6" s="86">
+        <v>0.80050706133146232</v>
+      </c>
+      <c r="E6" s="86">
+        <v>-0.81378476241257014</v>
+      </c>
+      <c r="F6" s="86">
+        <v>1</v>
+      </c>
+      <c r="G6" s="86"/>
+      <c r="H6" s="86"/>
+      <c r="I6" s="86"/>
+      <c r="J6" s="86"/>
+      <c r="K6" s="86"/>
+      <c r="L6" s="86"/>
+      <c r="M6" s="86"/>
+      <c r="N6" s="86"/>
+      <c r="O6" s="86"/>
+      <c r="P6" s="86"/>
+      <c r="Q6" s="86"/>
+      <c r="R6" s="86"/>
+      <c r="S6" s="86"/>
+      <c r="T6" s="86"/>
+      <c r="U6" s="86"/>
+      <c r="V6" s="86"/>
+      <c r="W6" s="86"/>
+      <c r="X6" s="86"/>
+      <c r="Y6" s="86"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="83" t="s">
+        <v>173</v>
+      </c>
+      <c r="B7" s="86">
+        <v>-0.40937219968250366</v>
+      </c>
+      <c r="C7" s="86">
+        <v>-0.24062558079337174</v>
+      </c>
+      <c r="D7" s="86">
+        <v>0.24013473533300858</v>
+      </c>
+      <c r="E7" s="86">
+        <v>-0.17615657920993991</v>
+      </c>
+      <c r="F7" s="86">
+        <v>0.21844348946250985</v>
+      </c>
+      <c r="G7" s="86">
+        <v>1</v>
+      </c>
+      <c r="H7" s="86"/>
+      <c r="I7" s="86"/>
+      <c r="J7" s="86"/>
+      <c r="K7" s="86"/>
+      <c r="L7" s="86"/>
+      <c r="M7" s="86"/>
+      <c r="N7" s="86"/>
+      <c r="O7" s="86"/>
+      <c r="P7" s="86"/>
+      <c r="Q7" s="86"/>
+      <c r="R7" s="86"/>
+      <c r="S7" s="86"/>
+      <c r="T7" s="86"/>
+      <c r="U7" s="86"/>
+      <c r="V7" s="86"/>
+      <c r="W7" s="86"/>
+      <c r="X7" s="86"/>
+      <c r="Y7" s="86"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="83" t="s">
+        <v>174</v>
+      </c>
+      <c r="B8" s="86">
+        <v>0.2064701282579329</v>
+      </c>
+      <c r="C8" s="86">
+        <v>0.13363062095621231</v>
+      </c>
+      <c r="D8" s="86">
+        <v>-0.13335803155218626</v>
+      </c>
+      <c r="E8" s="86">
+        <v>9.7827974015615812E-2</v>
+      </c>
+      <c r="F8" s="86">
+        <v>-0.1213118698538683</v>
+      </c>
+      <c r="G8" s="86">
+        <v>-0.59150144445301611</v>
+      </c>
+      <c r="H8" s="86">
+        <v>1</v>
+      </c>
+      <c r="I8" s="86"/>
+      <c r="J8" s="86"/>
+      <c r="K8" s="86"/>
+      <c r="L8" s="86"/>
+      <c r="M8" s="86"/>
+      <c r="N8" s="86"/>
+      <c r="O8" s="86"/>
+      <c r="P8" s="86"/>
+      <c r="Q8" s="86"/>
+      <c r="R8" s="86"/>
+      <c r="S8" s="86"/>
+      <c r="T8" s="86"/>
+      <c r="U8" s="86"/>
+      <c r="V8" s="86"/>
+      <c r="W8" s="86"/>
+      <c r="X8" s="86"/>
+      <c r="Y8" s="86"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="83" t="s">
+        <v>175</v>
+      </c>
+      <c r="B9" s="86">
+        <v>0.2064701282579329</v>
+      </c>
+      <c r="C9" s="86">
+        <v>0.13363062095621234</v>
+      </c>
+      <c r="D9" s="86">
+        <v>-0.13335803155218626</v>
+      </c>
+      <c r="E9" s="86">
+        <v>9.7827974015615812E-2</v>
+      </c>
+      <c r="F9" s="86">
+        <v>-0.1213118698538683</v>
+      </c>
+      <c r="G9" s="86">
+        <v>-0.59150144445301611</v>
+      </c>
+      <c r="H9" s="86">
+        <v>-3.1250000000000097E-2</v>
+      </c>
+      <c r="I9" s="86">
+        <v>1</v>
+      </c>
+      <c r="J9" s="86"/>
+      <c r="K9" s="86"/>
+      <c r="L9" s="86"/>
+      <c r="M9" s="86"/>
+      <c r="N9" s="86"/>
+      <c r="O9" s="86"/>
+      <c r="P9" s="86"/>
+      <c r="Q9" s="86"/>
+      <c r="R9" s="86"/>
+      <c r="S9" s="86"/>
+      <c r="T9" s="86"/>
+      <c r="U9" s="86"/>
+      <c r="V9" s="86"/>
+      <c r="W9" s="86"/>
+      <c r="X9" s="86"/>
+      <c r="Y9" s="86"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="83" t="s">
+        <v>176</v>
+      </c>
+      <c r="B10" s="86">
+        <v>4.7941143432472522E-2</v>
+      </c>
+      <c r="C10" s="86">
+        <v>0.1689159811730441</v>
+      </c>
+      <c r="D10" s="86">
+        <v>-0.16857141413961296</v>
+      </c>
+      <c r="E10" s="86">
+        <v>0.15141990995385896</v>
+      </c>
+      <c r="F10" s="86">
+        <v>-0.12657001882882701</v>
+      </c>
+      <c r="G10" s="86">
+        <v>-4.0645506075046016E-2</v>
+      </c>
+      <c r="H10" s="86">
+        <v>2.2572347453581727E-2</v>
+      </c>
+      <c r="I10" s="86">
+        <v>2.2572347453581727E-2</v>
+      </c>
+      <c r="J10" s="86">
+        <v>1</v>
+      </c>
+      <c r="K10" s="86"/>
+      <c r="L10" s="86"/>
+      <c r="M10" s="86"/>
+      <c r="N10" s="86"/>
+      <c r="O10" s="86"/>
+      <c r="P10" s="86"/>
+      <c r="Q10" s="86"/>
+      <c r="R10" s="86"/>
+      <c r="S10" s="86"/>
+      <c r="T10" s="86"/>
+      <c r="U10" s="86"/>
+      <c r="V10" s="86"/>
+      <c r="W10" s="86"/>
+      <c r="X10" s="86"/>
+      <c r="Y10" s="86"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="83" t="s">
+        <v>177</v>
+      </c>
+      <c r="B11" s="86">
+        <v>-0.42354601289696908</v>
+      </c>
+      <c r="C11" s="86">
+        <v>-0.46770717334674256</v>
+      </c>
+      <c r="D11" s="86">
+        <v>0.46675311043265155</v>
+      </c>
+      <c r="E11" s="86">
+        <v>-0.41926274578121053</v>
+      </c>
+      <c r="F11" s="86">
+        <v>0.35045651291117474</v>
+      </c>
+      <c r="G11" s="86">
+        <v>0.11254231022778623</v>
+      </c>
+      <c r="H11" s="86">
+        <v>-6.2500000000000042E-2</v>
+      </c>
+      <c r="I11" s="86">
+        <v>-6.2500000000000042E-2</v>
+      </c>
+      <c r="J11" s="86">
+        <v>-0.7674598134217786</v>
+      </c>
+      <c r="K11" s="86">
+        <v>1</v>
+      </c>
+      <c r="L11" s="86"/>
+      <c r="M11" s="86"/>
+      <c r="N11" s="86"/>
+      <c r="O11" s="86"/>
+      <c r="P11" s="86"/>
+      <c r="Q11" s="86"/>
+      <c r="R11" s="86"/>
+      <c r="S11" s="86"/>
+      <c r="T11" s="86"/>
+      <c r="U11" s="86"/>
+      <c r="V11" s="86"/>
+      <c r="W11" s="86"/>
+      <c r="X11" s="86"/>
+      <c r="Y11" s="86"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="83" t="s">
+        <v>178</v>
+      </c>
+      <c r="B12" s="86">
+        <v>-0.56094629067505208</v>
+      </c>
+      <c r="C12" s="86">
+        <v>-0.48279450151921821</v>
+      </c>
+      <c r="D12" s="86">
+        <v>0.481809662382092</v>
+      </c>
+      <c r="E12" s="86">
+        <v>-0.3534430028951282</v>
+      </c>
+      <c r="F12" s="86">
+        <v>0.43828804592365272</v>
+      </c>
+      <c r="G12" s="86">
+        <v>0.27591017991328259</v>
+      </c>
+      <c r="H12" s="86">
+        <v>-0.15322580645161285</v>
+      </c>
+      <c r="I12" s="86">
+        <v>-0.15322580645161291</v>
+      </c>
+      <c r="J12" s="86">
+        <v>-8.1551706929069462E-2</v>
+      </c>
+      <c r="K12" s="86">
+        <v>0.22580645161290325</v>
+      </c>
+      <c r="L12" s="86">
+        <v>1</v>
+      </c>
+      <c r="M12" s="86"/>
+      <c r="N12" s="86"/>
+      <c r="O12" s="86"/>
+      <c r="P12" s="86"/>
+      <c r="Q12" s="86"/>
+      <c r="R12" s="86"/>
+      <c r="S12" s="86"/>
+      <c r="T12" s="86"/>
+      <c r="U12" s="86"/>
+      <c r="V12" s="86"/>
+      <c r="W12" s="86"/>
+      <c r="X12" s="86"/>
+      <c r="Y12" s="86"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="83" t="s">
+        <v>179</v>
+      </c>
+      <c r="B13" s="86">
+        <v>5.4122225092713113E-3</v>
+      </c>
+      <c r="C13" s="86">
+        <v>0.22252462162536571</v>
+      </c>
+      <c r="D13" s="86">
+        <v>-0.22207069981047078</v>
+      </c>
+      <c r="E13" s="86">
+        <v>0.1629052738543682</v>
+      </c>
+      <c r="F13" s="86">
+        <v>-0.20201116888279116</v>
+      </c>
+      <c r="G13" s="86">
+        <v>9.3703953559000658E-2</v>
+      </c>
+      <c r="H13" s="86">
+        <v>-5.2038180890226576E-2</v>
+      </c>
+      <c r="I13" s="86">
+        <v>-5.2038180890226576E-2</v>
+      </c>
+      <c r="J13" s="86">
+        <v>3.7587964797009037E-2</v>
+      </c>
+      <c r="K13" s="86">
+        <v>-0.10407636178045325</v>
+      </c>
+      <c r="L13" s="86">
+        <v>-0.6983188145269128</v>
+      </c>
+      <c r="M13" s="86">
+        <v>1</v>
+      </c>
+      <c r="N13" s="86"/>
+      <c r="O13" s="86"/>
+      <c r="P13" s="86"/>
+      <c r="Q13" s="86"/>
+      <c r="R13" s="86"/>
+      <c r="S13" s="86"/>
+      <c r="T13" s="86"/>
+      <c r="U13" s="86"/>
+      <c r="V13" s="86"/>
+      <c r="W13" s="86"/>
+      <c r="X13" s="86"/>
+      <c r="Y13" s="86"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="83" t="s">
+        <v>180</v>
+      </c>
+      <c r="B14" s="86">
+        <v>6.8298341815840067E-15</v>
+      </c>
+      <c r="C14" s="86">
+        <v>1.0443996526137254E-16</v>
+      </c>
+      <c r="D14" s="86">
+        <v>-1.0422692106773353E-16</v>
+      </c>
+      <c r="E14" s="86">
+        <v>1.5603704304785335E-17</v>
+      </c>
+      <c r="F14" s="86">
+        <v>-1.6554503680555037E-16</v>
+      </c>
+      <c r="G14" s="86">
+        <v>2.9587283593366958E-16</v>
+      </c>
+      <c r="H14" s="86">
+        <v>-6.9781887052612257E-17</v>
+      </c>
+      <c r="I14" s="86">
+        <v>-6.9781887052612257E-17</v>
+      </c>
+      <c r="J14" s="86">
+        <v>-2.3690120647793115E-16</v>
+      </c>
+      <c r="K14" s="86">
+        <v>0</v>
+      </c>
+      <c r="L14" s="86">
+        <v>-2.9713577712725213E-16</v>
+      </c>
+      <c r="M14" s="86">
+        <v>1.3072760860698715E-16</v>
+      </c>
+      <c r="N14" s="86">
+        <v>1</v>
+      </c>
+      <c r="O14" s="86"/>
+      <c r="P14" s="86"/>
+      <c r="Q14" s="86"/>
+      <c r="R14" s="86"/>
+      <c r="S14" s="86"/>
+      <c r="T14" s="86"/>
+      <c r="U14" s="86"/>
+      <c r="V14" s="86"/>
+      <c r="W14" s="86"/>
+      <c r="X14" s="86"/>
+      <c r="Y14" s="86"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="83" t="s">
+        <v>181</v>
+      </c>
+      <c r="B15" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C15" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D15" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E15" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F15" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G15" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H15" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I15" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J15" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K15" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L15" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M15" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N15" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O15" s="86">
+        <v>1</v>
+      </c>
+      <c r="P15" s="86"/>
+      <c r="Q15" s="86"/>
+      <c r="R15" s="86"/>
+      <c r="S15" s="86"/>
+      <c r="T15" s="86"/>
+      <c r="U15" s="86"/>
+      <c r="V15" s="86"/>
+      <c r="W15" s="86"/>
+      <c r="X15" s="86"/>
+      <c r="Y15" s="86"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="83" t="s">
+        <v>182</v>
+      </c>
+      <c r="B16" s="86">
+        <v>-0.63644724213007908</v>
+      </c>
+      <c r="C16" s="86">
+        <v>-0.64888568452304984</v>
+      </c>
+      <c r="D16" s="86">
+        <v>0.64756204058007127</v>
+      </c>
+      <c r="E16" s="86">
+        <v>-0.47503462477680736</v>
+      </c>
+      <c r="F16" s="86">
+        <v>0.58906809792264891</v>
+      </c>
+      <c r="G16" s="86">
+        <v>0.37082892492880132</v>
+      </c>
+      <c r="H16" s="86">
+        <v>-0.20593861776197844</v>
+      </c>
+      <c r="I16" s="86">
+        <v>-0.20593861776197844</v>
+      </c>
+      <c r="J16" s="86">
+        <v>-0.10960716207035329</v>
+      </c>
+      <c r="K16" s="86">
+        <v>0.30348848933344197</v>
+      </c>
+      <c r="L16" s="86">
+        <v>0.74403629643037428</v>
+      </c>
+      <c r="M16" s="86">
+        <v>-0.34293347338819458</v>
+      </c>
+      <c r="N16" s="86">
+        <v>-2.3598342282655199E-16</v>
+      </c>
+      <c r="O16" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P16" s="86">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="86"/>
+      <c r="R16" s="86"/>
+      <c r="S16" s="86"/>
+      <c r="T16" s="86"/>
+      <c r="U16" s="86"/>
+      <c r="V16" s="86"/>
+      <c r="W16" s="86"/>
+      <c r="X16" s="86"/>
+      <c r="Y16" s="86"/>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="83" t="s">
+        <v>183</v>
+      </c>
+      <c r="B17" s="86">
+        <v>-0.63090569434588195</v>
+      </c>
+      <c r="C17" s="86">
+        <v>-0.64323583518874972</v>
+      </c>
+      <c r="D17" s="86">
+        <v>0.64192371621700783</v>
+      </c>
+      <c r="E17" s="86">
+        <v>-0.47089849706960152</v>
+      </c>
+      <c r="F17" s="86">
+        <v>0.58393908046967202</v>
+      </c>
+      <c r="G17" s="86">
+        <v>0.3676001165198311</v>
+      </c>
+      <c r="H17" s="86">
+        <v>-0.20414550968420586</v>
+      </c>
+      <c r="I17" s="86">
+        <v>-0.20414550968420586</v>
+      </c>
+      <c r="J17" s="86">
+        <v>-0.10865281222657011</v>
+      </c>
+      <c r="K17" s="86">
+        <v>0.3008460142714614</v>
+      </c>
+      <c r="L17" s="86">
+        <v>0.73755797047197014</v>
+      </c>
+      <c r="M17" s="86">
+        <v>-0.339947550747975</v>
+      </c>
+      <c r="N17" s="86">
+        <v>-2.1497449050234554E-16</v>
+      </c>
+      <c r="O17" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P17" s="86">
+        <v>0.99129299741224342</v>
+      </c>
+      <c r="Q17" s="86">
+        <v>1</v>
+      </c>
+      <c r="R17" s="86"/>
+      <c r="S17" s="86"/>
+      <c r="T17" s="86"/>
+      <c r="U17" s="86"/>
+      <c r="V17" s="86"/>
+      <c r="W17" s="86"/>
+      <c r="X17" s="86"/>
+      <c r="Y17" s="86"/>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="83" t="s">
+        <v>184</v>
+      </c>
+      <c r="B18" s="86">
+        <v>-0.26911365410861021</v>
+      </c>
+      <c r="C18" s="86">
+        <v>-0.30860669992418377</v>
+      </c>
+      <c r="D18" s="86">
+        <v>0.30752176228926043</v>
+      </c>
+      <c r="E18" s="86">
+        <v>6.976819652324362E-2</v>
+      </c>
+      <c r="F18" s="86">
+        <v>0.26379467179224692</v>
+      </c>
+      <c r="G18" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H18" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I18" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J18" s="86">
+        <v>-3.9904344223381058E-2</v>
+      </c>
+      <c r="K18" s="86">
+        <v>0.11526067913468739</v>
+      </c>
+      <c r="L18" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M18" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N18" s="86">
+        <v>1.6764008022404885E-15</v>
+      </c>
+      <c r="O18" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P18" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q18" s="86">
+        <v>0</v>
+      </c>
+      <c r="R18" s="86">
+        <v>1</v>
+      </c>
+      <c r="S18" s="86"/>
+      <c r="T18" s="86"/>
+      <c r="U18" s="86"/>
+      <c r="V18" s="86"/>
+      <c r="W18" s="86"/>
+      <c r="X18" s="86"/>
+      <c r="Y18" s="86"/>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="83" t="s">
+        <v>185</v>
+      </c>
+      <c r="B19" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C19" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D19" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E19" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F19" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G19" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H19" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I19" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J19" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K19" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L19" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M19" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N19" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O19" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P19" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q19" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R19" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S19" s="86">
+        <v>1</v>
+      </c>
+      <c r="T19" s="86"/>
+      <c r="U19" s="86"/>
+      <c r="V19" s="86"/>
+      <c r="W19" s="86"/>
+      <c r="X19" s="86"/>
+      <c r="Y19" s="86"/>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="83" t="s">
+        <v>186</v>
+      </c>
+      <c r="B20" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C20" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D20" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E20" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F20" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G20" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H20" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I20" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J20" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K20" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L20" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M20" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N20" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O20" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P20" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q20" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R20" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S20" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T20" s="86">
+        <v>1</v>
+      </c>
+      <c r="U20" s="86"/>
+      <c r="V20" s="86"/>
+      <c r="W20" s="86"/>
+      <c r="X20" s="86"/>
+      <c r="Y20" s="86"/>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="83" t="s">
+        <v>187</v>
+      </c>
+      <c r="B21" s="86">
+        <v>-0.65684655212468779</v>
+      </c>
+      <c r="C21" s="86">
+        <v>-0.74501977471698688</v>
+      </c>
+      <c r="D21" s="86">
+        <v>0.74350002950496497</v>
+      </c>
+      <c r="E21" s="86">
+        <v>-0.54541223142273476</v>
+      </c>
+      <c r="F21" s="86">
+        <v>0.67634005815658671</v>
+      </c>
+      <c r="G21" s="86">
+        <v>0.30504180067972075</v>
+      </c>
+      <c r="H21" s="86">
+        <v>-0.15636742794798861</v>
+      </c>
+      <c r="I21" s="86">
+        <v>-0.15636742794798861</v>
+      </c>
+      <c r="J21" s="86">
+        <v>-0.12584574623964012</v>
+      </c>
+      <c r="K21" s="86">
+        <v>0.34845109292030901</v>
+      </c>
+      <c r="L21" s="86">
+        <v>0.76338890244138069</v>
+      </c>
+      <c r="M21" s="86">
+        <v>-0.38484971956554048</v>
+      </c>
+      <c r="N21" s="86">
+        <v>2.2613484572857596E-16</v>
+      </c>
+      <c r="O21" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P21" s="86">
+        <v>0.78920382806196909</v>
+      </c>
+      <c r="Q21" s="86">
+        <v>0.79023941466963321</v>
+      </c>
+      <c r="R21" s="86">
+        <v>0.86221131987965471</v>
+      </c>
+      <c r="S21" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T21" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U21" s="86">
+        <v>1</v>
+      </c>
+      <c r="V21" s="86"/>
+      <c r="W21" s="86"/>
+      <c r="X21" s="86"/>
+      <c r="Y21" s="86"/>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="83" t="s">
+        <v>188</v>
+      </c>
+      <c r="B22" s="86">
+        <v>-0.6139086961176804</v>
+      </c>
+      <c r="C22" s="86">
+        <v>-0.5947704002421923</v>
+      </c>
+      <c r="D22" s="86">
+        <v>0.59355714456939646</v>
+      </c>
+      <c r="E22" s="86">
+        <v>-0.55235314072510733</v>
+      </c>
+      <c r="F22" s="86">
+        <v>0.46221314622956378</v>
+      </c>
+      <c r="G22" s="86">
+        <v>0.17095594914778819</v>
+      </c>
+      <c r="H22" s="86">
+        <v>-9.7651533876473781E-2</v>
+      </c>
+      <c r="I22" s="86">
+        <v>-0.12945252681650973</v>
+      </c>
+      <c r="J22" s="86">
+        <v>-0.16682497990664674</v>
+      </c>
+      <c r="K22" s="86">
+        <v>0.75679938754267162</v>
+      </c>
+      <c r="L22" s="86">
+        <v>0.28988744818847967</v>
+      </c>
+      <c r="M22" s="86">
+        <v>-0.12730765766412053</v>
+      </c>
+      <c r="N22" s="86">
+        <v>-5.1107312306118231E-16</v>
+      </c>
+      <c r="O22" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P22" s="86">
+        <v>0.38961465936441286</v>
+      </c>
+      <c r="Q22" s="86">
+        <v>0.38622228351709892</v>
+      </c>
+      <c r="R22" s="86">
+        <v>0.13174403224453668</v>
+      </c>
+      <c r="S22" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T22" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U22" s="86">
+        <v>0.44233475653467785</v>
+      </c>
+      <c r="V22" s="86">
+        <v>1</v>
+      </c>
+      <c r="W22" s="86"/>
+      <c r="X22" s="86"/>
+      <c r="Y22" s="86"/>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="83" t="s">
+        <v>189</v>
+      </c>
+      <c r="B23" s="86">
+        <v>-0.21401478203302254</v>
+      </c>
+      <c r="C23" s="86">
+        <v>0.6198960282048539</v>
+      </c>
+      <c r="D23" s="86">
+        <v>-0.6186315194591987</v>
+      </c>
+      <c r="E23" s="86">
+        <v>0.48946860211463999</v>
+      </c>
+      <c r="F23" s="86">
+        <v>-0.48615421148870491</v>
+      </c>
+      <c r="G23" s="86">
+        <v>0.12338455418429231</v>
+      </c>
+      <c r="H23" s="86">
+        <v>-6.5234209302127172E-2</v>
+      </c>
+      <c r="I23" s="86">
+        <v>-6.5234209302127172E-2</v>
+      </c>
+      <c r="J23" s="86">
+        <v>8.9003793955071492E-2</v>
+      </c>
+      <c r="K23" s="86">
+        <v>-4.5466267089361322E-2</v>
+      </c>
+      <c r="L23" s="86">
+        <v>2.8057724431021706E-3</v>
+      </c>
+      <c r="M23" s="86">
+        <v>0.29692043293801551</v>
+      </c>
+      <c r="N23" s="86">
+        <v>-1.4953176328571059E-15</v>
+      </c>
+      <c r="O23" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P23" s="86">
+        <v>-0.12444351312777445</v>
+      </c>
+      <c r="Q23" s="86">
+        <v>-0.12335998313694138</v>
+      </c>
+      <c r="R23" s="86">
+        <v>-0.2483609982908293</v>
+      </c>
+      <c r="S23" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T23" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U23" s="86">
+        <v>-0.22700623618415558</v>
+      </c>
+      <c r="V23" s="86">
+        <v>-1.911066179871496E-2</v>
+      </c>
+      <c r="W23" s="86">
+        <v>1</v>
+      </c>
+      <c r="X23" s="86"/>
+      <c r="Y23" s="86"/>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="83" t="s">
+        <v>190</v>
+      </c>
+      <c r="B24" s="86">
+        <v>0.88528380522770744</v>
+      </c>
+      <c r="C24" s="86">
+        <v>0.23877755083096783</v>
+      </c>
+      <c r="D24" s="86">
+        <v>-0.26368965366492136</v>
+      </c>
+      <c r="E24" s="86">
+        <v>0.12156889234959198</v>
+      </c>
+      <c r="F24" s="86">
+        <v>-0.28454014655997628</v>
+      </c>
+      <c r="G24" s="86">
+        <v>-0.49782758967774171</v>
+      </c>
+      <c r="H24" s="86">
+        <v>9.1766396712619255E-2</v>
+      </c>
+      <c r="I24" s="86">
+        <v>0.20604153224154134</v>
+      </c>
+      <c r="J24" s="86">
+        <v>2.501292668571123E-3</v>
+      </c>
+      <c r="K24" s="86">
+        <v>-0.24240180263710734</v>
+      </c>
+      <c r="L24" s="86">
+        <v>-0.44950454092705999</v>
+      </c>
+      <c r="M24" s="86">
+        <v>-9.4570075977804618E-2</v>
+      </c>
+      <c r="N24" s="86">
+        <v>-9.7431870026720007E-16</v>
+      </c>
+      <c r="O24" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P24" s="86">
+        <v>-0.48523636547251753</v>
+      </c>
+      <c r="Q24" s="86">
+        <v>-0.48101141118267471</v>
+      </c>
+      <c r="R24" s="86">
+        <v>-0.14641107432910491</v>
+      </c>
+      <c r="S24" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T24" s="86" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U24" s="86">
+        <v>-0.46861278010777019</v>
+      </c>
+      <c r="V24" s="86">
+        <v>-0.36164875740461316</v>
+      </c>
+      <c r="W24" s="86">
+        <v>-0.43432737670120619</v>
+      </c>
+      <c r="X24" s="86">
+        <v>1</v>
+      </c>
+      <c r="Y24" s="86"/>
+    </row>
+    <row r="25" spans="1:25" ht="18.5" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A25" s="84" t="s">
+        <v>191</v>
+      </c>
+      <c r="B25" s="87">
+        <v>-0.53311575526124477</v>
+      </c>
+      <c r="C25" s="87" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D25" s="87" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E25" s="87" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F25" s="87" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G25" s="87" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H25" s="87" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I25" s="87" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J25" s="87">
+        <v>-0.36806088975493934</v>
+      </c>
+      <c r="K25" s="87">
+        <v>0.66445163137920571</v>
+      </c>
+      <c r="L25" s="87" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M25" s="87" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N25" s="87">
+        <v>-2.0100642720231223E-16</v>
+      </c>
+      <c r="O25" s="87" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P25" s="87" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q25" s="87" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R25" s="87" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S25" s="87" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T25" s="87" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U25" s="87" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V25" s="87">
+        <v>0.63089909132674227</v>
+      </c>
+      <c r="W25" s="87">
+        <v>0.59991265498140522</v>
+      </c>
+      <c r="X25" s="87">
+        <v>-0.53311575526124488</v>
+      </c>
+      <c r="Y25" s="87">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <conditionalFormatting sqref="A1:Y25">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFFD9269-7F18-4E64-8D48-3C1F1E4D91C0}">
   <dimension ref="B2:AG39"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="6" topLeftCell="Q1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AB2" sqref="AB2:AF2"/>
+      <selection pane="topRight" activeCell="AB30" sqref="AB30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
EDA ipynb update comment and umap color bar
</commit_message>
<xml_diff>
--- a/chapter2/input/chapter2_demo_data.xlsx
+++ b/chapter2/input/chapter2_demo_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\副業関連\独立\執筆\practical-mi-guide\chapter2\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81551455-ABA1-499F-8765-2586EC360A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA7181E-8951-46DD-B9D4-9AA0D1974FC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="3850" windowWidth="36790" windowHeight="17100" activeTab="5" xr2:uid="{AFFCA931-CB2A-4AED-B7E5-2638B5FCE6AD}"/>
+    <workbookView xWindow="5890" yWindow="3850" windowWidth="32240" windowHeight="17100" activeTab="5" xr2:uid="{AFFCA931-CB2A-4AED-B7E5-2638B5FCE6AD}"/>
   </bookViews>
   <sheets>
     <sheet name="初期データ" sheetId="2" r:id="rId1"/>
@@ -1420,7 +1420,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1634,23 +1634,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1670,20 +1664,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3330,101 +3327,101 @@
       <c r="C7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="71">
+      <c r="D7" s="81">
         <v>45310</v>
       </c>
-      <c r="E7" s="72"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="73"/>
-      <c r="I7" s="71">
+      <c r="E7" s="82"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="82"/>
+      <c r="H7" s="83"/>
+      <c r="I7" s="81">
         <v>45321</v>
       </c>
-      <c r="J7" s="72"/>
-      <c r="K7" s="72"/>
-      <c r="L7" s="72"/>
-      <c r="M7" s="72"/>
-      <c r="N7" s="72"/>
-      <c r="O7" s="72"/>
-      <c r="P7" s="72"/>
-      <c r="Q7" s="73"/>
-      <c r="R7" s="71">
+      <c r="J7" s="82"/>
+      <c r="K7" s="82"/>
+      <c r="L7" s="82"/>
+      <c r="M7" s="82"/>
+      <c r="N7" s="82"/>
+      <c r="O7" s="82"/>
+      <c r="P7" s="82"/>
+      <c r="Q7" s="83"/>
+      <c r="R7" s="81">
         <v>45337</v>
       </c>
-      <c r="S7" s="72"/>
-      <c r="T7" s="72"/>
-      <c r="U7" s="73"/>
-      <c r="V7" s="71">
+      <c r="S7" s="82"/>
+      <c r="T7" s="82"/>
+      <c r="U7" s="83"/>
+      <c r="V7" s="81">
         <v>45350</v>
       </c>
-      <c r="W7" s="72"/>
-      <c r="X7" s="72"/>
-      <c r="Y7" s="73"/>
-      <c r="Z7" s="71">
+      <c r="W7" s="82"/>
+      <c r="X7" s="82"/>
+      <c r="Y7" s="83"/>
+      <c r="Z7" s="81">
         <v>45366</v>
       </c>
-      <c r="AA7" s="72"/>
-      <c r="AB7" s="72"/>
-      <c r="AC7" s="73"/>
-      <c r="AD7" s="71">
+      <c r="AA7" s="82"/>
+      <c r="AB7" s="82"/>
+      <c r="AC7" s="83"/>
+      <c r="AD7" s="81">
         <v>45392</v>
       </c>
-      <c r="AE7" s="72"/>
-      <c r="AF7" s="72"/>
-      <c r="AG7" s="72"/>
-      <c r="AH7" s="72"/>
-      <c r="AI7" s="72"/>
-      <c r="AJ7" s="73"/>
+      <c r="AE7" s="82"/>
+      <c r="AF7" s="82"/>
+      <c r="AG7" s="82"/>
+      <c r="AH7" s="82"/>
+      <c r="AI7" s="82"/>
+      <c r="AJ7" s="83"/>
     </row>
     <row r="8" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="C8" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D8" s="74" t="s">
+      <c r="D8" s="84" t="s">
         <v>63</v>
       </c>
-      <c r="E8" s="75"/>
-      <c r="F8" s="75"/>
-      <c r="G8" s="75"/>
-      <c r="H8" s="76"/>
-      <c r="I8" s="74" t="s">
+      <c r="E8" s="85"/>
+      <c r="F8" s="85"/>
+      <c r="G8" s="85"/>
+      <c r="H8" s="86"/>
+      <c r="I8" s="84" t="s">
         <v>64</v>
       </c>
-      <c r="J8" s="75"/>
-      <c r="K8" s="75"/>
-      <c r="L8" s="75"/>
-      <c r="M8" s="75"/>
-      <c r="N8" s="75"/>
-      <c r="O8" s="75"/>
-      <c r="P8" s="75"/>
-      <c r="Q8" s="76"/>
-      <c r="R8" s="74" t="s">
+      <c r="J8" s="85"/>
+      <c r="K8" s="85"/>
+      <c r="L8" s="85"/>
+      <c r="M8" s="85"/>
+      <c r="N8" s="85"/>
+      <c r="O8" s="85"/>
+      <c r="P8" s="85"/>
+      <c r="Q8" s="86"/>
+      <c r="R8" s="84" t="s">
         <v>63</v>
       </c>
-      <c r="S8" s="75"/>
-      <c r="T8" s="75"/>
-      <c r="U8" s="76"/>
-      <c r="V8" s="74" t="s">
+      <c r="S8" s="85"/>
+      <c r="T8" s="85"/>
+      <c r="U8" s="86"/>
+      <c r="V8" s="84" t="s">
         <v>64</v>
       </c>
-      <c r="W8" s="75"/>
-      <c r="X8" s="75"/>
-      <c r="Y8" s="76"/>
-      <c r="Z8" s="74" t="s">
+      <c r="W8" s="85"/>
+      <c r="X8" s="85"/>
+      <c r="Y8" s="86"/>
+      <c r="Z8" s="84" t="s">
         <v>64</v>
       </c>
-      <c r="AA8" s="75"/>
-      <c r="AB8" s="75"/>
-      <c r="AC8" s="76"/>
-      <c r="AD8" s="74" t="s">
+      <c r="AA8" s="85"/>
+      <c r="AB8" s="85"/>
+      <c r="AC8" s="86"/>
+      <c r="AD8" s="84" t="s">
         <v>63</v>
       </c>
-      <c r="AE8" s="75"/>
-      <c r="AF8" s="75"/>
-      <c r="AG8" s="75"/>
-      <c r="AH8" s="75"/>
-      <c r="AI8" s="75"/>
-      <c r="AJ8" s="76"/>
+      <c r="AE8" s="85"/>
+      <c r="AF8" s="85"/>
+      <c r="AG8" s="85"/>
+      <c r="AH8" s="85"/>
+      <c r="AI8" s="85"/>
+      <c r="AJ8" s="86"/>
     </row>
     <row r="9" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="C9" s="1" t="s">
@@ -5147,34 +5144,34 @@
       <c r="C26" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D26" s="77" t="s">
+      <c r="D26" s="75" t="s">
         <v>130</v>
       </c>
-      <c r="E26" s="78"/>
-      <c r="F26" s="78"/>
-      <c r="G26" s="78"/>
-      <c r="H26" s="78"/>
-      <c r="I26" s="78"/>
-      <c r="J26" s="78"/>
-      <c r="K26" s="78"/>
-      <c r="L26" s="78"/>
-      <c r="M26" s="78"/>
-      <c r="N26" s="78"/>
-      <c r="O26" s="78"/>
-      <c r="P26" s="78"/>
-      <c r="Q26" s="78"/>
-      <c r="R26" s="78"/>
-      <c r="S26" s="78"/>
-      <c r="T26" s="78"/>
-      <c r="U26" s="78"/>
-      <c r="V26" s="78"/>
-      <c r="W26" s="78"/>
-      <c r="X26" s="78"/>
-      <c r="Y26" s="78"/>
-      <c r="Z26" s="78"/>
-      <c r="AA26" s="78"/>
-      <c r="AB26" s="78"/>
-      <c r="AC26" s="79"/>
+      <c r="E26" s="76"/>
+      <c r="F26" s="76"/>
+      <c r="G26" s="76"/>
+      <c r="H26" s="76"/>
+      <c r="I26" s="76"/>
+      <c r="J26" s="76"/>
+      <c r="K26" s="76"/>
+      <c r="L26" s="76"/>
+      <c r="M26" s="76"/>
+      <c r="N26" s="76"/>
+      <c r="O26" s="76"/>
+      <c r="P26" s="76"/>
+      <c r="Q26" s="76"/>
+      <c r="R26" s="76"/>
+      <c r="S26" s="76"/>
+      <c r="T26" s="76"/>
+      <c r="U26" s="76"/>
+      <c r="V26" s="76"/>
+      <c r="W26" s="76"/>
+      <c r="X26" s="76"/>
+      <c r="Y26" s="76"/>
+      <c r="Z26" s="76"/>
+      <c r="AA26" s="76"/>
+      <c r="AB26" s="76"/>
+      <c r="AC26" s="77"/>
       <c r="AD26" s="8">
         <v>9.8199999999999985</v>
       </c>
@@ -5312,65 +5309,65 @@
       <c r="C29" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D29" s="80" t="s">
+      <c r="D29" s="78" t="s">
         <v>140</v>
       </c>
-      <c r="E29" s="81"/>
-      <c r="F29" s="81"/>
-      <c r="G29" s="81"/>
-      <c r="H29" s="81"/>
-      <c r="I29" s="81"/>
-      <c r="J29" s="81"/>
-      <c r="K29" s="81"/>
-      <c r="L29" s="81"/>
-      <c r="M29" s="81"/>
-      <c r="N29" s="81"/>
-      <c r="O29" s="81"/>
-      <c r="P29" s="81"/>
-      <c r="Q29" s="82"/>
-      <c r="R29" s="80" t="s">
+      <c r="E29" s="79"/>
+      <c r="F29" s="79"/>
+      <c r="G29" s="79"/>
+      <c r="H29" s="79"/>
+      <c r="I29" s="79"/>
+      <c r="J29" s="79"/>
+      <c r="K29" s="79"/>
+      <c r="L29" s="79"/>
+      <c r="M29" s="79"/>
+      <c r="N29" s="79"/>
+      <c r="O29" s="79"/>
+      <c r="P29" s="79"/>
+      <c r="Q29" s="80"/>
+      <c r="R29" s="78" t="s">
         <v>162</v>
       </c>
-      <c r="S29" s="81"/>
-      <c r="T29" s="81"/>
-      <c r="U29" s="81"/>
-      <c r="V29" s="81"/>
-      <c r="W29" s="81"/>
-      <c r="X29" s="81"/>
-      <c r="Y29" s="81"/>
-      <c r="Z29" s="81"/>
-      <c r="AA29" s="81"/>
-      <c r="AB29" s="81"/>
-      <c r="AC29" s="81"/>
-      <c r="AD29" s="81"/>
-      <c r="AE29" s="81"/>
-      <c r="AF29" s="81"/>
-      <c r="AG29" s="81"/>
-      <c r="AH29" s="81"/>
-      <c r="AI29" s="81"/>
-      <c r="AJ29" s="82"/>
+      <c r="S29" s="79"/>
+      <c r="T29" s="79"/>
+      <c r="U29" s="79"/>
+      <c r="V29" s="79"/>
+      <c r="W29" s="79"/>
+      <c r="X29" s="79"/>
+      <c r="Y29" s="79"/>
+      <c r="Z29" s="79"/>
+      <c r="AA29" s="79"/>
+      <c r="AB29" s="79"/>
+      <c r="AC29" s="79"/>
+      <c r="AD29" s="79"/>
+      <c r="AE29" s="79"/>
+      <c r="AF29" s="79"/>
+      <c r="AG29" s="79"/>
+      <c r="AH29" s="79"/>
+      <c r="AI29" s="79"/>
+      <c r="AJ29" s="80"/>
     </row>
     <row r="30" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="B30" s="21"/>
       <c r="C30" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D30" s="80" t="s">
+      <c r="D30" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="E30" s="81"/>
-      <c r="F30" s="81"/>
-      <c r="G30" s="81"/>
-      <c r="H30" s="81"/>
-      <c r="I30" s="81"/>
-      <c r="J30" s="81"/>
-      <c r="K30" s="81"/>
-      <c r="L30" s="81"/>
-      <c r="M30" s="81"/>
-      <c r="N30" s="81"/>
-      <c r="O30" s="81"/>
-      <c r="P30" s="81"/>
-      <c r="Q30" s="82"/>
+      <c r="E30" s="79"/>
+      <c r="F30" s="79"/>
+      <c r="G30" s="79"/>
+      <c r="H30" s="79"/>
+      <c r="I30" s="79"/>
+      <c r="J30" s="79"/>
+      <c r="K30" s="79"/>
+      <c r="L30" s="79"/>
+      <c r="M30" s="79"/>
+      <c r="N30" s="79"/>
+      <c r="O30" s="79"/>
+      <c r="P30" s="79"/>
+      <c r="Q30" s="80"/>
       <c r="R30" s="47">
         <v>100</v>
       </c>
@@ -5434,22 +5431,22 @@
       <c r="C31" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D31" s="80" t="s">
+      <c r="D31" s="78" t="s">
         <v>131</v>
       </c>
-      <c r="E31" s="81"/>
-      <c r="F31" s="81"/>
-      <c r="G31" s="81"/>
-      <c r="H31" s="81"/>
-      <c r="I31" s="81"/>
-      <c r="J31" s="81"/>
-      <c r="K31" s="81"/>
-      <c r="L31" s="81"/>
-      <c r="M31" s="81"/>
-      <c r="N31" s="81"/>
-      <c r="O31" s="81"/>
-      <c r="P31" s="81"/>
-      <c r="Q31" s="82"/>
+      <c r="E31" s="79"/>
+      <c r="F31" s="79"/>
+      <c r="G31" s="79"/>
+      <c r="H31" s="79"/>
+      <c r="I31" s="79"/>
+      <c r="J31" s="79"/>
+      <c r="K31" s="79"/>
+      <c r="L31" s="79"/>
+      <c r="M31" s="79"/>
+      <c r="N31" s="79"/>
+      <c r="O31" s="79"/>
+      <c r="P31" s="79"/>
+      <c r="Q31" s="80"/>
       <c r="R31" s="47">
         <v>0.01</v>
       </c>
@@ -6001,23 +5998,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="D26:AC26"/>
-    <mergeCell ref="D31:Q31"/>
-    <mergeCell ref="D30:Q30"/>
-    <mergeCell ref="D29:Q29"/>
-    <mergeCell ref="R29:AJ29"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="I7:Q7"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="I8:Q8"/>
+    <mergeCell ref="R8:U8"/>
+    <mergeCell ref="R7:U7"/>
     <mergeCell ref="V7:Y7"/>
     <mergeCell ref="V8:Y8"/>
     <mergeCell ref="Z7:AC7"/>
     <mergeCell ref="Z8:AC8"/>
     <mergeCell ref="AD7:AJ7"/>
     <mergeCell ref="AD8:AJ8"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="I7:Q7"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="I8:Q8"/>
-    <mergeCell ref="R8:U8"/>
-    <mergeCell ref="R7:U7"/>
+    <mergeCell ref="D26:AC26"/>
+    <mergeCell ref="D31:Q31"/>
+    <mergeCell ref="D30:Q30"/>
+    <mergeCell ref="D29:Q29"/>
+    <mergeCell ref="R29:AJ29"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15475,7 +15472,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC155531-539F-473A-BEFE-FAB0C4C3EE43}">
   <dimension ref="B4:AE39"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D1" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="D4" workbookViewId="0">
       <selection activeCell="T42" sqref="T42"/>
     </sheetView>
   </sheetViews>
@@ -18567,12 +18564,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{946DA809-6F7B-4F40-B49B-27E3855F241E}">
   <dimension ref="A1:Y25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.4140625" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.83203125" bestFit="1" customWidth="1"/>
@@ -18590,1373 +18590,1373 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="85"/>
-      <c r="B1" s="85" t="s">
+      <c r="A1" s="72"/>
+      <c r="B1" s="72" t="s">
         <v>168</v>
       </c>
-      <c r="C1" s="85" t="s">
+      <c r="C1" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="D1" s="85" t="s">
+      <c r="D1" s="72" t="s">
         <v>170</v>
       </c>
-      <c r="E1" s="85" t="s">
+      <c r="E1" s="72" t="s">
         <v>171</v>
       </c>
-      <c r="F1" s="85" t="s">
+      <c r="F1" s="72" t="s">
         <v>172</v>
       </c>
-      <c r="G1" s="85" t="s">
+      <c r="G1" s="72" t="s">
         <v>173</v>
       </c>
-      <c r="H1" s="85" t="s">
+      <c r="H1" s="72" t="s">
         <v>174</v>
       </c>
-      <c r="I1" s="85" t="s">
+      <c r="I1" s="72" t="s">
         <v>175</v>
       </c>
-      <c r="J1" s="85" t="s">
+      <c r="J1" s="72" t="s">
         <v>176</v>
       </c>
-      <c r="K1" s="85" t="s">
+      <c r="K1" s="72" t="s">
         <v>177</v>
       </c>
-      <c r="L1" s="85" t="s">
+      <c r="L1" s="72" t="s">
         <v>178</v>
       </c>
-      <c r="M1" s="85" t="s">
+      <c r="M1" s="72" t="s">
         <v>179</v>
       </c>
-      <c r="N1" s="85" t="s">
+      <c r="N1" s="72" t="s">
         <v>180</v>
       </c>
-      <c r="O1" s="85" t="s">
+      <c r="O1" s="72" t="s">
         <v>181</v>
       </c>
-      <c r="P1" s="85" t="s">
+      <c r="P1" s="72" t="s">
         <v>182</v>
       </c>
-      <c r="Q1" s="85" t="s">
+      <c r="Q1" s="72" t="s">
         <v>183</v>
       </c>
-      <c r="R1" s="85" t="s">
+      <c r="R1" s="72" t="s">
         <v>184</v>
       </c>
-      <c r="S1" s="85" t="s">
+      <c r="S1" s="72" t="s">
         <v>185</v>
       </c>
-      <c r="T1" s="85" t="s">
+      <c r="T1" s="72" t="s">
         <v>186</v>
       </c>
-      <c r="U1" s="85" t="s">
+      <c r="U1" s="72" t="s">
         <v>187</v>
       </c>
-      <c r="V1" s="85" t="s">
+      <c r="V1" s="72" t="s">
         <v>188</v>
       </c>
-      <c r="W1" s="85" t="s">
+      <c r="W1" s="72" t="s">
         <v>189</v>
       </c>
-      <c r="X1" s="85" t="s">
+      <c r="X1" s="72" t="s">
         <v>190</v>
       </c>
-      <c r="Y1" s="85" t="s">
+      <c r="Y1" s="72" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="83" t="s">
+      <c r="A2" t="s">
         <v>168</v>
       </c>
-      <c r="B2" s="86">
+      <c r="B2" s="73">
         <v>1</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="86"/>
-      <c r="N2" s="86"/>
-      <c r="O2" s="86"/>
-      <c r="P2" s="86"/>
-      <c r="Q2" s="86"/>
-      <c r="R2" s="86"/>
-      <c r="S2" s="86"/>
-      <c r="T2" s="86"/>
-      <c r="U2" s="86"/>
-      <c r="V2" s="86"/>
-      <c r="W2" s="86"/>
-      <c r="X2" s="86"/>
-      <c r="Y2" s="86"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="73"/>
+      <c r="M2" s="73"/>
+      <c r="N2" s="73"/>
+      <c r="O2" s="73"/>
+      <c r="P2" s="73"/>
+      <c r="Q2" s="73"/>
+      <c r="R2" s="73"/>
+      <c r="S2" s="73"/>
+      <c r="T2" s="73"/>
+      <c r="U2" s="73"/>
+      <c r="V2" s="73"/>
+      <c r="W2" s="73"/>
+      <c r="X2" s="73"/>
+      <c r="Y2" s="73"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="83" t="s">
+      <c r="A3" t="s">
         <v>169</v>
       </c>
-      <c r="B3" s="86">
+      <c r="B3" s="73">
         <v>0.54532269214902873</v>
       </c>
-      <c r="C3" s="86">
+      <c r="C3" s="73">
         <v>1</v>
       </c>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="86"/>
-      <c r="J3" s="86"/>
-      <c r="K3" s="86"/>
-      <c r="L3" s="86"/>
-      <c r="M3" s="86"/>
-      <c r="N3" s="86"/>
-      <c r="O3" s="86"/>
-      <c r="P3" s="86"/>
-      <c r="Q3" s="86"/>
-      <c r="R3" s="86"/>
-      <c r="S3" s="86"/>
-      <c r="T3" s="86"/>
-      <c r="U3" s="86"/>
-      <c r="V3" s="86"/>
-      <c r="W3" s="86"/>
-      <c r="X3" s="86"/>
-      <c r="Y3" s="86"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="73"/>
+      <c r="L3" s="73"/>
+      <c r="M3" s="73"/>
+      <c r="N3" s="73"/>
+      <c r="O3" s="73"/>
+      <c r="P3" s="73"/>
+      <c r="Q3" s="73"/>
+      <c r="R3" s="73"/>
+      <c r="S3" s="73"/>
+      <c r="T3" s="73"/>
+      <c r="U3" s="73"/>
+      <c r="V3" s="73"/>
+      <c r="W3" s="73"/>
+      <c r="X3" s="73"/>
+      <c r="Y3" s="73"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="83" t="s">
+      <c r="A4" t="s">
         <v>170</v>
       </c>
-      <c r="B4" s="86">
+      <c r="B4" s="73">
         <v>-0.5693038369307919</v>
       </c>
-      <c r="C4" s="86">
+      <c r="C4" s="73">
         <v>-0.99796012768573961</v>
       </c>
-      <c r="D4" s="86">
+      <c r="D4" s="73">
         <v>1</v>
       </c>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
-      <c r="G4" s="86"/>
-      <c r="H4" s="86"/>
-      <c r="I4" s="86"/>
-      <c r="J4" s="86"/>
-      <c r="K4" s="86"/>
-      <c r="L4" s="86"/>
-      <c r="M4" s="86"/>
-      <c r="N4" s="86"/>
-      <c r="O4" s="86"/>
-      <c r="P4" s="86"/>
-      <c r="Q4" s="86"/>
-      <c r="R4" s="86"/>
-      <c r="S4" s="86"/>
-      <c r="T4" s="86"/>
-      <c r="U4" s="86"/>
-      <c r="V4" s="86"/>
-      <c r="W4" s="86"/>
-      <c r="X4" s="86"/>
-      <c r="Y4" s="86"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="73"/>
+      <c r="L4" s="73"/>
+      <c r="M4" s="73"/>
+      <c r="N4" s="73"/>
+      <c r="O4" s="73"/>
+      <c r="P4" s="73"/>
+      <c r="Q4" s="73"/>
+      <c r="R4" s="73"/>
+      <c r="S4" s="73"/>
+      <c r="T4" s="73"/>
+      <c r="U4" s="73"/>
+      <c r="V4" s="73"/>
+      <c r="W4" s="73"/>
+      <c r="X4" s="73"/>
+      <c r="Y4" s="73"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="83" t="s">
+      <c r="A5" t="s">
         <v>171</v>
       </c>
-      <c r="B5" s="86">
+      <c r="B5" s="73">
         <v>0.37186951414850039</v>
       </c>
-      <c r="C5" s="86">
+      <c r="C5" s="73">
         <v>0.78685883447847571</v>
       </c>
-      <c r="D5" s="86">
+      <c r="D5" s="73">
         <v>-0.78525374292679184</v>
       </c>
-      <c r="E5" s="86">
+      <c r="E5" s="73">
         <v>1</v>
       </c>
-      <c r="F5" s="86"/>
-      <c r="G5" s="86"/>
-      <c r="H5" s="86"/>
-      <c r="I5" s="86"/>
-      <c r="J5" s="86"/>
-      <c r="K5" s="86"/>
-      <c r="L5" s="86"/>
-      <c r="M5" s="86"/>
-      <c r="N5" s="86"/>
-      <c r="O5" s="86"/>
-      <c r="P5" s="86"/>
-      <c r="Q5" s="86"/>
-      <c r="R5" s="86"/>
-      <c r="S5" s="86"/>
-      <c r="T5" s="86"/>
-      <c r="U5" s="86"/>
-      <c r="V5" s="86"/>
-      <c r="W5" s="86"/>
-      <c r="X5" s="86"/>
-      <c r="Y5" s="86"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="73"/>
+      <c r="K5" s="73"/>
+      <c r="L5" s="73"/>
+      <c r="M5" s="73"/>
+      <c r="N5" s="73"/>
+      <c r="O5" s="73"/>
+      <c r="P5" s="73"/>
+      <c r="Q5" s="73"/>
+      <c r="R5" s="73"/>
+      <c r="S5" s="73"/>
+      <c r="T5" s="73"/>
+      <c r="U5" s="73"/>
+      <c r="V5" s="73"/>
+      <c r="W5" s="73"/>
+      <c r="X5" s="73"/>
+      <c r="Y5" s="73"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="83" t="s">
+      <c r="A6" t="s">
         <v>172</v>
       </c>
-      <c r="B6" s="86">
+      <c r="B6" s="73">
         <v>-0.52142976010762865</v>
       </c>
-      <c r="C6" s="86">
+      <c r="C6" s="73">
         <v>-0.80214333130506021</v>
       </c>
-      <c r="D6" s="86">
+      <c r="D6" s="73">
         <v>0.80050706133146232</v>
       </c>
-      <c r="E6" s="86">
+      <c r="E6" s="73">
         <v>-0.81378476241257014</v>
       </c>
-      <c r="F6" s="86">
+      <c r="F6" s="73">
         <v>1</v>
       </c>
-      <c r="G6" s="86"/>
-      <c r="H6" s="86"/>
-      <c r="I6" s="86"/>
-      <c r="J6" s="86"/>
-      <c r="K6" s="86"/>
-      <c r="L6" s="86"/>
-      <c r="M6" s="86"/>
-      <c r="N6" s="86"/>
-      <c r="O6" s="86"/>
-      <c r="P6" s="86"/>
-      <c r="Q6" s="86"/>
-      <c r="R6" s="86"/>
-      <c r="S6" s="86"/>
-      <c r="T6" s="86"/>
-      <c r="U6" s="86"/>
-      <c r="V6" s="86"/>
-      <c r="W6" s="86"/>
-      <c r="X6" s="86"/>
-      <c r="Y6" s="86"/>
+      <c r="G6" s="73"/>
+      <c r="H6" s="73"/>
+      <c r="I6" s="73"/>
+      <c r="J6" s="73"/>
+      <c r="K6" s="73"/>
+      <c r="L6" s="73"/>
+      <c r="M6" s="73"/>
+      <c r="N6" s="73"/>
+      <c r="O6" s="73"/>
+      <c r="P6" s="73"/>
+      <c r="Q6" s="73"/>
+      <c r="R6" s="73"/>
+      <c r="S6" s="73"/>
+      <c r="T6" s="73"/>
+      <c r="U6" s="73"/>
+      <c r="V6" s="73"/>
+      <c r="W6" s="73"/>
+      <c r="X6" s="73"/>
+      <c r="Y6" s="73"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="83" t="s">
+      <c r="A7" t="s">
         <v>173</v>
       </c>
-      <c r="B7" s="86">
+      <c r="B7" s="73">
         <v>-0.40937219968250366</v>
       </c>
-      <c r="C7" s="86">
+      <c r="C7" s="73">
         <v>-0.24062558079337174</v>
       </c>
-      <c r="D7" s="86">
+      <c r="D7" s="73">
         <v>0.24013473533300858</v>
       </c>
-      <c r="E7" s="86">
+      <c r="E7" s="73">
         <v>-0.17615657920993991</v>
       </c>
-      <c r="F7" s="86">
+      <c r="F7" s="73">
         <v>0.21844348946250985</v>
       </c>
-      <c r="G7" s="86">
+      <c r="G7" s="73">
         <v>1</v>
       </c>
-      <c r="H7" s="86"/>
-      <c r="I7" s="86"/>
-      <c r="J7" s="86"/>
-      <c r="K7" s="86"/>
-      <c r="L7" s="86"/>
-      <c r="M7" s="86"/>
-      <c r="N7" s="86"/>
-      <c r="O7" s="86"/>
-      <c r="P7" s="86"/>
-      <c r="Q7" s="86"/>
-      <c r="R7" s="86"/>
-      <c r="S7" s="86"/>
-      <c r="T7" s="86"/>
-      <c r="U7" s="86"/>
-      <c r="V7" s="86"/>
-      <c r="W7" s="86"/>
-      <c r="X7" s="86"/>
-      <c r="Y7" s="86"/>
+      <c r="H7" s="73"/>
+      <c r="I7" s="73"/>
+      <c r="J7" s="73"/>
+      <c r="K7" s="73"/>
+      <c r="L7" s="73"/>
+      <c r="M7" s="73"/>
+      <c r="N7" s="73"/>
+      <c r="O7" s="73"/>
+      <c r="P7" s="73"/>
+      <c r="Q7" s="73"/>
+      <c r="R7" s="73"/>
+      <c r="S7" s="73"/>
+      <c r="T7" s="73"/>
+      <c r="U7" s="73"/>
+      <c r="V7" s="73"/>
+      <c r="W7" s="73"/>
+      <c r="X7" s="73"/>
+      <c r="Y7" s="73"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="83" t="s">
+      <c r="A8" t="s">
         <v>174</v>
       </c>
-      <c r="B8" s="86">
+      <c r="B8" s="73">
         <v>0.2064701282579329</v>
       </c>
-      <c r="C8" s="86">
+      <c r="C8" s="73">
         <v>0.13363062095621231</v>
       </c>
-      <c r="D8" s="86">
+      <c r="D8" s="73">
         <v>-0.13335803155218626</v>
       </c>
-      <c r="E8" s="86">
+      <c r="E8" s="73">
         <v>9.7827974015615812E-2</v>
       </c>
-      <c r="F8" s="86">
+      <c r="F8" s="73">
         <v>-0.1213118698538683</v>
       </c>
-      <c r="G8" s="86">
+      <c r="G8" s="73">
         <v>-0.59150144445301611</v>
       </c>
-      <c r="H8" s="86">
+      <c r="H8" s="73">
         <v>1</v>
       </c>
-      <c r="I8" s="86"/>
-      <c r="J8" s="86"/>
-      <c r="K8" s="86"/>
-      <c r="L8" s="86"/>
-      <c r="M8" s="86"/>
-      <c r="N8" s="86"/>
-      <c r="O8" s="86"/>
-      <c r="P8" s="86"/>
-      <c r="Q8" s="86"/>
-      <c r="R8" s="86"/>
-      <c r="S8" s="86"/>
-      <c r="T8" s="86"/>
-      <c r="U8" s="86"/>
-      <c r="V8" s="86"/>
-      <c r="W8" s="86"/>
-      <c r="X8" s="86"/>
-      <c r="Y8" s="86"/>
+      <c r="I8" s="73"/>
+      <c r="J8" s="73"/>
+      <c r="K8" s="73"/>
+      <c r="L8" s="73"/>
+      <c r="M8" s="73"/>
+      <c r="N8" s="73"/>
+      <c r="O8" s="73"/>
+      <c r="P8" s="73"/>
+      <c r="Q8" s="73"/>
+      <c r="R8" s="73"/>
+      <c r="S8" s="73"/>
+      <c r="T8" s="73"/>
+      <c r="U8" s="73"/>
+      <c r="V8" s="73"/>
+      <c r="W8" s="73"/>
+      <c r="X8" s="73"/>
+      <c r="Y8" s="73"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="83" t="s">
+      <c r="A9" t="s">
         <v>175</v>
       </c>
-      <c r="B9" s="86">
+      <c r="B9" s="73">
         <v>0.2064701282579329</v>
       </c>
-      <c r="C9" s="86">
+      <c r="C9" s="73">
         <v>0.13363062095621234</v>
       </c>
-      <c r="D9" s="86">
+      <c r="D9" s="73">
         <v>-0.13335803155218626</v>
       </c>
-      <c r="E9" s="86">
+      <c r="E9" s="73">
         <v>9.7827974015615812E-2</v>
       </c>
-      <c r="F9" s="86">
+      <c r="F9" s="73">
         <v>-0.1213118698538683</v>
       </c>
-      <c r="G9" s="86">
+      <c r="G9" s="73">
         <v>-0.59150144445301611</v>
       </c>
-      <c r="H9" s="86">
+      <c r="H9" s="73">
         <v>-3.1250000000000097E-2</v>
       </c>
-      <c r="I9" s="86">
+      <c r="I9" s="73">
         <v>1</v>
       </c>
-      <c r="J9" s="86"/>
-      <c r="K9" s="86"/>
-      <c r="L9" s="86"/>
-      <c r="M9" s="86"/>
-      <c r="N9" s="86"/>
-      <c r="O9" s="86"/>
-      <c r="P9" s="86"/>
-      <c r="Q9" s="86"/>
-      <c r="R9" s="86"/>
-      <c r="S9" s="86"/>
-      <c r="T9" s="86"/>
-      <c r="U9" s="86"/>
-      <c r="V9" s="86"/>
-      <c r="W9" s="86"/>
-      <c r="X9" s="86"/>
-      <c r="Y9" s="86"/>
+      <c r="J9" s="73"/>
+      <c r="K9" s="73"/>
+      <c r="L9" s="73"/>
+      <c r="M9" s="73"/>
+      <c r="N9" s="73"/>
+      <c r="O9" s="73"/>
+      <c r="P9" s="73"/>
+      <c r="Q9" s="73"/>
+      <c r="R9" s="73"/>
+      <c r="S9" s="73"/>
+      <c r="T9" s="73"/>
+      <c r="U9" s="73"/>
+      <c r="V9" s="73"/>
+      <c r="W9" s="73"/>
+      <c r="X9" s="73"/>
+      <c r="Y9" s="73"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="83" t="s">
+      <c r="A10" t="s">
         <v>176</v>
       </c>
-      <c r="B10" s="86">
+      <c r="B10" s="73">
         <v>4.7941143432472522E-2</v>
       </c>
-      <c r="C10" s="86">
+      <c r="C10" s="73">
         <v>0.1689159811730441</v>
       </c>
-      <c r="D10" s="86">
+      <c r="D10" s="73">
         <v>-0.16857141413961296</v>
       </c>
-      <c r="E10" s="86">
+      <c r="E10" s="73">
         <v>0.15141990995385896</v>
       </c>
-      <c r="F10" s="86">
+      <c r="F10" s="73">
         <v>-0.12657001882882701</v>
       </c>
-      <c r="G10" s="86">
+      <c r="G10" s="73">
         <v>-4.0645506075046016E-2</v>
       </c>
-      <c r="H10" s="86">
+      <c r="H10" s="73">
         <v>2.2572347453581727E-2</v>
       </c>
-      <c r="I10" s="86">
+      <c r="I10" s="73">
         <v>2.2572347453581727E-2</v>
       </c>
-      <c r="J10" s="86">
+      <c r="J10" s="73">
         <v>1</v>
       </c>
-      <c r="K10" s="86"/>
-      <c r="L10" s="86"/>
-      <c r="M10" s="86"/>
-      <c r="N10" s="86"/>
-      <c r="O10" s="86"/>
-      <c r="P10" s="86"/>
-      <c r="Q10" s="86"/>
-      <c r="R10" s="86"/>
-      <c r="S10" s="86"/>
-      <c r="T10" s="86"/>
-      <c r="U10" s="86"/>
-      <c r="V10" s="86"/>
-      <c r="W10" s="86"/>
-      <c r="X10" s="86"/>
-      <c r="Y10" s="86"/>
+      <c r="K10" s="73"/>
+      <c r="L10" s="73"/>
+      <c r="M10" s="73"/>
+      <c r="N10" s="73"/>
+      <c r="O10" s="73"/>
+      <c r="P10" s="73"/>
+      <c r="Q10" s="73"/>
+      <c r="R10" s="73"/>
+      <c r="S10" s="73"/>
+      <c r="T10" s="73"/>
+      <c r="U10" s="73"/>
+      <c r="V10" s="73"/>
+      <c r="W10" s="73"/>
+      <c r="X10" s="73"/>
+      <c r="Y10" s="73"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="83" t="s">
+      <c r="A11" t="s">
         <v>177</v>
       </c>
-      <c r="B11" s="86">
+      <c r="B11" s="73">
         <v>-0.42354601289696908</v>
       </c>
-      <c r="C11" s="86">
+      <c r="C11" s="73">
         <v>-0.46770717334674256</v>
       </c>
-      <c r="D11" s="86">
+      <c r="D11" s="73">
         <v>0.46675311043265155</v>
       </c>
-      <c r="E11" s="86">
+      <c r="E11" s="73">
         <v>-0.41926274578121053</v>
       </c>
-      <c r="F11" s="86">
+      <c r="F11" s="73">
         <v>0.35045651291117474</v>
       </c>
-      <c r="G11" s="86">
+      <c r="G11" s="73">
         <v>0.11254231022778623</v>
       </c>
-      <c r="H11" s="86">
+      <c r="H11" s="73">
         <v>-6.2500000000000042E-2</v>
       </c>
-      <c r="I11" s="86">
+      <c r="I11" s="73">
         <v>-6.2500000000000042E-2</v>
       </c>
-      <c r="J11" s="86">
+      <c r="J11" s="73">
         <v>-0.7674598134217786</v>
       </c>
-      <c r="K11" s="86">
+      <c r="K11" s="73">
         <v>1</v>
       </c>
-      <c r="L11" s="86"/>
-      <c r="M11" s="86"/>
-      <c r="N11" s="86"/>
-      <c r="O11" s="86"/>
-      <c r="P11" s="86"/>
-      <c r="Q11" s="86"/>
-      <c r="R11" s="86"/>
-      <c r="S11" s="86"/>
-      <c r="T11" s="86"/>
-      <c r="U11" s="86"/>
-      <c r="V11" s="86"/>
-      <c r="W11" s="86"/>
-      <c r="X11" s="86"/>
-      <c r="Y11" s="86"/>
+      <c r="L11" s="73"/>
+      <c r="M11" s="73"/>
+      <c r="N11" s="73"/>
+      <c r="O11" s="73"/>
+      <c r="P11" s="73"/>
+      <c r="Q11" s="73"/>
+      <c r="R11" s="73"/>
+      <c r="S11" s="73"/>
+      <c r="T11" s="73"/>
+      <c r="U11" s="73"/>
+      <c r="V11" s="73"/>
+      <c r="W11" s="73"/>
+      <c r="X11" s="73"/>
+      <c r="Y11" s="73"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="83" t="s">
+      <c r="A12" t="s">
         <v>178</v>
       </c>
-      <c r="B12" s="86">
+      <c r="B12" s="73">
         <v>-0.56094629067505208</v>
       </c>
-      <c r="C12" s="86">
+      <c r="C12" s="73">
         <v>-0.48279450151921821</v>
       </c>
-      <c r="D12" s="86">
+      <c r="D12" s="73">
         <v>0.481809662382092</v>
       </c>
-      <c r="E12" s="86">
+      <c r="E12" s="73">
         <v>-0.3534430028951282</v>
       </c>
-      <c r="F12" s="86">
+      <c r="F12" s="73">
         <v>0.43828804592365272</v>
       </c>
-      <c r="G12" s="86">
+      <c r="G12" s="73">
         <v>0.27591017991328259</v>
       </c>
-      <c r="H12" s="86">
+      <c r="H12" s="73">
         <v>-0.15322580645161285</v>
       </c>
-      <c r="I12" s="86">
+      <c r="I12" s="73">
         <v>-0.15322580645161291</v>
       </c>
-      <c r="J12" s="86">
+      <c r="J12" s="73">
         <v>-8.1551706929069462E-2</v>
       </c>
-      <c r="K12" s="86">
+      <c r="K12" s="73">
         <v>0.22580645161290325</v>
       </c>
-      <c r="L12" s="86">
+      <c r="L12" s="73">
         <v>1</v>
       </c>
-      <c r="M12" s="86"/>
-      <c r="N12" s="86"/>
-      <c r="O12" s="86"/>
-      <c r="P12" s="86"/>
-      <c r="Q12" s="86"/>
-      <c r="R12" s="86"/>
-      <c r="S12" s="86"/>
-      <c r="T12" s="86"/>
-      <c r="U12" s="86"/>
-      <c r="V12" s="86"/>
-      <c r="W12" s="86"/>
-      <c r="X12" s="86"/>
-      <c r="Y12" s="86"/>
+      <c r="M12" s="73"/>
+      <c r="N12" s="73"/>
+      <c r="O12" s="73"/>
+      <c r="P12" s="73"/>
+      <c r="Q12" s="73"/>
+      <c r="R12" s="73"/>
+      <c r="S12" s="73"/>
+      <c r="T12" s="73"/>
+      <c r="U12" s="73"/>
+      <c r="V12" s="73"/>
+      <c r="W12" s="73"/>
+      <c r="X12" s="73"/>
+      <c r="Y12" s="73"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="83" t="s">
+      <c r="A13" t="s">
         <v>179</v>
       </c>
-      <c r="B13" s="86">
+      <c r="B13" s="73">
         <v>5.4122225092713113E-3</v>
       </c>
-      <c r="C13" s="86">
+      <c r="C13" s="73">
         <v>0.22252462162536571</v>
       </c>
-      <c r="D13" s="86">
+      <c r="D13" s="73">
         <v>-0.22207069981047078</v>
       </c>
-      <c r="E13" s="86">
+      <c r="E13" s="73">
         <v>0.1629052738543682</v>
       </c>
-      <c r="F13" s="86">
+      <c r="F13" s="73">
         <v>-0.20201116888279116</v>
       </c>
-      <c r="G13" s="86">
+      <c r="G13" s="73">
         <v>9.3703953559000658E-2</v>
       </c>
-      <c r="H13" s="86">
+      <c r="H13" s="73">
         <v>-5.2038180890226576E-2</v>
       </c>
-      <c r="I13" s="86">
+      <c r="I13" s="73">
         <v>-5.2038180890226576E-2</v>
       </c>
-      <c r="J13" s="86">
+      <c r="J13" s="73">
         <v>3.7587964797009037E-2</v>
       </c>
-      <c r="K13" s="86">
+      <c r="K13" s="73">
         <v>-0.10407636178045325</v>
       </c>
-      <c r="L13" s="86">
+      <c r="L13" s="73">
         <v>-0.6983188145269128</v>
       </c>
-      <c r="M13" s="86">
+      <c r="M13" s="73">
         <v>1</v>
       </c>
-      <c r="N13" s="86"/>
-      <c r="O13" s="86"/>
-      <c r="P13" s="86"/>
-      <c r="Q13" s="86"/>
-      <c r="R13" s="86"/>
-      <c r="S13" s="86"/>
-      <c r="T13" s="86"/>
-      <c r="U13" s="86"/>
-      <c r="V13" s="86"/>
-      <c r="W13" s="86"/>
-      <c r="X13" s="86"/>
-      <c r="Y13" s="86"/>
+      <c r="N13" s="73"/>
+      <c r="O13" s="73"/>
+      <c r="P13" s="73"/>
+      <c r="Q13" s="73"/>
+      <c r="R13" s="73"/>
+      <c r="S13" s="73"/>
+      <c r="T13" s="73"/>
+      <c r="U13" s="73"/>
+      <c r="V13" s="73"/>
+      <c r="W13" s="73"/>
+      <c r="X13" s="73"/>
+      <c r="Y13" s="73"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="83" t="s">
+      <c r="A14" t="s">
         <v>180</v>
       </c>
-      <c r="B14" s="86">
+      <c r="B14" s="73">
         <v>6.8298341815840067E-15</v>
       </c>
-      <c r="C14" s="86">
+      <c r="C14" s="73">
         <v>1.0443996526137254E-16</v>
       </c>
-      <c r="D14" s="86">
+      <c r="D14" s="73">
         <v>-1.0422692106773353E-16</v>
       </c>
-      <c r="E14" s="86">
+      <c r="E14" s="73">
         <v>1.5603704304785335E-17</v>
       </c>
-      <c r="F14" s="86">
+      <c r="F14" s="73">
         <v>-1.6554503680555037E-16</v>
       </c>
-      <c r="G14" s="86">
+      <c r="G14" s="73">
         <v>2.9587283593366958E-16</v>
       </c>
-      <c r="H14" s="86">
+      <c r="H14" s="73">
         <v>-6.9781887052612257E-17</v>
       </c>
-      <c r="I14" s="86">
+      <c r="I14" s="73">
         <v>-6.9781887052612257E-17</v>
       </c>
-      <c r="J14" s="86">
+      <c r="J14" s="73">
         <v>-2.3690120647793115E-16</v>
       </c>
-      <c r="K14" s="86">
-        <v>0</v>
-      </c>
-      <c r="L14" s="86">
+      <c r="K14" s="73">
+        <v>0</v>
+      </c>
+      <c r="L14" s="73">
         <v>-2.9713577712725213E-16</v>
       </c>
-      <c r="M14" s="86">
+      <c r="M14" s="73">
         <v>1.3072760860698715E-16</v>
       </c>
-      <c r="N14" s="86">
+      <c r="N14" s="73">
         <v>1</v>
       </c>
-      <c r="O14" s="86"/>
-      <c r="P14" s="86"/>
-      <c r="Q14" s="86"/>
-      <c r="R14" s="86"/>
-      <c r="S14" s="86"/>
-      <c r="T14" s="86"/>
-      <c r="U14" s="86"/>
-      <c r="V14" s="86"/>
-      <c r="W14" s="86"/>
-      <c r="X14" s="86"/>
-      <c r="Y14" s="86"/>
+      <c r="O14" s="73"/>
+      <c r="P14" s="73"/>
+      <c r="Q14" s="73"/>
+      <c r="R14" s="73"/>
+      <c r="S14" s="73"/>
+      <c r="T14" s="73"/>
+      <c r="U14" s="73"/>
+      <c r="V14" s="73"/>
+      <c r="W14" s="73"/>
+      <c r="X14" s="73"/>
+      <c r="Y14" s="73"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="83" t="s">
+      <c r="A15" t="s">
         <v>181</v>
       </c>
-      <c r="B15" s="86" t="e">
+      <c r="B15" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="C15" s="86" t="e">
+      <c r="C15" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="D15" s="86" t="e">
+      <c r="D15" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="E15" s="86" t="e">
+      <c r="E15" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="F15" s="86" t="e">
+      <c r="F15" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="G15" s="86" t="e">
+      <c r="G15" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="H15" s="86" t="e">
+      <c r="H15" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="I15" s="86" t="e">
+      <c r="I15" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="J15" s="86" t="e">
+      <c r="J15" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="K15" s="86" t="e">
+      <c r="K15" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="L15" s="86" t="e">
+      <c r="L15" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="M15" s="86" t="e">
+      <c r="M15" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="N15" s="86" t="e">
+      <c r="N15" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="O15" s="86">
+      <c r="O15" s="73">
         <v>1</v>
       </c>
-      <c r="P15" s="86"/>
-      <c r="Q15" s="86"/>
-      <c r="R15" s="86"/>
-      <c r="S15" s="86"/>
-      <c r="T15" s="86"/>
-      <c r="U15" s="86"/>
-      <c r="V15" s="86"/>
-      <c r="W15" s="86"/>
-      <c r="X15" s="86"/>
-      <c r="Y15" s="86"/>
+      <c r="P15" s="73"/>
+      <c r="Q15" s="73"/>
+      <c r="R15" s="73"/>
+      <c r="S15" s="73"/>
+      <c r="T15" s="73"/>
+      <c r="U15" s="73"/>
+      <c r="V15" s="73"/>
+      <c r="W15" s="73"/>
+      <c r="X15" s="73"/>
+      <c r="Y15" s="73"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="83" t="s">
+      <c r="A16" t="s">
         <v>182</v>
       </c>
-      <c r="B16" s="86">
+      <c r="B16" s="73">
         <v>-0.63644724213007908</v>
       </c>
-      <c r="C16" s="86">
+      <c r="C16" s="73">
         <v>-0.64888568452304984</v>
       </c>
-      <c r="D16" s="86">
+      <c r="D16" s="73">
         <v>0.64756204058007127</v>
       </c>
-      <c r="E16" s="86">
+      <c r="E16" s="73">
         <v>-0.47503462477680736</v>
       </c>
-      <c r="F16" s="86">
+      <c r="F16" s="73">
         <v>0.58906809792264891</v>
       </c>
-      <c r="G16" s="86">
+      <c r="G16" s="73">
         <v>0.37082892492880132</v>
       </c>
-      <c r="H16" s="86">
+      <c r="H16" s="73">
         <v>-0.20593861776197844</v>
       </c>
-      <c r="I16" s="86">
+      <c r="I16" s="73">
         <v>-0.20593861776197844</v>
       </c>
-      <c r="J16" s="86">
+      <c r="J16" s="73">
         <v>-0.10960716207035329</v>
       </c>
-      <c r="K16" s="86">
+      <c r="K16" s="73">
         <v>0.30348848933344197</v>
       </c>
-      <c r="L16" s="86">
+      <c r="L16" s="73">
         <v>0.74403629643037428</v>
       </c>
-      <c r="M16" s="86">
+      <c r="M16" s="73">
         <v>-0.34293347338819458</v>
       </c>
-      <c r="N16" s="86">
+      <c r="N16" s="73">
         <v>-2.3598342282655199E-16</v>
       </c>
-      <c r="O16" s="86" t="e">
+      <c r="O16" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="P16" s="86">
+      <c r="P16" s="73">
         <v>1</v>
       </c>
-      <c r="Q16" s="86"/>
-      <c r="R16" s="86"/>
-      <c r="S16" s="86"/>
-      <c r="T16" s="86"/>
-      <c r="U16" s="86"/>
-      <c r="V16" s="86"/>
-      <c r="W16" s="86"/>
-      <c r="X16" s="86"/>
-      <c r="Y16" s="86"/>
+      <c r="Q16" s="73"/>
+      <c r="R16" s="73"/>
+      <c r="S16" s="73"/>
+      <c r="T16" s="73"/>
+      <c r="U16" s="73"/>
+      <c r="V16" s="73"/>
+      <c r="W16" s="73"/>
+      <c r="X16" s="73"/>
+      <c r="Y16" s="73"/>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="83" t="s">
+      <c r="A17" t="s">
         <v>183</v>
       </c>
-      <c r="B17" s="86">
+      <c r="B17" s="73">
         <v>-0.63090569434588195</v>
       </c>
-      <c r="C17" s="86">
+      <c r="C17" s="73">
         <v>-0.64323583518874972</v>
       </c>
-      <c r="D17" s="86">
+      <c r="D17" s="73">
         <v>0.64192371621700783</v>
       </c>
-      <c r="E17" s="86">
+      <c r="E17" s="73">
         <v>-0.47089849706960152</v>
       </c>
-      <c r="F17" s="86">
+      <c r="F17" s="73">
         <v>0.58393908046967202</v>
       </c>
-      <c r="G17" s="86">
+      <c r="G17" s="73">
         <v>0.3676001165198311</v>
       </c>
-      <c r="H17" s="86">
+      <c r="H17" s="73">
         <v>-0.20414550968420586</v>
       </c>
-      <c r="I17" s="86">
+      <c r="I17" s="73">
         <v>-0.20414550968420586</v>
       </c>
-      <c r="J17" s="86">
+      <c r="J17" s="73">
         <v>-0.10865281222657011</v>
       </c>
-      <c r="K17" s="86">
+      <c r="K17" s="73">
         <v>0.3008460142714614</v>
       </c>
-      <c r="L17" s="86">
+      <c r="L17" s="73">
         <v>0.73755797047197014</v>
       </c>
-      <c r="M17" s="86">
+      <c r="M17" s="73">
         <v>-0.339947550747975</v>
       </c>
-      <c r="N17" s="86">
+      <c r="N17" s="73">
         <v>-2.1497449050234554E-16</v>
       </c>
-      <c r="O17" s="86" t="e">
+      <c r="O17" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="P17" s="86">
+      <c r="P17" s="73">
         <v>0.99129299741224342</v>
       </c>
-      <c r="Q17" s="86">
+      <c r="Q17" s="73">
         <v>1</v>
       </c>
-      <c r="R17" s="86"/>
-      <c r="S17" s="86"/>
-      <c r="T17" s="86"/>
-      <c r="U17" s="86"/>
-      <c r="V17" s="86"/>
-      <c r="W17" s="86"/>
-      <c r="X17" s="86"/>
-      <c r="Y17" s="86"/>
+      <c r="R17" s="73"/>
+      <c r="S17" s="73"/>
+      <c r="T17" s="73"/>
+      <c r="U17" s="73"/>
+      <c r="V17" s="73"/>
+      <c r="W17" s="73"/>
+      <c r="X17" s="73"/>
+      <c r="Y17" s="73"/>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="83" t="s">
+      <c r="A18" t="s">
         <v>184</v>
       </c>
-      <c r="B18" s="86">
+      <c r="B18" s="73">
         <v>-0.26911365410861021</v>
       </c>
-      <c r="C18" s="86">
+      <c r="C18" s="73">
         <v>-0.30860669992418377</v>
       </c>
-      <c r="D18" s="86">
+      <c r="D18" s="73">
         <v>0.30752176228926043</v>
       </c>
-      <c r="E18" s="86">
+      <c r="E18" s="73">
         <v>6.976819652324362E-2</v>
       </c>
-      <c r="F18" s="86">
+      <c r="F18" s="73">
         <v>0.26379467179224692</v>
       </c>
-      <c r="G18" s="86" t="e">
+      <c r="G18" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="H18" s="86" t="e">
+      <c r="H18" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="I18" s="86" t="e">
+      <c r="I18" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="J18" s="86">
+      <c r="J18" s="73">
         <v>-3.9904344223381058E-2</v>
       </c>
-      <c r="K18" s="86">
+      <c r="K18" s="73">
         <v>0.11526067913468739</v>
       </c>
-      <c r="L18" s="86" t="e">
+      <c r="L18" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="M18" s="86" t="e">
+      <c r="M18" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="N18" s="86">
+      <c r="N18" s="73">
         <v>1.6764008022404885E-15</v>
       </c>
-      <c r="O18" s="86" t="e">
+      <c r="O18" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="P18" s="86" t="e">
+      <c r="P18" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="Q18" s="86">
-        <v>0</v>
-      </c>
-      <c r="R18" s="86">
+      <c r="Q18" s="73">
+        <v>0</v>
+      </c>
+      <c r="R18" s="73">
         <v>1</v>
       </c>
-      <c r="S18" s="86"/>
-      <c r="T18" s="86"/>
-      <c r="U18" s="86"/>
-      <c r="V18" s="86"/>
-      <c r="W18" s="86"/>
-      <c r="X18" s="86"/>
-      <c r="Y18" s="86"/>
+      <c r="S18" s="73"/>
+      <c r="T18" s="73"/>
+      <c r="U18" s="73"/>
+      <c r="V18" s="73"/>
+      <c r="W18" s="73"/>
+      <c r="X18" s="73"/>
+      <c r="Y18" s="73"/>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="83" t="s">
+      <c r="A19" t="s">
         <v>185</v>
       </c>
-      <c r="B19" s="86" t="e">
+      <c r="B19" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="C19" s="86" t="e">
+      <c r="C19" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="D19" s="86" t="e">
+      <c r="D19" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="E19" s="86" t="e">
+      <c r="E19" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="F19" s="86" t="e">
+      <c r="F19" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="G19" s="86" t="e">
+      <c r="G19" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="H19" s="86" t="e">
+      <c r="H19" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="I19" s="86" t="e">
+      <c r="I19" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="J19" s="86" t="e">
+      <c r="J19" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="K19" s="86" t="e">
+      <c r="K19" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="L19" s="86" t="e">
+      <c r="L19" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="M19" s="86" t="e">
+      <c r="M19" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="N19" s="86" t="e">
+      <c r="N19" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="O19" s="86" t="e">
+      <c r="O19" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="P19" s="86" t="e">
+      <c r="P19" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="Q19" s="86" t="e">
+      <c r="Q19" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="R19" s="86" t="e">
+      <c r="R19" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="S19" s="86">
+      <c r="S19" s="73">
         <v>1</v>
       </c>
-      <c r="T19" s="86"/>
-      <c r="U19" s="86"/>
-      <c r="V19" s="86"/>
-      <c r="W19" s="86"/>
-      <c r="X19" s="86"/>
-      <c r="Y19" s="86"/>
+      <c r="T19" s="73"/>
+      <c r="U19" s="73"/>
+      <c r="V19" s="73"/>
+      <c r="W19" s="73"/>
+      <c r="X19" s="73"/>
+      <c r="Y19" s="73"/>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="83" t="s">
+      <c r="A20" t="s">
         <v>186</v>
       </c>
-      <c r="B20" s="86" t="e">
+      <c r="B20" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="C20" s="86" t="e">
+      <c r="C20" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="D20" s="86" t="e">
+      <c r="D20" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="E20" s="86" t="e">
+      <c r="E20" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="F20" s="86" t="e">
+      <c r="F20" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="G20" s="86" t="e">
+      <c r="G20" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="H20" s="86" t="e">
+      <c r="H20" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="I20" s="86" t="e">
+      <c r="I20" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="J20" s="86" t="e">
+      <c r="J20" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="K20" s="86" t="e">
+      <c r="K20" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="L20" s="86" t="e">
+      <c r="L20" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="M20" s="86" t="e">
+      <c r="M20" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="N20" s="86" t="e">
+      <c r="N20" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="O20" s="86" t="e">
+      <c r="O20" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="P20" s="86" t="e">
+      <c r="P20" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="Q20" s="86" t="e">
+      <c r="Q20" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="R20" s="86" t="e">
+      <c r="R20" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="S20" s="86" t="e">
+      <c r="S20" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="T20" s="86">
+      <c r="T20" s="73">
         <v>1</v>
       </c>
-      <c r="U20" s="86"/>
-      <c r="V20" s="86"/>
-      <c r="W20" s="86"/>
-      <c r="X20" s="86"/>
-      <c r="Y20" s="86"/>
+      <c r="U20" s="73"/>
+      <c r="V20" s="73"/>
+      <c r="W20" s="73"/>
+      <c r="X20" s="73"/>
+      <c r="Y20" s="73"/>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="83" t="s">
+      <c r="A21" t="s">
         <v>187</v>
       </c>
-      <c r="B21" s="86">
+      <c r="B21" s="73">
         <v>-0.65684655212468779</v>
       </c>
-      <c r="C21" s="86">
+      <c r="C21" s="73">
         <v>-0.74501977471698688</v>
       </c>
-      <c r="D21" s="86">
+      <c r="D21" s="73">
         <v>0.74350002950496497</v>
       </c>
-      <c r="E21" s="86">
+      <c r="E21" s="73">
         <v>-0.54541223142273476</v>
       </c>
-      <c r="F21" s="86">
+      <c r="F21" s="73">
         <v>0.67634005815658671</v>
       </c>
-      <c r="G21" s="86">
+      <c r="G21" s="73">
         <v>0.30504180067972075</v>
       </c>
-      <c r="H21" s="86">
+      <c r="H21" s="73">
         <v>-0.15636742794798861</v>
       </c>
-      <c r="I21" s="86">
+      <c r="I21" s="73">
         <v>-0.15636742794798861</v>
       </c>
-      <c r="J21" s="86">
+      <c r="J21" s="73">
         <v>-0.12584574623964012</v>
       </c>
-      <c r="K21" s="86">
+      <c r="K21" s="73">
         <v>0.34845109292030901</v>
       </c>
-      <c r="L21" s="86">
+      <c r="L21" s="73">
         <v>0.76338890244138069</v>
       </c>
-      <c r="M21" s="86">
+      <c r="M21" s="73">
         <v>-0.38484971956554048</v>
       </c>
-      <c r="N21" s="86">
+      <c r="N21" s="73">
         <v>2.2613484572857596E-16</v>
       </c>
-      <c r="O21" s="86" t="e">
+      <c r="O21" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="P21" s="86">
+      <c r="P21" s="73">
         <v>0.78920382806196909</v>
       </c>
-      <c r="Q21" s="86">
+      <c r="Q21" s="73">
         <v>0.79023941466963321</v>
       </c>
-      <c r="R21" s="86">
+      <c r="R21" s="73">
         <v>0.86221131987965471</v>
       </c>
-      <c r="S21" s="86" t="e">
+      <c r="S21" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="T21" s="86" t="e">
+      <c r="T21" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="U21" s="86">
+      <c r="U21" s="73">
         <v>1</v>
       </c>
-      <c r="V21" s="86"/>
-      <c r="W21" s="86"/>
-      <c r="X21" s="86"/>
-      <c r="Y21" s="86"/>
+      <c r="V21" s="73"/>
+      <c r="W21" s="73"/>
+      <c r="X21" s="73"/>
+      <c r="Y21" s="73"/>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="83" t="s">
+      <c r="A22" t="s">
         <v>188</v>
       </c>
-      <c r="B22" s="86">
+      <c r="B22" s="73">
         <v>-0.6139086961176804</v>
       </c>
-      <c r="C22" s="86">
+      <c r="C22" s="73">
         <v>-0.5947704002421923</v>
       </c>
-      <c r="D22" s="86">
+      <c r="D22" s="73">
         <v>0.59355714456939646</v>
       </c>
-      <c r="E22" s="86">
+      <c r="E22" s="73">
         <v>-0.55235314072510733</v>
       </c>
-      <c r="F22" s="86">
+      <c r="F22" s="73">
         <v>0.46221314622956378</v>
       </c>
-      <c r="G22" s="86">
+      <c r="G22" s="73">
         <v>0.17095594914778819</v>
       </c>
-      <c r="H22" s="86">
+      <c r="H22" s="73">
         <v>-9.7651533876473781E-2</v>
       </c>
-      <c r="I22" s="86">
+      <c r="I22" s="73">
         <v>-0.12945252681650973</v>
       </c>
-      <c r="J22" s="86">
+      <c r="J22" s="73">
         <v>-0.16682497990664674</v>
       </c>
-      <c r="K22" s="86">
+      <c r="K22" s="73">
         <v>0.75679938754267162</v>
       </c>
-      <c r="L22" s="86">
+      <c r="L22" s="73">
         <v>0.28988744818847967</v>
       </c>
-      <c r="M22" s="86">
+      <c r="M22" s="73">
         <v>-0.12730765766412053</v>
       </c>
-      <c r="N22" s="86">
+      <c r="N22" s="73">
         <v>-5.1107312306118231E-16</v>
       </c>
-      <c r="O22" s="86" t="e">
+      <c r="O22" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="P22" s="86">
+      <c r="P22" s="73">
         <v>0.38961465936441286</v>
       </c>
-      <c r="Q22" s="86">
+      <c r="Q22" s="73">
         <v>0.38622228351709892</v>
       </c>
-      <c r="R22" s="86">
+      <c r="R22" s="73">
         <v>0.13174403224453668</v>
       </c>
-      <c r="S22" s="86" t="e">
+      <c r="S22" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="T22" s="86" t="e">
+      <c r="T22" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="U22" s="86">
+      <c r="U22" s="73">
         <v>0.44233475653467785</v>
       </c>
-      <c r="V22" s="86">
+      <c r="V22" s="73">
         <v>1</v>
       </c>
-      <c r="W22" s="86"/>
-      <c r="X22" s="86"/>
-      <c r="Y22" s="86"/>
+      <c r="W22" s="73"/>
+      <c r="X22" s="73"/>
+      <c r="Y22" s="73"/>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="83" t="s">
+      <c r="A23" t="s">
         <v>189</v>
       </c>
-      <c r="B23" s="86">
+      <c r="B23" s="73">
         <v>-0.21401478203302254</v>
       </c>
-      <c r="C23" s="86">
+      <c r="C23" s="73">
         <v>0.6198960282048539</v>
       </c>
-      <c r="D23" s="86">
+      <c r="D23" s="73">
         <v>-0.6186315194591987</v>
       </c>
-      <c r="E23" s="86">
+      <c r="E23" s="73">
         <v>0.48946860211463999</v>
       </c>
-      <c r="F23" s="86">
+      <c r="F23" s="73">
         <v>-0.48615421148870491</v>
       </c>
-      <c r="G23" s="86">
+      <c r="G23" s="73">
         <v>0.12338455418429231</v>
       </c>
-      <c r="H23" s="86">
+      <c r="H23" s="73">
         <v>-6.5234209302127172E-2</v>
       </c>
-      <c r="I23" s="86">
+      <c r="I23" s="73">
         <v>-6.5234209302127172E-2</v>
       </c>
-      <c r="J23" s="86">
+      <c r="J23" s="73">
         <v>8.9003793955071492E-2</v>
       </c>
-      <c r="K23" s="86">
+      <c r="K23" s="73">
         <v>-4.5466267089361322E-2</v>
       </c>
-      <c r="L23" s="86">
+      <c r="L23" s="73">
         <v>2.8057724431021706E-3</v>
       </c>
-      <c r="M23" s="86">
+      <c r="M23" s="73">
         <v>0.29692043293801551</v>
       </c>
-      <c r="N23" s="86">
+      <c r="N23" s="73">
         <v>-1.4953176328571059E-15</v>
       </c>
-      <c r="O23" s="86" t="e">
+      <c r="O23" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="P23" s="86">
+      <c r="P23" s="73">
         <v>-0.12444351312777445</v>
       </c>
-      <c r="Q23" s="86">
+      <c r="Q23" s="73">
         <v>-0.12335998313694138</v>
       </c>
-      <c r="R23" s="86">
+      <c r="R23" s="73">
         <v>-0.2483609982908293</v>
       </c>
-      <c r="S23" s="86" t="e">
+      <c r="S23" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="T23" s="86" t="e">
+      <c r="T23" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="U23" s="86">
+      <c r="U23" s="73">
         <v>-0.22700623618415558</v>
       </c>
-      <c r="V23" s="86">
+      <c r="V23" s="73">
         <v>-1.911066179871496E-2</v>
       </c>
-      <c r="W23" s="86">
+      <c r="W23" s="73">
         <v>1</v>
       </c>
-      <c r="X23" s="86"/>
-      <c r="Y23" s="86"/>
+      <c r="X23" s="73"/>
+      <c r="Y23" s="73"/>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="83" t="s">
+      <c r="A24" t="s">
         <v>190</v>
       </c>
-      <c r="B24" s="86">
+      <c r="B24" s="73">
         <v>0.88528380522770744</v>
       </c>
-      <c r="C24" s="86">
+      <c r="C24" s="73">
         <v>0.23877755083096783</v>
       </c>
-      <c r="D24" s="86">
+      <c r="D24" s="73">
         <v>-0.26368965366492136</v>
       </c>
-      <c r="E24" s="86">
+      <c r="E24" s="73">
         <v>0.12156889234959198</v>
       </c>
-      <c r="F24" s="86">
+      <c r="F24" s="73">
         <v>-0.28454014655997628</v>
       </c>
-      <c r="G24" s="86">
+      <c r="G24" s="73">
         <v>-0.49782758967774171</v>
       </c>
-      <c r="H24" s="86">
+      <c r="H24" s="73">
         <v>9.1766396712619255E-2</v>
       </c>
-      <c r="I24" s="86">
+      <c r="I24" s="73">
         <v>0.20604153224154134</v>
       </c>
-      <c r="J24" s="86">
+      <c r="J24" s="73">
         <v>2.501292668571123E-3</v>
       </c>
-      <c r="K24" s="86">
+      <c r="K24" s="73">
         <v>-0.24240180263710734</v>
       </c>
-      <c r="L24" s="86">
+      <c r="L24" s="73">
         <v>-0.44950454092705999</v>
       </c>
-      <c r="M24" s="86">
+      <c r="M24" s="73">
         <v>-9.4570075977804618E-2</v>
       </c>
-      <c r="N24" s="86">
+      <c r="N24" s="73">
         <v>-9.7431870026720007E-16</v>
       </c>
-      <c r="O24" s="86" t="e">
+      <c r="O24" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="P24" s="86">
+      <c r="P24" s="73">
         <v>-0.48523636547251753</v>
       </c>
-      <c r="Q24" s="86">
+      <c r="Q24" s="73">
         <v>-0.48101141118267471</v>
       </c>
-      <c r="R24" s="86">
+      <c r="R24" s="73">
         <v>-0.14641107432910491</v>
       </c>
-      <c r="S24" s="86" t="e">
+      <c r="S24" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="T24" s="86" t="e">
+      <c r="T24" s="73" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="U24" s="86">
+      <c r="U24" s="73">
         <v>-0.46861278010777019</v>
       </c>
-      <c r="V24" s="86">
+      <c r="V24" s="73">
         <v>-0.36164875740461316</v>
       </c>
-      <c r="W24" s="86">
+      <c r="W24" s="73">
         <v>-0.43432737670120619</v>
       </c>
-      <c r="X24" s="86">
+      <c r="X24" s="73">
         <v>1</v>
       </c>
-      <c r="Y24" s="86"/>
+      <c r="Y24" s="73"/>
     </row>
     <row r="25" spans="1:25" ht="18.5" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A25" s="84" t="s">
+      <c r="A25" s="71" t="s">
         <v>191</v>
       </c>
-      <c r="B25" s="87">
+      <c r="B25" s="74">
         <v>-0.53311575526124477</v>
       </c>
-      <c r="C25" s="87" t="e">
+      <c r="C25" s="74" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="D25" s="87" t="e">
+      <c r="D25" s="74" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="E25" s="87" t="e">
+      <c r="E25" s="74" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="F25" s="87" t="e">
+      <c r="F25" s="74" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="G25" s="87" t="e">
+      <c r="G25" s="74" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="H25" s="87" t="e">
+      <c r="H25" s="74" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="I25" s="87" t="e">
+      <c r="I25" s="74" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="J25" s="87">
+      <c r="J25" s="74">
         <v>-0.36806088975493934</v>
       </c>
-      <c r="K25" s="87">
+      <c r="K25" s="74">
         <v>0.66445163137920571</v>
       </c>
-      <c r="L25" s="87" t="e">
+      <c r="L25" s="74" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="M25" s="87" t="e">
+      <c r="M25" s="74" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="N25" s="87">
+      <c r="N25" s="74">
         <v>-2.0100642720231223E-16</v>
       </c>
-      <c r="O25" s="87" t="e">
+      <c r="O25" s="74" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="P25" s="87" t="e">
+      <c r="P25" s="74" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="Q25" s="87" t="e">
+      <c r="Q25" s="74" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="R25" s="87" t="e">
+      <c r="R25" s="74" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="S25" s="87" t="e">
+      <c r="S25" s="74" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="T25" s="87" t="e">
+      <c r="T25" s="74" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="U25" s="87" t="e">
+      <c r="U25" s="74" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="V25" s="87">
+      <c r="V25" s="74">
         <v>0.63089909132674227</v>
       </c>
-      <c r="W25" s="87">
+      <c r="W25" s="74">
         <v>0.59991265498140522</v>
       </c>
-      <c r="X25" s="87">
+      <c r="X25" s="74">
         <v>-0.53311575526124488</v>
       </c>
-      <c r="Y25" s="87">
+      <c r="Y25" s="74">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix xlsx data   ST target
</commit_message>
<xml_diff>
--- a/chapter2/input/chapter2_demo_data.xlsx
+++ b/chapter2/input/chapter2_demo_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\副業関連\独立\執筆\practical-mi-guide\chapter2\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53DC8A4E-C55B-42DE-B245-E77C8D95B7D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0EC40AA-0ABD-4ADF-9D92-A6D549873895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="2420" windowWidth="35850" windowHeight="17630" activeTab="6" xr2:uid="{AFFCA931-CB2A-4AED-B7E5-2638B5FCE6AD}"/>
+    <workbookView xWindow="590" yWindow="3490" windowWidth="30300" windowHeight="17850" activeTab="6" xr2:uid="{AFFCA931-CB2A-4AED-B7E5-2638B5FCE6AD}"/>
   </bookViews>
   <sheets>
     <sheet name="初期データ" sheetId="2" r:id="rId1"/>
@@ -450,10 +450,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>30－38</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>DP_031</t>
   </si>
   <si>
@@ -680,6 +676,10 @@
   </si>
   <si>
     <t>DP_test_09</t>
+  </si>
+  <si>
+    <t>32－38</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -1142,23 +1142,11 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1178,55 +1166,29 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="34">
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -2109,6 +2071,44 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -2241,33 +2241,33 @@
   <tableColumns count="29">
     <tableColumn id="1" xr3:uid="{82FD5B8D-2E76-4D53-95D8-6876F7437804}" name="サンプルID" dataDxfId="28"/>
     <tableColumn id="3" xr3:uid="{565DF522-859F-4F76-896F-52B5DB3706A9}" name="サンプル作成日" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{E9A22458-9FAB-4C13-9BE1-E66B79D90E8E}" name="担当者" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{614AD84F-0894-4343-A1D6-B518FAC6CDDC}" name="備考" dataDxfId="0"/>
-    <tableColumn id="6" xr3:uid="{3FE65FF5-2F1D-461D-9A27-9E364D47118F}" name="材料１" dataDxfId="26"/>
-    <tableColumn id="7" xr3:uid="{0319F8E7-300B-423E-9F06-BA16CF0DAB79}" name="材料２" dataDxfId="25"/>
-    <tableColumn id="8" xr3:uid="{7E73EAEC-77E2-41F2-B774-DAAA3A632F64}" name="材料３" dataDxfId="24"/>
-    <tableColumn id="9" xr3:uid="{2CAAD817-10C9-4A44-AFE0-171643F19D48}" name="材料４" dataDxfId="23"/>
-    <tableColumn id="10" xr3:uid="{4E0EEAC3-E19D-4FE7-933C-29E7C72E55D4}" name="材料５" dataDxfId="22"/>
-    <tableColumn id="11" xr3:uid="{DB55EB1E-83C3-46B1-8CAC-13E30A014C4C}" name="材料６" dataDxfId="21"/>
-    <tableColumn id="12" xr3:uid="{CC5EB82F-01B1-4A3B-AA90-23FF297DB203}" name="材料７" dataDxfId="20"/>
-    <tableColumn id="13" xr3:uid="{4AD58833-F3C1-46EA-9A7A-28F4B407835C}" name="材料８" dataDxfId="19"/>
-    <tableColumn id="14" xr3:uid="{EBD908AF-2D92-4A5C-99A1-5AC362AFB46C}" name="材料９" dataDxfId="18"/>
-    <tableColumn id="15" xr3:uid="{47F894FC-5641-4762-B81D-3A2CCA2FAAE3}" name="材料１０" dataDxfId="17"/>
-    <tableColumn id="16" xr3:uid="{4A508673-F9E6-4041-B040-6F6CFB42A1EE}" name="材料１１" dataDxfId="16"/>
-    <tableColumn id="17" xr3:uid="{3F9A4085-1BF4-4F18-8AA4-C8C69C6ED772}" name="材料１２" dataDxfId="15"/>
-    <tableColumn id="18" xr3:uid="{62C19D5A-8AF0-4735-9145-9A0A3AEC2022}" name="材料１３" dataDxfId="14"/>
-    <tableColumn id="19" xr3:uid="{A5556EA9-99A9-4F71-B90E-B88247A4EE0D}" name="塗布量" dataDxfId="13"/>
-    <tableColumn id="20" xr3:uid="{DAFEFD21-D65D-402E-AAED-F9D07B777569}" name="乾燥方式" dataDxfId="12"/>
-    <tableColumn id="21" xr3:uid="{1AF0029C-E222-4CF8-878F-C1AC9EDB34CF}" name="乾燥温度" dataDxfId="11"/>
-    <tableColumn id="22" xr3:uid="{61383965-32FF-4B6B-A130-112343B8352F}" name="乾燥時間" dataDxfId="10"/>
-    <tableColumn id="23" xr3:uid="{0DEA56C1-3AF8-488E-821F-D7ECE7DC486D}" name="擦過回数" dataDxfId="9"/>
-    <tableColumn id="24" xr3:uid="{1116544B-F4E0-45DF-ABA0-F7FE6533AD70}" name="擦過圧力" dataDxfId="8"/>
-    <tableColumn id="25" xr3:uid="{D9ACC828-BCC8-4B08-A153-E07A256FF1B0}" name="耐擦過性(n10" dataDxfId="7"/>
-    <tableColumn id="26" xr3:uid="{6D431567-CF0D-4A1A-BE2F-46F42416D8E0}" name="画像濃度" dataDxfId="6"/>
-    <tableColumn id="27" xr3:uid="{60BC8876-82FC-443A-B9E3-6F1E0B2F7B23}" name="粘度" dataDxfId="5"/>
-    <tableColumn id="28" xr3:uid="{F7778685-BDA9-4350-82B1-916E77C1E470}" name="表面張力" dataDxfId="4"/>
-    <tableColumn id="29" xr3:uid="{F314C44F-690D-4D00-BEA1-B1C1779E325A}" name="保存後粘度" dataDxfId="3"/>
-    <tableColumn id="30" xr3:uid="{3298EE1A-A00C-4093-9609-D7C71EB0FDE7}" name="保存後状態" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{E9A22458-9FAB-4C13-9BE1-E66B79D90E8E}" name="担当者" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{614AD84F-0894-4343-A1D6-B518FAC6CDDC}" name="備考" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{3FE65FF5-2F1D-461D-9A27-9E364D47118F}" name="材料１" dataDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{0319F8E7-300B-423E-9F06-BA16CF0DAB79}" name="材料２" dataDxfId="23"/>
+    <tableColumn id="8" xr3:uid="{7E73EAEC-77E2-41F2-B774-DAAA3A632F64}" name="材料３" dataDxfId="22"/>
+    <tableColumn id="9" xr3:uid="{2CAAD817-10C9-4A44-AFE0-171643F19D48}" name="材料４" dataDxfId="21"/>
+    <tableColumn id="10" xr3:uid="{4E0EEAC3-E19D-4FE7-933C-29E7C72E55D4}" name="材料５" dataDxfId="20"/>
+    <tableColumn id="11" xr3:uid="{DB55EB1E-83C3-46B1-8CAC-13E30A014C4C}" name="材料６" dataDxfId="19"/>
+    <tableColumn id="12" xr3:uid="{CC5EB82F-01B1-4A3B-AA90-23FF297DB203}" name="材料７" dataDxfId="18"/>
+    <tableColumn id="13" xr3:uid="{4AD58833-F3C1-46EA-9A7A-28F4B407835C}" name="材料８" dataDxfId="17"/>
+    <tableColumn id="14" xr3:uid="{EBD908AF-2D92-4A5C-99A1-5AC362AFB46C}" name="材料９" dataDxfId="16"/>
+    <tableColumn id="15" xr3:uid="{47F894FC-5641-4762-B81D-3A2CCA2FAAE3}" name="材料１０" dataDxfId="15"/>
+    <tableColumn id="16" xr3:uid="{4A508673-F9E6-4041-B040-6F6CFB42A1EE}" name="材料１１" dataDxfId="14"/>
+    <tableColumn id="17" xr3:uid="{3F9A4085-1BF4-4F18-8AA4-C8C69C6ED772}" name="材料１２" dataDxfId="13"/>
+    <tableColumn id="18" xr3:uid="{62C19D5A-8AF0-4735-9145-9A0A3AEC2022}" name="材料１３" dataDxfId="12"/>
+    <tableColumn id="19" xr3:uid="{A5556EA9-99A9-4F71-B90E-B88247A4EE0D}" name="塗布量" dataDxfId="11"/>
+    <tableColumn id="20" xr3:uid="{DAFEFD21-D65D-402E-AAED-F9D07B777569}" name="乾燥方式" dataDxfId="10"/>
+    <tableColumn id="21" xr3:uid="{1AF0029C-E222-4CF8-878F-C1AC9EDB34CF}" name="乾燥温度" dataDxfId="9"/>
+    <tableColumn id="22" xr3:uid="{61383965-32FF-4B6B-A130-112343B8352F}" name="乾燥時間" dataDxfId="8"/>
+    <tableColumn id="23" xr3:uid="{0DEA56C1-3AF8-488E-821F-D7ECE7DC486D}" name="擦過回数" dataDxfId="7"/>
+    <tableColumn id="24" xr3:uid="{1116544B-F4E0-45DF-ABA0-F7FE6533AD70}" name="擦過圧力" dataDxfId="6"/>
+    <tableColumn id="25" xr3:uid="{D9ACC828-BCC8-4B08-A153-E07A256FF1B0}" name="耐擦過性(n10" dataDxfId="5"/>
+    <tableColumn id="26" xr3:uid="{6D431567-CF0D-4A1A-BE2F-46F42416D8E0}" name="画像濃度" dataDxfId="4"/>
+    <tableColumn id="27" xr3:uid="{60BC8876-82FC-443A-B9E3-6F1E0B2F7B23}" name="粘度" dataDxfId="3"/>
+    <tableColumn id="28" xr3:uid="{F7778685-BDA9-4350-82B1-916E77C1E470}" name="表面張力" dataDxfId="2"/>
+    <tableColumn id="29" xr3:uid="{F314C44F-690D-4D00-BEA1-B1C1779E325A}" name="保存後粘度" dataDxfId="1"/>
+    <tableColumn id="30" xr3:uid="{3298EE1A-A00C-4093-9609-D7C71EB0FDE7}" name="保存後状態" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2695,114 +2695,114 @@
         <v>64</v>
       </c>
       <c r="AH5" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI5" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="AI5" s="12" t="s">
+      <c r="AJ5" s="12" t="s">
         <v>75</v>
-      </c>
-      <c r="AJ5" s="12" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="6" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="75">
+      <c r="D6" s="83">
         <v>45310</v>
       </c>
-      <c r="E6" s="76"/>
-      <c r="F6" s="76"/>
-      <c r="G6" s="76"/>
-      <c r="H6" s="77"/>
-      <c r="I6" s="75">
+      <c r="E6" s="84"/>
+      <c r="F6" s="84"/>
+      <c r="G6" s="84"/>
+      <c r="H6" s="85"/>
+      <c r="I6" s="83">
         <v>45321</v>
       </c>
-      <c r="J6" s="76"/>
-      <c r="K6" s="76"/>
-      <c r="L6" s="76"/>
-      <c r="M6" s="76"/>
-      <c r="N6" s="76"/>
-      <c r="O6" s="76"/>
-      <c r="P6" s="76"/>
-      <c r="Q6" s="77"/>
-      <c r="R6" s="75">
+      <c r="J6" s="84"/>
+      <c r="K6" s="84"/>
+      <c r="L6" s="84"/>
+      <c r="M6" s="84"/>
+      <c r="N6" s="84"/>
+      <c r="O6" s="84"/>
+      <c r="P6" s="84"/>
+      <c r="Q6" s="85"/>
+      <c r="R6" s="83">
         <v>45337</v>
       </c>
-      <c r="S6" s="76"/>
-      <c r="T6" s="76"/>
-      <c r="U6" s="77"/>
-      <c r="V6" s="75">
+      <c r="S6" s="84"/>
+      <c r="T6" s="84"/>
+      <c r="U6" s="85"/>
+      <c r="V6" s="83">
         <v>45350</v>
       </c>
-      <c r="W6" s="76"/>
-      <c r="X6" s="76"/>
-      <c r="Y6" s="77"/>
-      <c r="Z6" s="75">
+      <c r="W6" s="84"/>
+      <c r="X6" s="84"/>
+      <c r="Y6" s="85"/>
+      <c r="Z6" s="83">
         <v>45366</v>
       </c>
-      <c r="AA6" s="76"/>
-      <c r="AB6" s="76"/>
-      <c r="AC6" s="77"/>
-      <c r="AD6" s="75">
+      <c r="AA6" s="84"/>
+      <c r="AB6" s="84"/>
+      <c r="AC6" s="85"/>
+      <c r="AD6" s="83">
         <v>45392</v>
       </c>
-      <c r="AE6" s="76"/>
-      <c r="AF6" s="76"/>
-      <c r="AG6" s="76"/>
-      <c r="AH6" s="76"/>
-      <c r="AI6" s="76"/>
-      <c r="AJ6" s="77"/>
+      <c r="AE6" s="84"/>
+      <c r="AF6" s="84"/>
+      <c r="AG6" s="84"/>
+      <c r="AH6" s="84"/>
+      <c r="AI6" s="84"/>
+      <c r="AJ6" s="85"/>
     </row>
     <row r="7" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="C7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="78" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="79"/>
-      <c r="F7" s="79"/>
-      <c r="G7" s="79"/>
-      <c r="H7" s="80"/>
-      <c r="I7" s="78" t="s">
+      <c r="D7" s="86" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="87"/>
+      <c r="F7" s="87"/>
+      <c r="G7" s="87"/>
+      <c r="H7" s="88"/>
+      <c r="I7" s="86" t="s">
         <v>41</v>
       </c>
-      <c r="J7" s="79"/>
-      <c r="K7" s="79"/>
-      <c r="L7" s="79"/>
-      <c r="M7" s="79"/>
-      <c r="N7" s="79"/>
-      <c r="O7" s="79"/>
-      <c r="P7" s="79"/>
-      <c r="Q7" s="80"/>
-      <c r="R7" s="78" t="s">
-        <v>40</v>
-      </c>
-      <c r="S7" s="79"/>
-      <c r="T7" s="79"/>
-      <c r="U7" s="80"/>
-      <c r="V7" s="78" t="s">
+      <c r="J7" s="87"/>
+      <c r="K7" s="87"/>
+      <c r="L7" s="87"/>
+      <c r="M7" s="87"/>
+      <c r="N7" s="87"/>
+      <c r="O7" s="87"/>
+      <c r="P7" s="87"/>
+      <c r="Q7" s="88"/>
+      <c r="R7" s="86" t="s">
+        <v>40</v>
+      </c>
+      <c r="S7" s="87"/>
+      <c r="T7" s="87"/>
+      <c r="U7" s="88"/>
+      <c r="V7" s="86" t="s">
         <v>41</v>
       </c>
-      <c r="W7" s="79"/>
-      <c r="X7" s="79"/>
-      <c r="Y7" s="80"/>
-      <c r="Z7" s="78" t="s">
+      <c r="W7" s="87"/>
+      <c r="X7" s="87"/>
+      <c r="Y7" s="88"/>
+      <c r="Z7" s="86" t="s">
         <v>41</v>
       </c>
-      <c r="AA7" s="79"/>
-      <c r="AB7" s="79"/>
-      <c r="AC7" s="80"/>
-      <c r="AD7" s="78" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE7" s="79"/>
-      <c r="AF7" s="79"/>
-      <c r="AG7" s="79"/>
-      <c r="AH7" s="79"/>
-      <c r="AI7" s="79"/>
-      <c r="AJ7" s="80"/>
+      <c r="AA7" s="87"/>
+      <c r="AB7" s="87"/>
+      <c r="AC7" s="88"/>
+      <c r="AD7" s="86" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE7" s="87"/>
+      <c r="AF7" s="87"/>
+      <c r="AG7" s="87"/>
+      <c r="AH7" s="87"/>
+      <c r="AI7" s="87"/>
+      <c r="AJ7" s="88"/>
     </row>
     <row r="8" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="C8" s="1" t="s">
@@ -2853,7 +2853,7 @@
         <v>53</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D9" s="50">
         <v>46.9</v>
@@ -2958,7 +2958,7 @@
     <row r="10" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="21"/>
       <c r="C10" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D10" s="50">
         <v>40</v>
@@ -3063,7 +3063,7 @@
     <row r="11" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="21"/>
       <c r="C11" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D11" s="50">
         <v>0</v>
@@ -3168,7 +3168,7 @@
     <row r="12" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="21"/>
       <c r="C12" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D12" s="50">
         <v>2</v>
@@ -3273,7 +3273,7 @@
     <row r="13" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="21"/>
       <c r="C13" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D13" s="50">
         <v>0</v>
@@ -3378,7 +3378,7 @@
     <row r="14" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="21"/>
       <c r="C14" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D14" s="50">
         <v>2</v>
@@ -3483,7 +3483,7 @@
     <row r="15" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="21"/>
       <c r="C15" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D15" s="50">
         <v>0</v>
@@ -3588,7 +3588,7 @@
     <row r="16" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="21"/>
       <c r="C16" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D16" s="50">
         <v>0</v>
@@ -3693,7 +3693,7 @@
     <row r="17" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" s="21"/>
       <c r="C17" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D17" s="50">
         <v>5</v>
@@ -3798,7 +3798,7 @@
     <row r="18" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" s="21"/>
       <c r="C18" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D18" s="50">
         <v>0</v>
@@ -3903,7 +3903,7 @@
     <row r="19" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="21"/>
       <c r="C19" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D19" s="50">
         <v>4</v>
@@ -4008,7 +4008,7 @@
     <row r="20" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" s="21"/>
       <c r="C20" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D20" s="50">
         <v>0</v>
@@ -4113,7 +4113,7 @@
     <row r="21" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" s="22"/>
       <c r="C21" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D21" s="50">
         <v>0.1</v>
@@ -4465,51 +4465,51 @@
       <c r="C25" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="81" t="s">
+      <c r="D25" s="77" t="s">
         <v>58</v>
       </c>
-      <c r="E25" s="82"/>
-      <c r="F25" s="82"/>
-      <c r="G25" s="82"/>
-      <c r="H25" s="82"/>
-      <c r="I25" s="82"/>
-      <c r="J25" s="82"/>
-      <c r="K25" s="82"/>
-      <c r="L25" s="82"/>
-      <c r="M25" s="82"/>
-      <c r="N25" s="82"/>
-      <c r="O25" s="82"/>
-      <c r="P25" s="82"/>
-      <c r="Q25" s="82"/>
-      <c r="R25" s="82"/>
-      <c r="S25" s="82"/>
-      <c r="T25" s="82"/>
-      <c r="U25" s="82"/>
-      <c r="V25" s="82"/>
-      <c r="W25" s="82"/>
-      <c r="X25" s="82"/>
-      <c r="Y25" s="82"/>
-      <c r="Z25" s="82"/>
-      <c r="AA25" s="82"/>
-      <c r="AB25" s="82"/>
-      <c r="AC25" s="83"/>
+      <c r="E25" s="78"/>
+      <c r="F25" s="78"/>
+      <c r="G25" s="78"/>
+      <c r="H25" s="78"/>
+      <c r="I25" s="78"/>
+      <c r="J25" s="78"/>
+      <c r="K25" s="78"/>
+      <c r="L25" s="78"/>
+      <c r="M25" s="78"/>
+      <c r="N25" s="78"/>
+      <c r="O25" s="78"/>
+      <c r="P25" s="78"/>
+      <c r="Q25" s="78"/>
+      <c r="R25" s="78"/>
+      <c r="S25" s="78"/>
+      <c r="T25" s="78"/>
+      <c r="U25" s="78"/>
+      <c r="V25" s="78"/>
+      <c r="W25" s="78"/>
+      <c r="X25" s="78"/>
+      <c r="Y25" s="78"/>
+      <c r="Z25" s="78"/>
+      <c r="AA25" s="78"/>
+      <c r="AB25" s="78"/>
+      <c r="AC25" s="79"/>
       <c r="AD25" s="8">
         <v>9.8199999999999985</v>
       </c>
       <c r="AE25" s="46" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF25" s="8" t="s">
         <v>83</v>
-      </c>
-      <c r="AF25" s="8" t="s">
-        <v>84</v>
       </c>
       <c r="AG25" s="8">
         <v>10.069999999999999</v>
       </c>
       <c r="AH25" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="AI25" s="45" t="s">
         <v>85</v>
-      </c>
-      <c r="AI25" s="45" t="s">
-        <v>86</v>
       </c>
       <c r="AJ25" s="1">
         <v>12.6</v>
@@ -4630,65 +4630,65 @@
       <c r="C28" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D28" s="84" t="s">
+      <c r="D28" s="80" t="s">
         <v>66</v>
       </c>
-      <c r="E28" s="85"/>
-      <c r="F28" s="85"/>
-      <c r="G28" s="85"/>
-      <c r="H28" s="85"/>
-      <c r="I28" s="85"/>
-      <c r="J28" s="85"/>
-      <c r="K28" s="85"/>
-      <c r="L28" s="85"/>
-      <c r="M28" s="85"/>
-      <c r="N28" s="85"/>
-      <c r="O28" s="85"/>
-      <c r="P28" s="85"/>
-      <c r="Q28" s="86"/>
-      <c r="R28" s="84" t="s">
-        <v>82</v>
-      </c>
-      <c r="S28" s="85"/>
-      <c r="T28" s="85"/>
-      <c r="U28" s="85"/>
-      <c r="V28" s="85"/>
-      <c r="W28" s="85"/>
-      <c r="X28" s="85"/>
-      <c r="Y28" s="85"/>
-      <c r="Z28" s="85"/>
-      <c r="AA28" s="85"/>
-      <c r="AB28" s="85"/>
-      <c r="AC28" s="85"/>
-      <c r="AD28" s="85"/>
-      <c r="AE28" s="85"/>
-      <c r="AF28" s="85"/>
-      <c r="AG28" s="85"/>
-      <c r="AH28" s="85"/>
-      <c r="AI28" s="85"/>
-      <c r="AJ28" s="86"/>
+      <c r="E28" s="81"/>
+      <c r="F28" s="81"/>
+      <c r="G28" s="81"/>
+      <c r="H28" s="81"/>
+      <c r="I28" s="81"/>
+      <c r="J28" s="81"/>
+      <c r="K28" s="81"/>
+      <c r="L28" s="81"/>
+      <c r="M28" s="81"/>
+      <c r="N28" s="81"/>
+      <c r="O28" s="81"/>
+      <c r="P28" s="81"/>
+      <c r="Q28" s="82"/>
+      <c r="R28" s="80" t="s">
+        <v>81</v>
+      </c>
+      <c r="S28" s="81"/>
+      <c r="T28" s="81"/>
+      <c r="U28" s="81"/>
+      <c r="V28" s="81"/>
+      <c r="W28" s="81"/>
+      <c r="X28" s="81"/>
+      <c r="Y28" s="81"/>
+      <c r="Z28" s="81"/>
+      <c r="AA28" s="81"/>
+      <c r="AB28" s="81"/>
+      <c r="AC28" s="81"/>
+      <c r="AD28" s="81"/>
+      <c r="AE28" s="81"/>
+      <c r="AF28" s="81"/>
+      <c r="AG28" s="81"/>
+      <c r="AH28" s="81"/>
+      <c r="AI28" s="81"/>
+      <c r="AJ28" s="82"/>
     </row>
     <row r="29" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="B29" s="21"/>
       <c r="C29" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D29" s="84" t="s">
+      <c r="D29" s="80" t="s">
         <v>60</v>
       </c>
-      <c r="E29" s="85"/>
-      <c r="F29" s="85"/>
-      <c r="G29" s="85"/>
-      <c r="H29" s="85"/>
-      <c r="I29" s="85"/>
-      <c r="J29" s="85"/>
-      <c r="K29" s="85"/>
-      <c r="L29" s="85"/>
-      <c r="M29" s="85"/>
-      <c r="N29" s="85"/>
-      <c r="O29" s="85"/>
-      <c r="P29" s="85"/>
-      <c r="Q29" s="86"/>
+      <c r="E29" s="81"/>
+      <c r="F29" s="81"/>
+      <c r="G29" s="81"/>
+      <c r="H29" s="81"/>
+      <c r="I29" s="81"/>
+      <c r="J29" s="81"/>
+      <c r="K29" s="81"/>
+      <c r="L29" s="81"/>
+      <c r="M29" s="81"/>
+      <c r="N29" s="81"/>
+      <c r="O29" s="81"/>
+      <c r="P29" s="81"/>
+      <c r="Q29" s="82"/>
       <c r="R29" s="47">
         <v>100</v>
       </c>
@@ -4752,22 +4752,22 @@
       <c r="C30" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D30" s="84" t="s">
+      <c r="D30" s="80" t="s">
         <v>59</v>
       </c>
-      <c r="E30" s="85"/>
-      <c r="F30" s="85"/>
-      <c r="G30" s="85"/>
-      <c r="H30" s="85"/>
-      <c r="I30" s="85"/>
-      <c r="J30" s="85"/>
-      <c r="K30" s="85"/>
-      <c r="L30" s="85"/>
-      <c r="M30" s="85"/>
-      <c r="N30" s="85"/>
-      <c r="O30" s="85"/>
-      <c r="P30" s="85"/>
-      <c r="Q30" s="86"/>
+      <c r="E30" s="81"/>
+      <c r="F30" s="81"/>
+      <c r="G30" s="81"/>
+      <c r="H30" s="81"/>
+      <c r="I30" s="81"/>
+      <c r="J30" s="81"/>
+      <c r="K30" s="81"/>
+      <c r="L30" s="81"/>
+      <c r="M30" s="81"/>
+      <c r="N30" s="81"/>
+      <c r="O30" s="81"/>
+      <c r="P30" s="81"/>
+      <c r="Q30" s="82"/>
       <c r="R30" s="47">
         <v>0.01</v>
       </c>
@@ -5319,23 +5319,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="D25:AC25"/>
-    <mergeCell ref="D30:Q30"/>
-    <mergeCell ref="D29:Q29"/>
-    <mergeCell ref="D28:Q28"/>
-    <mergeCell ref="R28:AJ28"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="I6:Q6"/>
+    <mergeCell ref="R6:U6"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="I7:Q7"/>
+    <mergeCell ref="R7:U7"/>
     <mergeCell ref="V6:Y6"/>
     <mergeCell ref="Z6:AC6"/>
     <mergeCell ref="AD6:AJ6"/>
     <mergeCell ref="V7:Y7"/>
     <mergeCell ref="Z7:AC7"/>
     <mergeCell ref="AD7:AJ7"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="I6:Q6"/>
-    <mergeCell ref="R6:U6"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="I7:Q7"/>
-    <mergeCell ref="R7:U7"/>
+    <mergeCell ref="D25:AC25"/>
+    <mergeCell ref="D30:Q30"/>
+    <mergeCell ref="D29:Q29"/>
+    <mergeCell ref="D28:Q28"/>
+    <mergeCell ref="R28:AJ28"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5469,13 +5469,13 @@
         <v>64</v>
       </c>
       <c r="AH5" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI5" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="AI5" s="12" t="s">
+      <c r="AJ5" s="12" t="s">
         <v>75</v>
-      </c>
-      <c r="AJ5" s="12" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="6" spans="2:36" x14ac:dyDescent="0.55000000000000004">
@@ -5735,7 +5735,7 @@
         <v>53</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D9" s="50">
         <v>46.9</v>
@@ -5840,7 +5840,7 @@
     <row r="10" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="21"/>
       <c r="C10" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D10" s="50">
         <v>40</v>
@@ -5945,7 +5945,7 @@
     <row r="11" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="21"/>
       <c r="C11" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D11" s="50">
         <v>0</v>
@@ -6050,7 +6050,7 @@
     <row r="12" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="21"/>
       <c r="C12" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D12" s="50">
         <v>2</v>
@@ -6155,7 +6155,7 @@
     <row r="13" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="21"/>
       <c r="C13" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D13" s="50">
         <v>0</v>
@@ -6260,7 +6260,7 @@
     <row r="14" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="21"/>
       <c r="C14" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D14" s="50">
         <v>2</v>
@@ -6365,7 +6365,7 @@
     <row r="15" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="21"/>
       <c r="C15" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D15" s="50">
         <v>0</v>
@@ -6470,7 +6470,7 @@
     <row r="16" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="21"/>
       <c r="C16" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D16" s="50">
         <v>0</v>
@@ -6575,7 +6575,7 @@
     <row r="17" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" s="21"/>
       <c r="C17" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D17" s="50">
         <v>5</v>
@@ -6680,7 +6680,7 @@
     <row r="18" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" s="21"/>
       <c r="C18" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D18" s="50">
         <v>0</v>
@@ -6785,7 +6785,7 @@
     <row r="19" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="21"/>
       <c r="C19" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D19" s="50">
         <v>4</v>
@@ -6890,7 +6890,7 @@
     <row r="20" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" s="21"/>
       <c r="C20" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D20" s="50">
         <v>0</v>
@@ -6995,7 +6995,7 @@
     <row r="21" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" s="22"/>
       <c r="C21" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D21" s="50">
         <v>0.1</v>
@@ -7429,19 +7429,19 @@
         <v>9.8199999999999985</v>
       </c>
       <c r="AE25" s="46" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF25" s="8" t="s">
         <v>83</v>
-      </c>
-      <c r="AF25" s="8" t="s">
-        <v>84</v>
       </c>
       <c r="AG25" s="8">
         <v>10.069999999999999</v>
       </c>
       <c r="AH25" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="AI25" s="45" t="s">
         <v>85</v>
-      </c>
-      <c r="AI25" s="45" t="s">
-        <v>86</v>
       </c>
       <c r="AJ25" s="1">
         <v>12.6</v>
@@ -7605,61 +7605,61 @@
         <v>66</v>
       </c>
       <c r="R28" s="47" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="S28" s="47" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="T28" s="47" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="U28" s="47" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="V28" s="47" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="W28" s="47" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="X28" s="47" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Y28" s="47" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Z28" s="47" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA28" s="47" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AB28" s="47" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AC28" s="47" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AD28" s="47" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AE28" s="47" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AF28" s="47" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AG28" s="47" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AH28" s="47" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AI28" s="47" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AJ28" s="47" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="2:36" x14ac:dyDescent="0.55000000000000004">
@@ -8447,43 +8447,43 @@
         <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="O6" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="P6" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="Q6" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="R6" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="S6" s="24" t="s">
         <v>8</v>
@@ -10850,7 +10850,7 @@
         <v>34</v>
       </c>
       <c r="U34" s="40" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="V34" s="24">
         <v>2</v>
@@ -10934,7 +10934,7 @@
         <v>32</v>
       </c>
       <c r="U35" s="40" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="V35" s="24">
         <v>2</v>
@@ -11047,7 +11047,7 @@
     </row>
     <row r="37" spans="2:29" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="B37" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C37" s="28">
         <v>45392</v>
@@ -11102,7 +11102,7 @@
         <v>34</v>
       </c>
       <c r="U37" s="40" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="V37" s="24">
         <v>2</v>
@@ -11131,7 +11131,7 @@
     </row>
     <row r="38" spans="2:29" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="B38" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C38" s="28">
         <v>45392</v>
@@ -11186,7 +11186,7 @@
         <v>32</v>
       </c>
       <c r="U38" s="40" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="V38" s="24">
         <v>2</v>
@@ -11215,7 +11215,7 @@
     </row>
     <row r="39" spans="2:29" x14ac:dyDescent="0.55000000000000004">
       <c r="B39" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C39" s="28">
         <v>45392</v>
@@ -11386,43 +11386,43 @@
         <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="O6" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="P6" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="Q6" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="R6" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="S6" s="24" t="s">
         <v>8</v>
@@ -14027,7 +14027,7 @@
     </row>
     <row r="37" spans="2:30" x14ac:dyDescent="0.55000000000000004">
       <c r="B37" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C37" s="28">
         <v>45392</v>
@@ -14114,7 +14114,7 @@
     </row>
     <row r="38" spans="2:30" x14ac:dyDescent="0.55000000000000004">
       <c r="B38" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C38" s="28">
         <v>45392</v>
@@ -14201,7 +14201,7 @@
     </row>
     <row r="39" spans="2:30" x14ac:dyDescent="0.55000000000000004">
       <c r="B39" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C39" s="28">
         <v>45392</v>
@@ -14297,11 +14297,11 @@
   <dimension ref="B4:AD39"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="H17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="3" topLeftCell="M7" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
       <selection pane="topRight" activeCell="E4" sqref="E4"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="Z17" sqref="Z17"/>
+      <selection pane="bottomRight" activeCell="Z15" sqref="Z15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -14329,13 +14329,13 @@
         <v>38</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AA4" t="s">
         <v>49</v>
       </c>
       <c r="AB4" t="s">
-        <v>73</v>
+        <v>121</v>
       </c>
       <c r="AC4" t="s">
         <v>49</v>
@@ -14358,13 +14358,13 @@
       <c r="Q5" s="9"/>
       <c r="R5" s="9"/>
       <c r="S5" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="T5" s="9"/>
       <c r="U5" s="14"/>
       <c r="V5" s="14"/>
       <c r="W5" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X5" s="9"/>
       <c r="Y5" s="18" t="s">
@@ -14372,7 +14372,7 @@
       </c>
       <c r="Z5" s="19"/>
       <c r="AA5" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AB5" s="9"/>
       <c r="AC5" s="9"/>
@@ -14392,43 +14392,43 @@
         <v>1</v>
       </c>
       <c r="F6" s="62" t="s">
+        <v>98</v>
+      </c>
+      <c r="G6" s="62" t="s">
         <v>99</v>
       </c>
-      <c r="G6" s="62" t="s">
+      <c r="H6" s="62" t="s">
         <v>100</v>
       </c>
-      <c r="H6" s="62" t="s">
+      <c r="I6" s="62" t="s">
         <v>101</v>
       </c>
-      <c r="I6" s="62" t="s">
+      <c r="J6" s="62" t="s">
         <v>102</v>
       </c>
-      <c r="J6" s="62" t="s">
+      <c r="K6" s="62" t="s">
         <v>103</v>
       </c>
-      <c r="K6" s="62" t="s">
+      <c r="L6" s="62" t="s">
         <v>104</v>
       </c>
-      <c r="L6" s="62" t="s">
+      <c r="M6" s="62" t="s">
         <v>105</v>
       </c>
-      <c r="M6" s="62" t="s">
+      <c r="N6" s="62" t="s">
         <v>106</v>
       </c>
-      <c r="N6" s="62" t="s">
+      <c r="O6" s="62" t="s">
         <v>107</v>
       </c>
-      <c r="O6" s="62" t="s">
+      <c r="P6" s="62" t="s">
         <v>108</v>
       </c>
-      <c r="P6" s="62" t="s">
+      <c r="Q6" s="62" t="s">
         <v>109</v>
       </c>
-      <c r="Q6" s="62" t="s">
+      <c r="R6" s="62" t="s">
         <v>110</v>
-      </c>
-      <c r="R6" s="62" t="s">
-        <v>111</v>
       </c>
       <c r="S6" s="62" t="s">
         <v>63</v>
@@ -14464,7 +14464,7 @@
         <v>10</v>
       </c>
       <c r="AD6" s="63" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="2:30" x14ac:dyDescent="0.55000000000000004">
@@ -16953,7 +16953,7 @@
     </row>
     <row r="37" spans="2:30" x14ac:dyDescent="0.55000000000000004">
       <c r="B37" s="59" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C37" s="28">
         <v>45392</v>
@@ -17040,7 +17040,7 @@
     </row>
     <row r="38" spans="2:30" x14ac:dyDescent="0.55000000000000004">
       <c r="B38" s="59" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C38" s="28">
         <v>45392</v>
@@ -17127,7 +17127,7 @@
     </row>
     <row r="39" spans="2:30" x14ac:dyDescent="0.55000000000000004">
       <c r="B39" s="64" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C39" s="65">
         <v>45392</v>
@@ -17225,8 +17225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{946DA809-6F7B-4F40-B49B-27E3855F241E}">
   <dimension ref="A1:Y25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="W25" sqref="W25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -17253,81 +17253,81 @@
     <row r="1" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="72"/>
       <c r="B1" s="72" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="72" t="s">
         <v>99</v>
       </c>
-      <c r="C1" s="72" t="s">
+      <c r="D1" s="72" t="s">
         <v>100</v>
       </c>
-      <c r="D1" s="72" t="s">
+      <c r="E1" s="72" t="s">
         <v>101</v>
       </c>
-      <c r="E1" s="72" t="s">
+      <c r="F1" s="72" t="s">
         <v>102</v>
       </c>
-      <c r="F1" s="72" t="s">
+      <c r="G1" s="72" t="s">
         <v>103</v>
       </c>
-      <c r="G1" s="72" t="s">
+      <c r="H1" s="72" t="s">
         <v>104</v>
       </c>
-      <c r="H1" s="72" t="s">
+      <c r="I1" s="72" t="s">
         <v>105</v>
       </c>
-      <c r="I1" s="72" t="s">
+      <c r="J1" s="72" t="s">
         <v>106</v>
       </c>
-      <c r="J1" s="72" t="s">
+      <c r="K1" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="K1" s="72" t="s">
+      <c r="L1" s="72" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="72" t="s">
+      <c r="M1" s="72" t="s">
         <v>109</v>
       </c>
-      <c r="M1" s="72" t="s">
+      <c r="N1" s="72" t="s">
         <v>110</v>
       </c>
-      <c r="N1" s="72" t="s">
-        <v>111</v>
-      </c>
       <c r="O1" s="72" t="s">
+        <v>87</v>
+      </c>
+      <c r="P1" s="72" t="s">
         <v>88</v>
       </c>
-      <c r="P1" s="72" t="s">
+      <c r="Q1" s="72" t="s">
         <v>89</v>
       </c>
-      <c r="Q1" s="72" t="s">
+      <c r="R1" s="72" t="s">
         <v>90</v>
       </c>
-      <c r="R1" s="72" t="s">
+      <c r="S1" s="72" t="s">
         <v>91</v>
       </c>
-      <c r="S1" s="72" t="s">
+      <c r="T1" s="72" t="s">
         <v>92</v>
       </c>
-      <c r="T1" s="72" t="s">
+      <c r="U1" s="72" t="s">
         <v>93</v>
       </c>
-      <c r="U1" s="72" t="s">
+      <c r="V1" s="72" t="s">
         <v>94</v>
       </c>
-      <c r="V1" s="72" t="s">
+      <c r="W1" s="72" t="s">
         <v>95</v>
       </c>
-      <c r="W1" s="72" t="s">
+      <c r="X1" s="72" t="s">
         <v>96</v>
       </c>
-      <c r="X1" s="72" t="s">
+      <c r="Y1" s="72" t="s">
         <v>97</v>
-      </c>
-      <c r="Y1" s="72" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B2" s="73">
         <v>1</v>
@@ -17358,7 +17358,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B3" s="73">
         <v>0.54532269214902873</v>
@@ -17391,7 +17391,7 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B4" s="73">
         <v>-0.5693038369307919</v>
@@ -17426,7 +17426,7 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B5" s="73">
         <v>0.37186951414850039</v>
@@ -17463,7 +17463,7 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B6" s="73">
         <v>-0.52142976010762865</v>
@@ -17502,7 +17502,7 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B7" s="73">
         <v>-0.40937219968250366</v>
@@ -17543,7 +17543,7 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B8" s="73">
         <v>0.2064701282579329</v>
@@ -17586,7 +17586,7 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B9" s="73">
         <v>0.2064701282579329</v>
@@ -17631,7 +17631,7 @@
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B10" s="73">
         <v>4.7941143432472522E-2</v>
@@ -17678,7 +17678,7 @@
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B11" s="73">
         <v>-0.42354601289696908</v>
@@ -17727,7 +17727,7 @@
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B12" s="73">
         <v>-0.56094629067505208</v>
@@ -17778,7 +17778,7 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B13" s="73">
         <v>5.4122225092713113E-3</v>
@@ -17831,7 +17831,7 @@
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B14" s="73">
         <v>6.8298341815840067E-15</v>
@@ -17886,7 +17886,7 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B15" s="73" t="e">
         <v>#DIV/0!</v>
@@ -17943,7 +17943,7 @@
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B16" s="73">
         <v>-0.63644724213007908</v>
@@ -18002,7 +18002,7 @@
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B17" s="73">
         <v>-0.63090569434588195</v>
@@ -18063,7 +18063,7 @@
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B18" s="73">
         <v>-0.26911365410861021</v>
@@ -18126,7 +18126,7 @@
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B19" s="73" t="e">
         <v>#DIV/0!</v>
@@ -18191,7 +18191,7 @@
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B20" s="73" t="e">
         <v>#DIV/0!</v>
@@ -18258,7 +18258,7 @@
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B21" s="73">
         <v>-0.65684655212468779</v>
@@ -18327,7 +18327,7 @@
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B22" s="73">
         <v>-0.6139086961176804</v>
@@ -18398,7 +18398,7 @@
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B23" s="73">
         <v>-0.21401478203302254</v>
@@ -18471,7 +18471,7 @@
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B24" s="73">
         <v>0.88528380522770744</v>
@@ -18546,7 +18546,7 @@
     </row>
     <row r="25" spans="1:25" ht="18.5" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A25" s="71" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B25" s="74">
         <v>-0.53311575526124477</v>
@@ -18643,9 +18643,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFFD9269-7F18-4E64-8D48-3C1F1E4D91C0}">
   <dimension ref="B2:AF47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B45" sqref="B45:B47"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="5" topLeftCell="Q1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AA9" sqref="AA9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -18676,13 +18676,13 @@
         <v>38</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AC2" t="s">
         <v>49</v>
       </c>
       <c r="AD2" t="s">
-        <v>73</v>
+        <v>121</v>
       </c>
       <c r="AE2" t="s">
         <v>49</v>
@@ -18705,17 +18705,17 @@
       <c r="Q3" s="9"/>
       <c r="R3" s="9"/>
       <c r="S3" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="T3" s="9"/>
       <c r="U3" s="14"/>
       <c r="V3" s="14"/>
       <c r="W3" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X3" s="9"/>
       <c r="Y3" s="57" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Z3" s="19"/>
       <c r="AA3" s="18" t="s">
@@ -18723,7 +18723,7 @@
       </c>
       <c r="AB3" s="19"/>
       <c r="AC3" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AD3" s="9"/>
       <c r="AE3" s="9"/>
@@ -18743,43 +18743,43 @@
         <v>1</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="S4" s="1" t="s">
         <v>63</v>
@@ -21750,7 +21750,7 @@
     </row>
     <row r="35" spans="2:32" x14ac:dyDescent="0.55000000000000004">
       <c r="B35" s="41" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C35" s="52">
         <v>45392</v>
@@ -21849,7 +21849,7 @@
     </row>
     <row r="36" spans="2:32" x14ac:dyDescent="0.55000000000000004">
       <c r="B36" s="41" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C36" s="52">
         <v>45392</v>
@@ -21948,7 +21948,7 @@
     </row>
     <row r="37" spans="2:32" x14ac:dyDescent="0.55000000000000004">
       <c r="B37" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C37" s="52">
         <v>45392</v>
@@ -22047,7 +22047,7 @@
     </row>
     <row r="39" spans="2:32" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B39" s="41" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C39" s="52"/>
       <c r="D39" s="52"/>
@@ -22140,7 +22140,7 @@
     </row>
     <row r="40" spans="2:32" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B40" s="41" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C40" s="52"/>
       <c r="D40" s="52"/>
@@ -22233,7 +22233,7 @@
     </row>
     <row r="41" spans="2:32" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B41" s="41" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C41" s="52"/>
       <c r="D41" s="52"/>
@@ -22326,7 +22326,7 @@
     </row>
     <row r="42" spans="2:32" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B42" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C42" s="54"/>
       <c r="D42" s="54"/>
@@ -22395,15 +22395,15 @@
       <c r="Z42" s="55">
         <v>2</v>
       </c>
-      <c r="AA42" s="87">
+      <c r="AA42" s="75">
         <f t="shared" si="13"/>
         <v>5</v>
       </c>
-      <c r="AB42" s="88">
+      <c r="AB42" s="76">
         <f t="shared" si="14"/>
         <v>1.46</v>
       </c>
-      <c r="AC42" s="87">
+      <c r="AC42" s="75">
         <f t="shared" si="15"/>
         <v>9.1999999999999993</v>
       </c>
@@ -22411,7 +22411,7 @@
         <f t="shared" si="16"/>
         <v>34</v>
       </c>
-      <c r="AE42" s="87">
+      <c r="AE42" s="75">
         <f t="shared" si="17"/>
         <v>11.6</v>
       </c>
@@ -22419,7 +22419,7 @@
     </row>
     <row r="43" spans="2:32" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B43" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C43" s="54"/>
       <c r="D43" s="54"/>
@@ -22488,15 +22488,15 @@
       <c r="Z43" s="55">
         <v>2</v>
       </c>
-      <c r="AA43" s="87">
+      <c r="AA43" s="75">
         <f t="shared" si="13"/>
         <v>5</v>
       </c>
-      <c r="AB43" s="88">
+      <c r="AB43" s="76">
         <f t="shared" si="14"/>
         <v>1.43</v>
       </c>
-      <c r="AC43" s="87">
+      <c r="AC43" s="75">
         <f t="shared" si="15"/>
         <v>9.1</v>
       </c>
@@ -22504,7 +22504,7 @@
         <f t="shared" si="16"/>
         <v>34</v>
       </c>
-      <c r="AE43" s="87">
+      <c r="AE43" s="75">
         <f t="shared" si="17"/>
         <v>11.5</v>
       </c>
@@ -22512,7 +22512,7 @@
     </row>
     <row r="44" spans="2:32" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B44" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C44" s="54"/>
       <c r="D44" s="54"/>
@@ -22581,15 +22581,15 @@
       <c r="Z44" s="55">
         <v>2</v>
       </c>
-      <c r="AA44" s="87">
+      <c r="AA44" s="75">
         <f t="shared" si="13"/>
         <v>5</v>
       </c>
-      <c r="AB44" s="88">
+      <c r="AB44" s="76">
         <f t="shared" si="14"/>
         <v>1.41</v>
       </c>
-      <c r="AC44" s="87">
+      <c r="AC44" s="75">
         <f t="shared" si="15"/>
         <v>9</v>
       </c>
@@ -22597,7 +22597,7 @@
         <f t="shared" si="16"/>
         <v>34</v>
       </c>
-      <c r="AE44" s="87">
+      <c r="AE44" s="75">
         <f t="shared" si="17"/>
         <v>11.4</v>
       </c>
@@ -22605,7 +22605,7 @@
     </row>
     <row r="45" spans="2:32" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B45" s="41" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C45" s="52"/>
       <c r="D45" s="52"/>
@@ -22698,7 +22698,7 @@
     </row>
     <row r="46" spans="2:32" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B46" s="41" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C46" s="52"/>
       <c r="D46" s="52"/>
@@ -22791,7 +22791,7 @@
     </row>
     <row r="47" spans="2:32" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B47" s="41" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C47" s="52"/>
       <c r="D47" s="52"/>

</xml_diff>

<commit_message>
add chapter4 power query xlsx
</commit_message>
<xml_diff>
--- a/chapter2/input/chapter2_demo_data.xlsx
+++ b/chapter2/input/chapter2_demo_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\副業関連\独立\執筆\practical-mi-guide\chapter2\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0EC40AA-0ABD-4ADF-9D92-A6D549873895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACF01F2C-443B-43C0-8C5D-008D42E1DDF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="590" yWindow="3490" windowWidth="30300" windowHeight="17850" activeTab="6" xr2:uid="{AFFCA931-CB2A-4AED-B7E5-2638B5FCE6AD}"/>
+    <workbookView xWindow="9700" yWindow="2470" windowWidth="22490" windowHeight="17850" activeTab="4" xr2:uid="{AFFCA931-CB2A-4AED-B7E5-2638B5FCE6AD}"/>
   </bookViews>
   <sheets>
     <sheet name="初期データ" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1207" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1208" uniqueCount="123">
   <si>
     <t>サンプル作成日</t>
     <rPh sb="4" eb="7">
@@ -681,6 +681,14 @@
     <t>32－38</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>0:自然乾燥
+1:ドライヤー</t>
+    <rPh sb="2" eb="6">
+      <t>シゼンカンソウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
@@ -1148,6 +1156,24 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1164,24 +1190,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2708,101 +2716,101 @@
       <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="83">
+      <c r="D6" s="77">
         <v>45310</v>
       </c>
-      <c r="E6" s="84"/>
-      <c r="F6" s="84"/>
-      <c r="G6" s="84"/>
-      <c r="H6" s="85"/>
-      <c r="I6" s="83">
+      <c r="E6" s="78"/>
+      <c r="F6" s="78"/>
+      <c r="G6" s="78"/>
+      <c r="H6" s="79"/>
+      <c r="I6" s="77">
         <v>45321</v>
       </c>
-      <c r="J6" s="84"/>
-      <c r="K6" s="84"/>
-      <c r="L6" s="84"/>
-      <c r="M6" s="84"/>
-      <c r="N6" s="84"/>
-      <c r="O6" s="84"/>
-      <c r="P6" s="84"/>
-      <c r="Q6" s="85"/>
-      <c r="R6" s="83">
+      <c r="J6" s="78"/>
+      <c r="K6" s="78"/>
+      <c r="L6" s="78"/>
+      <c r="M6" s="78"/>
+      <c r="N6" s="78"/>
+      <c r="O6" s="78"/>
+      <c r="P6" s="78"/>
+      <c r="Q6" s="79"/>
+      <c r="R6" s="77">
         <v>45337</v>
       </c>
-      <c r="S6" s="84"/>
-      <c r="T6" s="84"/>
-      <c r="U6" s="85"/>
-      <c r="V6" s="83">
+      <c r="S6" s="78"/>
+      <c r="T6" s="78"/>
+      <c r="U6" s="79"/>
+      <c r="V6" s="77">
         <v>45350</v>
       </c>
-      <c r="W6" s="84"/>
-      <c r="X6" s="84"/>
-      <c r="Y6" s="85"/>
-      <c r="Z6" s="83">
+      <c r="W6" s="78"/>
+      <c r="X6" s="78"/>
+      <c r="Y6" s="79"/>
+      <c r="Z6" s="77">
         <v>45366</v>
       </c>
-      <c r="AA6" s="84"/>
-      <c r="AB6" s="84"/>
-      <c r="AC6" s="85"/>
-      <c r="AD6" s="83">
+      <c r="AA6" s="78"/>
+      <c r="AB6" s="78"/>
+      <c r="AC6" s="79"/>
+      <c r="AD6" s="77">
         <v>45392</v>
       </c>
-      <c r="AE6" s="84"/>
-      <c r="AF6" s="84"/>
-      <c r="AG6" s="84"/>
-      <c r="AH6" s="84"/>
-      <c r="AI6" s="84"/>
-      <c r="AJ6" s="85"/>
+      <c r="AE6" s="78"/>
+      <c r="AF6" s="78"/>
+      <c r="AG6" s="78"/>
+      <c r="AH6" s="78"/>
+      <c r="AI6" s="78"/>
+      <c r="AJ6" s="79"/>
     </row>
     <row r="7" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="C7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="86" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="87"/>
-      <c r="F7" s="87"/>
-      <c r="G7" s="87"/>
-      <c r="H7" s="88"/>
-      <c r="I7" s="86" t="s">
+      <c r="D7" s="80" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="81"/>
+      <c r="F7" s="81"/>
+      <c r="G7" s="81"/>
+      <c r="H7" s="82"/>
+      <c r="I7" s="80" t="s">
         <v>41</v>
       </c>
-      <c r="J7" s="87"/>
-      <c r="K7" s="87"/>
-      <c r="L7" s="87"/>
-      <c r="M7" s="87"/>
-      <c r="N7" s="87"/>
-      <c r="O7" s="87"/>
-      <c r="P7" s="87"/>
-      <c r="Q7" s="88"/>
-      <c r="R7" s="86" t="s">
-        <v>40</v>
-      </c>
-      <c r="S7" s="87"/>
-      <c r="T7" s="87"/>
-      <c r="U7" s="88"/>
-      <c r="V7" s="86" t="s">
+      <c r="J7" s="81"/>
+      <c r="K7" s="81"/>
+      <c r="L7" s="81"/>
+      <c r="M7" s="81"/>
+      <c r="N7" s="81"/>
+      <c r="O7" s="81"/>
+      <c r="P7" s="81"/>
+      <c r="Q7" s="82"/>
+      <c r="R7" s="80" t="s">
+        <v>40</v>
+      </c>
+      <c r="S7" s="81"/>
+      <c r="T7" s="81"/>
+      <c r="U7" s="82"/>
+      <c r="V7" s="80" t="s">
         <v>41</v>
       </c>
-      <c r="W7" s="87"/>
-      <c r="X7" s="87"/>
-      <c r="Y7" s="88"/>
-      <c r="Z7" s="86" t="s">
+      <c r="W7" s="81"/>
+      <c r="X7" s="81"/>
+      <c r="Y7" s="82"/>
+      <c r="Z7" s="80" t="s">
         <v>41</v>
       </c>
-      <c r="AA7" s="87"/>
-      <c r="AB7" s="87"/>
-      <c r="AC7" s="88"/>
-      <c r="AD7" s="86" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE7" s="87"/>
-      <c r="AF7" s="87"/>
-      <c r="AG7" s="87"/>
-      <c r="AH7" s="87"/>
-      <c r="AI7" s="87"/>
-      <c r="AJ7" s="88"/>
+      <c r="AA7" s="81"/>
+      <c r="AB7" s="81"/>
+      <c r="AC7" s="82"/>
+      <c r="AD7" s="80" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE7" s="81"/>
+      <c r="AF7" s="81"/>
+      <c r="AG7" s="81"/>
+      <c r="AH7" s="81"/>
+      <c r="AI7" s="81"/>
+      <c r="AJ7" s="82"/>
     </row>
     <row r="8" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="C8" s="1" t="s">
@@ -4465,34 +4473,34 @@
       <c r="C25" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="77" t="s">
+      <c r="D25" s="83" t="s">
         <v>58</v>
       </c>
-      <c r="E25" s="78"/>
-      <c r="F25" s="78"/>
-      <c r="G25" s="78"/>
-      <c r="H25" s="78"/>
-      <c r="I25" s="78"/>
-      <c r="J25" s="78"/>
-      <c r="K25" s="78"/>
-      <c r="L25" s="78"/>
-      <c r="M25" s="78"/>
-      <c r="N25" s="78"/>
-      <c r="O25" s="78"/>
-      <c r="P25" s="78"/>
-      <c r="Q25" s="78"/>
-      <c r="R25" s="78"/>
-      <c r="S25" s="78"/>
-      <c r="T25" s="78"/>
-      <c r="U25" s="78"/>
-      <c r="V25" s="78"/>
-      <c r="W25" s="78"/>
-      <c r="X25" s="78"/>
-      <c r="Y25" s="78"/>
-      <c r="Z25" s="78"/>
-      <c r="AA25" s="78"/>
-      <c r="AB25" s="78"/>
-      <c r="AC25" s="79"/>
+      <c r="E25" s="84"/>
+      <c r="F25" s="84"/>
+      <c r="G25" s="84"/>
+      <c r="H25" s="84"/>
+      <c r="I25" s="84"/>
+      <c r="J25" s="84"/>
+      <c r="K25" s="84"/>
+      <c r="L25" s="84"/>
+      <c r="M25" s="84"/>
+      <c r="N25" s="84"/>
+      <c r="O25" s="84"/>
+      <c r="P25" s="84"/>
+      <c r="Q25" s="84"/>
+      <c r="R25" s="84"/>
+      <c r="S25" s="84"/>
+      <c r="T25" s="84"/>
+      <c r="U25" s="84"/>
+      <c r="V25" s="84"/>
+      <c r="W25" s="84"/>
+      <c r="X25" s="84"/>
+      <c r="Y25" s="84"/>
+      <c r="Z25" s="84"/>
+      <c r="AA25" s="84"/>
+      <c r="AB25" s="84"/>
+      <c r="AC25" s="85"/>
       <c r="AD25" s="8">
         <v>9.8199999999999985</v>
       </c>
@@ -4630,65 +4638,65 @@
       <c r="C28" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D28" s="80" t="s">
+      <c r="D28" s="86" t="s">
         <v>66</v>
       </c>
-      <c r="E28" s="81"/>
-      <c r="F28" s="81"/>
-      <c r="G28" s="81"/>
-      <c r="H28" s="81"/>
-      <c r="I28" s="81"/>
-      <c r="J28" s="81"/>
-      <c r="K28" s="81"/>
-      <c r="L28" s="81"/>
-      <c r="M28" s="81"/>
-      <c r="N28" s="81"/>
-      <c r="O28" s="81"/>
-      <c r="P28" s="81"/>
-      <c r="Q28" s="82"/>
-      <c r="R28" s="80" t="s">
+      <c r="E28" s="87"/>
+      <c r="F28" s="87"/>
+      <c r="G28" s="87"/>
+      <c r="H28" s="87"/>
+      <c r="I28" s="87"/>
+      <c r="J28" s="87"/>
+      <c r="K28" s="87"/>
+      <c r="L28" s="87"/>
+      <c r="M28" s="87"/>
+      <c r="N28" s="87"/>
+      <c r="O28" s="87"/>
+      <c r="P28" s="87"/>
+      <c r="Q28" s="88"/>
+      <c r="R28" s="86" t="s">
         <v>81</v>
       </c>
-      <c r="S28" s="81"/>
-      <c r="T28" s="81"/>
-      <c r="U28" s="81"/>
-      <c r="V28" s="81"/>
-      <c r="W28" s="81"/>
-      <c r="X28" s="81"/>
-      <c r="Y28" s="81"/>
-      <c r="Z28" s="81"/>
-      <c r="AA28" s="81"/>
-      <c r="AB28" s="81"/>
-      <c r="AC28" s="81"/>
-      <c r="AD28" s="81"/>
-      <c r="AE28" s="81"/>
-      <c r="AF28" s="81"/>
-      <c r="AG28" s="81"/>
-      <c r="AH28" s="81"/>
-      <c r="AI28" s="81"/>
-      <c r="AJ28" s="82"/>
+      <c r="S28" s="87"/>
+      <c r="T28" s="87"/>
+      <c r="U28" s="87"/>
+      <c r="V28" s="87"/>
+      <c r="W28" s="87"/>
+      <c r="X28" s="87"/>
+      <c r="Y28" s="87"/>
+      <c r="Z28" s="87"/>
+      <c r="AA28" s="87"/>
+      <c r="AB28" s="87"/>
+      <c r="AC28" s="87"/>
+      <c r="AD28" s="87"/>
+      <c r="AE28" s="87"/>
+      <c r="AF28" s="87"/>
+      <c r="AG28" s="87"/>
+      <c r="AH28" s="87"/>
+      <c r="AI28" s="87"/>
+      <c r="AJ28" s="88"/>
     </row>
     <row r="29" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="B29" s="21"/>
       <c r="C29" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D29" s="80" t="s">
+      <c r="D29" s="86" t="s">
         <v>60</v>
       </c>
-      <c r="E29" s="81"/>
-      <c r="F29" s="81"/>
-      <c r="G29" s="81"/>
-      <c r="H29" s="81"/>
-      <c r="I29" s="81"/>
-      <c r="J29" s="81"/>
-      <c r="K29" s="81"/>
-      <c r="L29" s="81"/>
-      <c r="M29" s="81"/>
-      <c r="N29" s="81"/>
-      <c r="O29" s="81"/>
-      <c r="P29" s="81"/>
-      <c r="Q29" s="82"/>
+      <c r="E29" s="87"/>
+      <c r="F29" s="87"/>
+      <c r="G29" s="87"/>
+      <c r="H29" s="87"/>
+      <c r="I29" s="87"/>
+      <c r="J29" s="87"/>
+      <c r="K29" s="87"/>
+      <c r="L29" s="87"/>
+      <c r="M29" s="87"/>
+      <c r="N29" s="87"/>
+      <c r="O29" s="87"/>
+      <c r="P29" s="87"/>
+      <c r="Q29" s="88"/>
       <c r="R29" s="47">
         <v>100</v>
       </c>
@@ -4752,22 +4760,22 @@
       <c r="C30" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D30" s="80" t="s">
+      <c r="D30" s="86" t="s">
         <v>59</v>
       </c>
-      <c r="E30" s="81"/>
-      <c r="F30" s="81"/>
-      <c r="G30" s="81"/>
-      <c r="H30" s="81"/>
-      <c r="I30" s="81"/>
-      <c r="J30" s="81"/>
-      <c r="K30" s="81"/>
-      <c r="L30" s="81"/>
-      <c r="M30" s="81"/>
-      <c r="N30" s="81"/>
-      <c r="O30" s="81"/>
-      <c r="P30" s="81"/>
-      <c r="Q30" s="82"/>
+      <c r="E30" s="87"/>
+      <c r="F30" s="87"/>
+      <c r="G30" s="87"/>
+      <c r="H30" s="87"/>
+      <c r="I30" s="87"/>
+      <c r="J30" s="87"/>
+      <c r="K30" s="87"/>
+      <c r="L30" s="87"/>
+      <c r="M30" s="87"/>
+      <c r="N30" s="87"/>
+      <c r="O30" s="87"/>
+      <c r="P30" s="87"/>
+      <c r="Q30" s="88"/>
       <c r="R30" s="47">
         <v>0.01</v>
       </c>
@@ -5319,23 +5327,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="D25:AC25"/>
+    <mergeCell ref="D30:Q30"/>
+    <mergeCell ref="D29:Q29"/>
+    <mergeCell ref="D28:Q28"/>
+    <mergeCell ref="R28:AJ28"/>
+    <mergeCell ref="V6:Y6"/>
+    <mergeCell ref="Z6:AC6"/>
+    <mergeCell ref="AD6:AJ6"/>
+    <mergeCell ref="V7:Y7"/>
+    <mergeCell ref="Z7:AC7"/>
+    <mergeCell ref="AD7:AJ7"/>
     <mergeCell ref="D6:H6"/>
     <mergeCell ref="I6:Q6"/>
     <mergeCell ref="R6:U6"/>
     <mergeCell ref="D7:H7"/>
     <mergeCell ref="I7:Q7"/>
     <mergeCell ref="R7:U7"/>
-    <mergeCell ref="V6:Y6"/>
-    <mergeCell ref="Z6:AC6"/>
-    <mergeCell ref="AD6:AJ6"/>
-    <mergeCell ref="V7:Y7"/>
-    <mergeCell ref="Z7:AC7"/>
-    <mergeCell ref="AD7:AJ7"/>
-    <mergeCell ref="D25:AC25"/>
-    <mergeCell ref="D30:Q30"/>
-    <mergeCell ref="D29:Q29"/>
-    <mergeCell ref="D28:Q28"/>
-    <mergeCell ref="R28:AJ28"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5347,10 +5355,10 @@
   <dimension ref="B5:AJ36"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="8" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="8" topLeftCell="M9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="AE17" sqref="AE17"/>
+      <selection pane="bottomRight" activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -11308,7 +11316,7 @@
   <dimension ref="B5:AD39"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="5" ySplit="5" topLeftCell="F26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="5" topLeftCell="O6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight" activeCell="P15" sqref="P15:P25"/>
@@ -14296,12 +14304,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC155531-539F-473A-BEFE-FAB0C4C3EE43}">
   <dimension ref="B4:AD39"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="M7" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <pane xSplit="5" ySplit="3" topLeftCell="O7" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
       <selection pane="topRight" activeCell="E4" sqref="E4"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="Z15" sqref="Z15"/>
+      <selection pane="bottomRight" activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -14322,6 +14330,9 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:30" ht="90" x14ac:dyDescent="0.55000000000000004">
+      <c r="T4" s="3" t="s">
+        <v>122</v>
+      </c>
       <c r="V4" s="3" t="s">
         <v>50</v>
       </c>
@@ -18643,7 +18654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFFD9269-7F18-4E64-8D48-3C1F1E4D91C0}">
   <dimension ref="B2:AF47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" topLeftCell="Q1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="AA9" sqref="AA9"/>
     </sheetView>

</xml_diff>

<commit_message>
update readme and chapter2 xlsx
</commit_message>
<xml_diff>
--- a/chapter2/input/chapter2_demo_data.xlsx
+++ b/chapter2/input/chapter2_demo_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\副業関連\独立\執筆\practical-mi-guide\chapter2\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\副業関連\独立\workdir\practical-mi-guide\chapter2\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACF01F2C-443B-43C0-8C5D-008D42E1DDF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87855621-3F0F-48BD-BA58-CF9C08FB6631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9700" yWindow="2470" windowWidth="22490" windowHeight="17850" activeTab="4" xr2:uid="{AFFCA931-CB2A-4AED-B7E5-2638B5FCE6AD}"/>
+    <workbookView xWindow="1990" yWindow="2510" windowWidth="34540" windowHeight="17720" activeTab="5" xr2:uid="{AFFCA931-CB2A-4AED-B7E5-2638B5FCE6AD}"/>
   </bookViews>
   <sheets>
     <sheet name="初期データ" sheetId="2" r:id="rId1"/>
@@ -1156,6 +1156,24 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1172,24 +1190,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2581,10 +2581,10 @@
   <dimension ref="B5:AJ36"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="8" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="8" topLeftCell="F9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8:XFD8"/>
+      <selection pane="bottomRight" activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -2716,101 +2716,103 @@
       <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="77">
+      <c r="D6" s="83">
         <v>45310</v>
       </c>
-      <c r="E6" s="78"/>
-      <c r="F6" s="78"/>
-      <c r="G6" s="78"/>
-      <c r="H6" s="79"/>
-      <c r="I6" s="77">
+      <c r="E6" s="84"/>
+      <c r="F6" s="84"/>
+      <c r="G6" s="84"/>
+      <c r="H6" s="85"/>
+      <c r="I6" s="83">
         <v>45321</v>
       </c>
-      <c r="J6" s="78"/>
-      <c r="K6" s="78"/>
-      <c r="L6" s="78"/>
-      <c r="M6" s="78"/>
-      <c r="N6" s="78"/>
-      <c r="O6" s="78"/>
-      <c r="P6" s="78"/>
-      <c r="Q6" s="79"/>
-      <c r="R6" s="77">
+      <c r="J6" s="84"/>
+      <c r="K6" s="84"/>
+      <c r="L6" s="84"/>
+      <c r="M6" s="84"/>
+      <c r="N6" s="84"/>
+      <c r="O6" s="84">
+        <v>45329</v>
+      </c>
+      <c r="P6" s="84"/>
+      <c r="Q6" s="85"/>
+      <c r="R6" s="83">
         <v>45337</v>
       </c>
-      <c r="S6" s="78"/>
-      <c r="T6" s="78"/>
-      <c r="U6" s="79"/>
-      <c r="V6" s="77">
+      <c r="S6" s="84"/>
+      <c r="T6" s="84"/>
+      <c r="U6" s="85"/>
+      <c r="V6" s="83">
         <v>45350</v>
       </c>
-      <c r="W6" s="78"/>
-      <c r="X6" s="78"/>
-      <c r="Y6" s="79"/>
-      <c r="Z6" s="77">
+      <c r="W6" s="84"/>
+      <c r="X6" s="84"/>
+      <c r="Y6" s="85"/>
+      <c r="Z6" s="83">
         <v>45366</v>
       </c>
-      <c r="AA6" s="78"/>
-      <c r="AB6" s="78"/>
-      <c r="AC6" s="79"/>
-      <c r="AD6" s="77">
+      <c r="AA6" s="84"/>
+      <c r="AB6" s="84"/>
+      <c r="AC6" s="85"/>
+      <c r="AD6" s="83">
         <v>45392</v>
       </c>
-      <c r="AE6" s="78"/>
-      <c r="AF6" s="78"/>
-      <c r="AG6" s="78"/>
-      <c r="AH6" s="78"/>
-      <c r="AI6" s="78"/>
-      <c r="AJ6" s="79"/>
+      <c r="AE6" s="84"/>
+      <c r="AF6" s="84"/>
+      <c r="AG6" s="84"/>
+      <c r="AH6" s="84"/>
+      <c r="AI6" s="84"/>
+      <c r="AJ6" s="85"/>
     </row>
     <row r="7" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="C7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="80" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="81"/>
-      <c r="F7" s="81"/>
-      <c r="G7" s="81"/>
-      <c r="H7" s="82"/>
-      <c r="I7" s="80" t="s">
+      <c r="D7" s="86" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="87"/>
+      <c r="F7" s="87"/>
+      <c r="G7" s="87"/>
+      <c r="H7" s="88"/>
+      <c r="I7" s="86" t="s">
         <v>41</v>
       </c>
-      <c r="J7" s="81"/>
-      <c r="K7" s="81"/>
-      <c r="L7" s="81"/>
-      <c r="M7" s="81"/>
-      <c r="N7" s="81"/>
-      <c r="O7" s="81"/>
-      <c r="P7" s="81"/>
-      <c r="Q7" s="82"/>
-      <c r="R7" s="80" t="s">
-        <v>40</v>
-      </c>
-      <c r="S7" s="81"/>
-      <c r="T7" s="81"/>
-      <c r="U7" s="82"/>
-      <c r="V7" s="80" t="s">
+      <c r="J7" s="87"/>
+      <c r="K7" s="87"/>
+      <c r="L7" s="87"/>
+      <c r="M7" s="87"/>
+      <c r="N7" s="87"/>
+      <c r="O7" s="87"/>
+      <c r="P7" s="87"/>
+      <c r="Q7" s="88"/>
+      <c r="R7" s="86" t="s">
+        <v>40</v>
+      </c>
+      <c r="S7" s="87"/>
+      <c r="T7" s="87"/>
+      <c r="U7" s="88"/>
+      <c r="V7" s="86" t="s">
         <v>41</v>
       </c>
-      <c r="W7" s="81"/>
-      <c r="X7" s="81"/>
-      <c r="Y7" s="82"/>
-      <c r="Z7" s="80" t="s">
+      <c r="W7" s="87"/>
+      <c r="X7" s="87"/>
+      <c r="Y7" s="88"/>
+      <c r="Z7" s="86" t="s">
         <v>41</v>
       </c>
-      <c r="AA7" s="81"/>
-      <c r="AB7" s="81"/>
-      <c r="AC7" s="82"/>
-      <c r="AD7" s="80" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE7" s="81"/>
-      <c r="AF7" s="81"/>
-      <c r="AG7" s="81"/>
-      <c r="AH7" s="81"/>
-      <c r="AI7" s="81"/>
-      <c r="AJ7" s="82"/>
+      <c r="AA7" s="87"/>
+      <c r="AB7" s="87"/>
+      <c r="AC7" s="88"/>
+      <c r="AD7" s="86" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE7" s="87"/>
+      <c r="AF7" s="87"/>
+      <c r="AG7" s="87"/>
+      <c r="AH7" s="87"/>
+      <c r="AI7" s="87"/>
+      <c r="AJ7" s="88"/>
     </row>
     <row r="8" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="C8" s="1" t="s">
@@ -4473,34 +4475,34 @@
       <c r="C25" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="83" t="s">
+      <c r="D25" s="77" t="s">
         <v>58</v>
       </c>
-      <c r="E25" s="84"/>
-      <c r="F25" s="84"/>
-      <c r="G25" s="84"/>
-      <c r="H25" s="84"/>
-      <c r="I25" s="84"/>
-      <c r="J25" s="84"/>
-      <c r="K25" s="84"/>
-      <c r="L25" s="84"/>
-      <c r="M25" s="84"/>
-      <c r="N25" s="84"/>
-      <c r="O25" s="84"/>
-      <c r="P25" s="84"/>
-      <c r="Q25" s="84"/>
-      <c r="R25" s="84"/>
-      <c r="S25" s="84"/>
-      <c r="T25" s="84"/>
-      <c r="U25" s="84"/>
-      <c r="V25" s="84"/>
-      <c r="W25" s="84"/>
-      <c r="X25" s="84"/>
-      <c r="Y25" s="84"/>
-      <c r="Z25" s="84"/>
-      <c r="AA25" s="84"/>
-      <c r="AB25" s="84"/>
-      <c r="AC25" s="85"/>
+      <c r="E25" s="78"/>
+      <c r="F25" s="78"/>
+      <c r="G25" s="78"/>
+      <c r="H25" s="78"/>
+      <c r="I25" s="78"/>
+      <c r="J25" s="78"/>
+      <c r="K25" s="78"/>
+      <c r="L25" s="78"/>
+      <c r="M25" s="78"/>
+      <c r="N25" s="78"/>
+      <c r="O25" s="78"/>
+      <c r="P25" s="78"/>
+      <c r="Q25" s="78"/>
+      <c r="R25" s="78"/>
+      <c r="S25" s="78"/>
+      <c r="T25" s="78"/>
+      <c r="U25" s="78"/>
+      <c r="V25" s="78"/>
+      <c r="W25" s="78"/>
+      <c r="X25" s="78"/>
+      <c r="Y25" s="78"/>
+      <c r="Z25" s="78"/>
+      <c r="AA25" s="78"/>
+      <c r="AB25" s="78"/>
+      <c r="AC25" s="79"/>
       <c r="AD25" s="8">
         <v>9.8199999999999985</v>
       </c>
@@ -4638,65 +4640,65 @@
       <c r="C28" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D28" s="86" t="s">
+      <c r="D28" s="80" t="s">
         <v>66</v>
       </c>
-      <c r="E28" s="87"/>
-      <c r="F28" s="87"/>
-      <c r="G28" s="87"/>
-      <c r="H28" s="87"/>
-      <c r="I28" s="87"/>
-      <c r="J28" s="87"/>
-      <c r="K28" s="87"/>
-      <c r="L28" s="87"/>
-      <c r="M28" s="87"/>
-      <c r="N28" s="87"/>
-      <c r="O28" s="87"/>
-      <c r="P28" s="87"/>
-      <c r="Q28" s="88"/>
-      <c r="R28" s="86" t="s">
+      <c r="E28" s="81"/>
+      <c r="F28" s="81"/>
+      <c r="G28" s="81"/>
+      <c r="H28" s="81"/>
+      <c r="I28" s="81"/>
+      <c r="J28" s="81"/>
+      <c r="K28" s="81"/>
+      <c r="L28" s="81"/>
+      <c r="M28" s="81"/>
+      <c r="N28" s="81"/>
+      <c r="O28" s="81"/>
+      <c r="P28" s="81"/>
+      <c r="Q28" s="82"/>
+      <c r="R28" s="80" t="s">
         <v>81</v>
       </c>
-      <c r="S28" s="87"/>
-      <c r="T28" s="87"/>
-      <c r="U28" s="87"/>
-      <c r="V28" s="87"/>
-      <c r="W28" s="87"/>
-      <c r="X28" s="87"/>
-      <c r="Y28" s="87"/>
-      <c r="Z28" s="87"/>
-      <c r="AA28" s="87"/>
-      <c r="AB28" s="87"/>
-      <c r="AC28" s="87"/>
-      <c r="AD28" s="87"/>
-      <c r="AE28" s="87"/>
-      <c r="AF28" s="87"/>
-      <c r="AG28" s="87"/>
-      <c r="AH28" s="87"/>
-      <c r="AI28" s="87"/>
-      <c r="AJ28" s="88"/>
+      <c r="S28" s="81"/>
+      <c r="T28" s="81"/>
+      <c r="U28" s="81"/>
+      <c r="V28" s="81"/>
+      <c r="W28" s="81"/>
+      <c r="X28" s="81"/>
+      <c r="Y28" s="81"/>
+      <c r="Z28" s="81"/>
+      <c r="AA28" s="81"/>
+      <c r="AB28" s="81"/>
+      <c r="AC28" s="81"/>
+      <c r="AD28" s="81"/>
+      <c r="AE28" s="81"/>
+      <c r="AF28" s="81"/>
+      <c r="AG28" s="81"/>
+      <c r="AH28" s="81"/>
+      <c r="AI28" s="81"/>
+      <c r="AJ28" s="82"/>
     </row>
     <row r="29" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="B29" s="21"/>
       <c r="C29" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D29" s="86" t="s">
+      <c r="D29" s="80" t="s">
         <v>60</v>
       </c>
-      <c r="E29" s="87"/>
-      <c r="F29" s="87"/>
-      <c r="G29" s="87"/>
-      <c r="H29" s="87"/>
-      <c r="I29" s="87"/>
-      <c r="J29" s="87"/>
-      <c r="K29" s="87"/>
-      <c r="L29" s="87"/>
-      <c r="M29" s="87"/>
-      <c r="N29" s="87"/>
-      <c r="O29" s="87"/>
-      <c r="P29" s="87"/>
-      <c r="Q29" s="88"/>
+      <c r="E29" s="81"/>
+      <c r="F29" s="81"/>
+      <c r="G29" s="81"/>
+      <c r="H29" s="81"/>
+      <c r="I29" s="81"/>
+      <c r="J29" s="81"/>
+      <c r="K29" s="81"/>
+      <c r="L29" s="81"/>
+      <c r="M29" s="81"/>
+      <c r="N29" s="81"/>
+      <c r="O29" s="81"/>
+      <c r="P29" s="81"/>
+      <c r="Q29" s="82"/>
       <c r="R29" s="47">
         <v>100</v>
       </c>
@@ -4760,22 +4762,22 @@
       <c r="C30" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D30" s="86" t="s">
+      <c r="D30" s="80" t="s">
         <v>59</v>
       </c>
-      <c r="E30" s="87"/>
-      <c r="F30" s="87"/>
-      <c r="G30" s="87"/>
-      <c r="H30" s="87"/>
-      <c r="I30" s="87"/>
-      <c r="J30" s="87"/>
-      <c r="K30" s="87"/>
-      <c r="L30" s="87"/>
-      <c r="M30" s="87"/>
-      <c r="N30" s="87"/>
-      <c r="O30" s="87"/>
-      <c r="P30" s="87"/>
-      <c r="Q30" s="88"/>
+      <c r="E30" s="81"/>
+      <c r="F30" s="81"/>
+      <c r="G30" s="81"/>
+      <c r="H30" s="81"/>
+      <c r="I30" s="81"/>
+      <c r="J30" s="81"/>
+      <c r="K30" s="81"/>
+      <c r="L30" s="81"/>
+      <c r="M30" s="81"/>
+      <c r="N30" s="81"/>
+      <c r="O30" s="81"/>
+      <c r="P30" s="81"/>
+      <c r="Q30" s="82"/>
       <c r="R30" s="47">
         <v>0.01</v>
       </c>
@@ -5326,24 +5328,25 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="D25:AC25"/>
-    <mergeCell ref="D30:Q30"/>
-    <mergeCell ref="D29:Q29"/>
-    <mergeCell ref="D28:Q28"/>
-    <mergeCell ref="R28:AJ28"/>
+  <mergeCells count="18">
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="R6:U6"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="I7:Q7"/>
+    <mergeCell ref="R7:U7"/>
+    <mergeCell ref="I6:N6"/>
+    <mergeCell ref="O6:Q6"/>
     <mergeCell ref="V6:Y6"/>
     <mergeCell ref="Z6:AC6"/>
     <mergeCell ref="AD6:AJ6"/>
     <mergeCell ref="V7:Y7"/>
     <mergeCell ref="Z7:AC7"/>
     <mergeCell ref="AD7:AJ7"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="I6:Q6"/>
-    <mergeCell ref="R6:U6"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="I7:Q7"/>
-    <mergeCell ref="R7:U7"/>
+    <mergeCell ref="D25:AC25"/>
+    <mergeCell ref="D30:Q30"/>
+    <mergeCell ref="D29:Q29"/>
+    <mergeCell ref="D28:Q28"/>
+    <mergeCell ref="R28:AJ28"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5355,10 +5358,10 @@
   <dimension ref="B5:AJ36"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="8" topLeftCell="M9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="8" topLeftCell="E9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="E28" sqref="E28"/>
+      <selection pane="bottomRight" activeCell="Q6" sqref="O6:Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -5524,13 +5527,13 @@
         <v>45321</v>
       </c>
       <c r="O6" s="17">
-        <v>45321</v>
+        <v>45329</v>
       </c>
       <c r="P6" s="15">
-        <v>45321</v>
+        <v>45329</v>
       </c>
       <c r="Q6" s="15">
-        <v>45321</v>
+        <v>45329</v>
       </c>
       <c r="R6" s="15">
         <v>45337</v>
@@ -8382,7 +8385,7 @@
   <dimension ref="B5:AC39"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="C25" sqref="C25:C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -9458,7 +9461,7 @@
         <v>23</v>
       </c>
       <c r="C18" s="25">
-        <v>45321</v>
+        <v>45329</v>
       </c>
       <c r="D18" s="24" t="s">
         <v>41</v>
@@ -9542,7 +9545,7 @@
         <v>24</v>
       </c>
       <c r="C19" s="28">
-        <v>45321</v>
+        <v>45329</v>
       </c>
       <c r="D19" s="26" t="s">
         <v>41</v>
@@ -9626,7 +9629,7 @@
         <v>25</v>
       </c>
       <c r="C20" s="28">
-        <v>45321</v>
+        <v>45329</v>
       </c>
       <c r="D20" s="26" t="s">
         <v>41</v>
@@ -11319,7 +11322,7 @@
       <pane xSplit="5" ySplit="5" topLeftCell="O6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="P15" sqref="P15:P25"/>
+      <selection pane="bottomRight" activeCell="C18" sqref="C18:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -12411,7 +12414,7 @@
         <v>23</v>
       </c>
       <c r="C18" s="25">
-        <v>45321</v>
+        <v>45329</v>
       </c>
       <c r="D18" s="24" t="s">
         <v>41</v>
@@ -12496,7 +12499,7 @@
         <v>24</v>
       </c>
       <c r="C19" s="28">
-        <v>45321</v>
+        <v>45329</v>
       </c>
       <c r="D19" s="26" t="s">
         <v>41</v>
@@ -12581,7 +12584,7 @@
         <v>25</v>
       </c>
       <c r="C20" s="28">
-        <v>45321</v>
+        <v>45329</v>
       </c>
       <c r="D20" s="26" t="s">
         <v>41</v>
@@ -14304,12 +14307,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC155531-539F-473A-BEFE-FAB0C4C3EE43}">
   <dimension ref="B4:AD39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="O7" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
+      <pane xSplit="5" ySplit="3" topLeftCell="F12" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
       <selection pane="topRight" activeCell="E4" sqref="E4"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="T5" sqref="T5"/>
+      <selection pane="bottomRight" activeCell="C20" sqref="C18:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -15376,7 +15379,7 @@
         <v>23</v>
       </c>
       <c r="C18" s="25">
-        <v>45321</v>
+        <v>45329</v>
       </c>
       <c r="D18" s="24" t="s">
         <v>41</v>
@@ -15457,7 +15460,7 @@
         <v>24</v>
       </c>
       <c r="C19" s="28">
-        <v>45321</v>
+        <v>45329</v>
       </c>
       <c r="D19" s="26" t="s">
         <v>41</v>
@@ -15538,7 +15541,7 @@
         <v>25</v>
       </c>
       <c r="C20" s="28">
-        <v>45321</v>
+        <v>45329</v>
       </c>
       <c r="D20" s="26" t="s">
         <v>41</v>
@@ -17236,7 +17239,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{946DA809-6F7B-4F40-B49B-27E3855F241E}">
   <dimension ref="A1:Y25"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="W25" sqref="W25"/>
     </sheetView>
   </sheetViews>
@@ -18654,9 +18657,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFFD9269-7F18-4E64-8D48-3C1F1E4D91C0}">
   <dimension ref="B2:AF47"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" topLeftCell="Q1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AA9" sqref="AA9"/>
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C16" sqref="C16:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -19909,7 +19912,7 @@
         <v>23</v>
       </c>
       <c r="C16" s="52">
-        <v>45321</v>
+        <v>45329</v>
       </c>
       <c r="D16" s="52" t="s">
         <v>41</v>
@@ -20006,7 +20009,7 @@
         <v>24</v>
       </c>
       <c r="C17" s="52">
-        <v>45321</v>
+        <v>45329</v>
       </c>
       <c r="D17" s="52" t="s">
         <v>41</v>
@@ -20103,7 +20106,7 @@
         <v>25</v>
       </c>
       <c r="C18" s="52">
-        <v>45321</v>
+        <v>45329</v>
       </c>
       <c r="D18" s="52" t="s">
         <v>41</v>

</xml_diff>